<commit_message>
separate directories for XLS and XML
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="5"/>
+    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="3M" sheetId="5" r:id="rId1"/>
@@ -1876,6 +1876,7 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1907,7 +1908,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="3"/>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="H3" s="41" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_T3F1#0002</v>
+        <v>HKD_YC3MRH_T3F1#0003</v>
       </c>
       <c r="I3" s="40" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="H4" s="31" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_TOM3F1#0002</v>
+        <v>HKD_YC3MRH_TOM3F1#0003</v>
       </c>
       <c r="I4" s="39" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="H5" s="36" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0002</v>
+        <v>HKD_YC3MRH_1x4F#0003</v>
       </c>
       <c r="I5" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -2414,7 +2414,7 @@
       </c>
       <c r="H6" s="36" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0002</v>
+        <v>HKD_YC3MRH_2x5F#0003</v>
       </c>
       <c r="I6" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="H7" s="36" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0002</v>
+        <v>HKD_YC3MRH_3x6F#0003</v>
       </c>
       <c r="I7" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -2484,7 +2484,7 @@
       </c>
       <c r="H8" s="36" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0002</v>
+        <v>HKD_YC3MRH_4x7F#0003</v>
       </c>
       <c r="I8" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="H9" s="36" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0002</v>
+        <v>HKD_YC3MRH_5x8F#0003</v>
       </c>
       <c r="I9" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="H10" s="36" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0002</v>
+        <v>HKD_YC3MRH_6x9F#0003</v>
       </c>
       <c r="I10" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H11" s="36" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0002</v>
+        <v>HKD_YC3MRH_7x10F#0003</v>
       </c>
       <c r="I11" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -2624,7 +2624,7 @@
       </c>
       <c r="H12" s="36" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0002</v>
+        <v>HKD_YC3MRH_8x11F#0003</v>
       </c>
       <c r="I12" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="H13" s="31" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0002</v>
+        <v>HKD_YC3MRH_9x12F#0003</v>
       </c>
       <c r="I13" s="30" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -2715,12 +2715,12 @@
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="189"/>
     </row>
     <row r="3" spans="1:22" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="D8" s="19" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Projects\quantlib\QuantLibXL\Data2\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -2803,12 +2803,12 @@
     </row>
     <row r="11" spans="1:22" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="186" t="s">
+      <c r="B12" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="187"/>
-      <c r="D12" s="187"/>
-      <c r="E12" s="188"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="189"/>
       <c r="V12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2980,13 +2980,13 @@
         <f>K2&amp;"_Swaps.xml"</f>
         <v>HKD_YC3MRH_Swaps.xml</v>
       </c>
-      <c r="L3" s="45">
+      <c r="L3" s="45" t="e">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(L4:L50,SerializationPath&amp;K3,FileOverwrite,,Serialize),"---")</f>
-        <v>45</v>
-      </c>
-      <c r="M3" s="62" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="M3" s="62" t="e">
         <f ca="1">_xll.ohRangeRetrieveError(L3)</f>
-        <v/>
+        <v>#NUM!</v>
       </c>
       <c r="N3" s="61"/>
       <c r="S3" s="85" t="s">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="L4" s="83" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,S4,Currency,T4,U4,V4,W4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H_Hibor3M#0003</v>
+        <v>HKD_YC3MRH_QM3H_Hibor3M#0004</v>
       </c>
       <c r="M4" s="82" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="L6" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H1Y#0002</v>
+        <v>HKD_YC3MRH_QM3H1Y#0003</v>
       </c>
       <c r="M6" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="L7" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15M#0002</v>
+        <v>HKD_YC3MRH_QM3H15M#0003</v>
       </c>
       <c r="M7" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="L8" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18M#0002</v>
+        <v>HKD_YC3MRH_QM3H18M#0003</v>
       </c>
       <c r="M8" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -3262,7 +3262,7 @@
       </c>
       <c r="L9" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21M#0002</v>
+        <v>HKD_YC3MRH_QM3H21M#0003</v>
       </c>
       <c r="M9" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="L10" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H2Y#0002</v>
+        <v>HKD_YC3MRH_QM3H2Y#0003</v>
       </c>
       <c r="M10" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="L11" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H3Y#0002</v>
+        <v>HKD_YC3MRH_QM3H3Y#0003</v>
       </c>
       <c r="M11" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="L12" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H4Y#0002</v>
+        <v>HKD_YC3MRH_QM3H4Y#0003</v>
       </c>
       <c r="M12" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="L13" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H5Y#0002</v>
+        <v>HKD_YC3MRH_QM3H5Y#0003</v>
       </c>
       <c r="M13" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="L14" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H6Y#0002</v>
+        <v>HKD_YC3MRH_QM3H6Y#0003</v>
       </c>
       <c r="M14" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -3559,7 +3559,7 @@
       </c>
       <c r="L15" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H7Y#0002</v>
+        <v>HKD_YC3MRH_QM3H7Y#0003</v>
       </c>
       <c r="M15" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="L16" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H8Y#0002</v>
+        <v>HKD_YC3MRH_QM3H8Y#0003</v>
       </c>
       <c r="M16" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="L17" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H9Y#0002</v>
+        <v>HKD_YC3MRH_QM3H9Y#0003</v>
       </c>
       <c r="M17" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="L18" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H10Y#0002</v>
+        <v>HKD_YC3MRH_QM3H10Y#0003</v>
       </c>
       <c r="M18" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="L19" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H11Y#0002</v>
+        <v>HKD_YC3MRH_QM3H11Y#0003</v>
       </c>
       <c r="M19" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="L20" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H12Y#0002</v>
+        <v>HKD_YC3MRH_QM3H12Y#0003</v>
       </c>
       <c r="M20" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="L21" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H13Y#0002</v>
+        <v>HKD_YC3MRH_QM3H13Y#0003</v>
       </c>
       <c r="M21" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="L22" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H14Y#0002</v>
+        <v>HKD_YC3MRH_QM3H14Y#0003</v>
       </c>
       <c r="M22" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="L23" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15Y#0002</v>
+        <v>HKD_YC3MRH_QM3H15Y#0003</v>
       </c>
       <c r="M23" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="L24" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H16Y#0002</v>
+        <v>HKD_YC3MRH_QM3H16Y#0003</v>
       </c>
       <c r="M24" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="L25" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H17Y#0002</v>
+        <v>HKD_YC3MRH_QM3H17Y#0003</v>
       </c>
       <c r="M25" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="L26" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18Y#0002</v>
+        <v>HKD_YC3MRH_QM3H18Y#0003</v>
       </c>
       <c r="M26" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="L27" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H19Y#0002</v>
+        <v>HKD_YC3MRH_QM3H19Y#0003</v>
       </c>
       <c r="M27" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -4144,7 +4144,7 @@
       </c>
       <c r="L28" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H20Y#0002</v>
+        <v>HKD_YC3MRH_QM3H20Y#0003</v>
       </c>
       <c r="M28" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="L29" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21Y#0002</v>
+        <v>HKD_YC3MRH_QM3H21Y#0003</v>
       </c>
       <c r="M29" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="L30" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H22Y#0002</v>
+        <v>HKD_YC3MRH_QM3H22Y#0003</v>
       </c>
       <c r="M30" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="L31" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H23Y#0002</v>
+        <v>HKD_YC3MRH_QM3H23Y#0003</v>
       </c>
       <c r="M31" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -4324,7 +4324,7 @@
       </c>
       <c r="L32" s="63" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H24Y#0002</v>
+        <v>HKD_YC3MRH_QM3H24Y#0003</v>
       </c>
       <c r="M32" s="62" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -4367,13 +4367,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H25Y</v>
       </c>
-      <c r="L33" s="63" t="str">
+      <c r="L33" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H25Y#0002</v>
-      </c>
-      <c r="M33" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L33)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M33" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L33)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N33" s="61"/>
     </row>
@@ -4412,13 +4412,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H26Y</v>
       </c>
-      <c r="L34" s="63" t="str">
+      <c r="L34" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H26Y#0002</v>
-      </c>
-      <c r="M34" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L34)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M34" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L34)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N34" s="61"/>
     </row>
@@ -4457,13 +4457,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H27Y</v>
       </c>
-      <c r="L35" s="63" t="str">
+      <c r="L35" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H27Y#0002</v>
-      </c>
-      <c r="M35" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L35)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M35" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L35)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N35" s="61"/>
     </row>
@@ -4502,13 +4502,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H28Y</v>
       </c>
-      <c r="L36" s="63" t="str">
+      <c r="L36" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H28Y#0002</v>
-      </c>
-      <c r="M36" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L36)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M36" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L36)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N36" s="61"/>
     </row>
@@ -4547,13 +4547,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H29Y</v>
       </c>
-      <c r="L37" s="63" t="str">
+      <c r="L37" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H29Y#0002</v>
-      </c>
-      <c r="M37" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L37)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M37" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L37)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N37" s="61"/>
     </row>
@@ -4592,13 +4592,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H30Y</v>
       </c>
-      <c r="L38" s="63" t="str">
+      <c r="L38" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H30Y#0002</v>
-      </c>
-      <c r="M38" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L38)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M38" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L38)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N38" s="61"/>
     </row>
@@ -4637,13 +4637,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H35Y</v>
       </c>
-      <c r="L39" s="63" t="str">
+      <c r="L39" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H35Y#0002</v>
-      </c>
-      <c r="M39" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L39)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M39" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L39)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N39" s="61"/>
     </row>
@@ -4682,13 +4682,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H40Y</v>
       </c>
-      <c r="L40" s="63" t="str">
+      <c r="L40" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H40Y#0002</v>
-      </c>
-      <c r="M40" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L40)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M40" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L40)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N40" s="61"/>
     </row>
@@ -4727,13 +4727,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H50Y</v>
       </c>
-      <c r="L41" s="63" t="str">
+      <c r="L41" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H50Y#0002</v>
-      </c>
-      <c r="M41" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L41)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M41" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L41)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N41" s="61"/>
     </row>
@@ -4772,13 +4772,13 @@
         <f t="shared" si="2"/>
         <v>HKD_YC3MRH_QM3H60Y</v>
       </c>
-      <c r="L42" s="63" t="str">
+      <c r="L42" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H60Y#0002</v>
-      </c>
-      <c r="M42" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L42)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M42" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L42)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N42" s="61"/>
     </row>
@@ -4830,13 +4830,13 @@
         <f t="shared" ref="K44:K50" si="4">$K$2&amp;"_"&amp;$D44&amp;$E44&amp;$C44</f>
         <v>HKD_YC3MRH_1S12</v>
       </c>
-      <c r="L44" s="63" t="str">
+      <c r="L44" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S12#0002</v>
-      </c>
-      <c r="M44" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L44)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M44" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L44)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N44" s="61"/>
       <c r="O44" s="59"/>
@@ -4873,13 +4873,13 @@
         <f t="shared" si="4"/>
         <v>HKD_YC3MRH_2S12</v>
       </c>
-      <c r="L45" s="63" t="str">
+      <c r="L45" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2S12#0002</v>
-      </c>
-      <c r="M45" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L45)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M45" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L45)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N45" s="61"/>
       <c r="O45" s="59"/>
@@ -4918,13 +4918,13 @@
         <f t="shared" si="4"/>
         <v>HKD_YC3MRH_3S12</v>
       </c>
-      <c r="L46" s="63" t="str">
+      <c r="L46" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3S12#0002</v>
-      </c>
-      <c r="M46" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L46)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M46" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L46)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N46" s="61"/>
       <c r="O46" s="59"/>
@@ -4963,13 +4963,13 @@
         <f t="shared" si="4"/>
         <v>HKD_YC3MRH_4S12</v>
       </c>
-      <c r="L47" s="63" t="str">
+      <c r="L47" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4S12#0002</v>
-      </c>
-      <c r="M47" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L47)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M47" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L47)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N47" s="61"/>
       <c r="O47" s="59"/>
@@ -5008,13 +5008,13 @@
         <f t="shared" si="4"/>
         <v>HKD_YC3MRH_1S24</v>
       </c>
-      <c r="L48" s="63" t="str">
+      <c r="L48" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S24#0002</v>
-      </c>
-      <c r="M48" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L48)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M48" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L48)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N48" s="61"/>
       <c r="O48" s="59"/>
@@ -5053,13 +5053,13 @@
         <f t="shared" si="4"/>
         <v>HKD_YC3MRH_2S24</v>
       </c>
-      <c r="L49" s="63" t="str">
+      <c r="L49" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2S24#0002</v>
-      </c>
-      <c r="M49" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L49)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M49" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L49)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N49" s="61"/>
       <c r="O49" s="59"/>
@@ -5098,13 +5098,13 @@
         <f t="shared" si="4"/>
         <v>HKD_YC3MRH_1S36</v>
       </c>
-      <c r="L50" s="63" t="str">
+      <c r="L50" s="63" t="e">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1S36#0002</v>
-      </c>
-      <c r="M50" s="62" t="str">
-        <f>_xll.ohRangeRetrieveError(L50)</f>
-        <v/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M50" s="62" t="e">
+        <f ca="1">_xll.ohRangeRetrieveError(L50)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N50" s="61"/>
       <c r="O50" s="59"/>
@@ -5189,12 +5189,12 @@
     </row>
     <row r="2" spans="1:22" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="189"/>
     </row>
     <row r="3" spans="1:22" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
@@ -5253,7 +5253,7 @@
       </c>
       <c r="D8" s="19" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\Projects\quantlib\QuantLibXL\Data2\</v>
+        <v>C:\Projects\quantlib\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -5277,12 +5277,12 @@
     </row>
     <row r="11" spans="1:22" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="186" t="s">
+      <c r="B12" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="187"/>
-      <c r="D12" s="187"/>
-      <c r="E12" s="188"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="189"/>
       <c r="V12" s="1" t="s">
         <v>4</v>
       </c>
@@ -5436,11 +5436,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="190" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="190"/>
-      <c r="D1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="192"/>
       <c r="E1" s="164" t="s">
         <v>148</v>
       </c>
@@ -6161,9 +6161,9 @@
         <f>_xll.ohObjectPropertyValues(E18,"Rate")</f>
         <v>HKD1x4F_Quote</v>
       </c>
-      <c r="G18" s="146" t="e">
+      <c r="G18" s="146">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="H18" s="146"/>
       <c r="I18" s="145" t="b">
@@ -6206,9 +6206,9 @@
         <f>_xll.ohObjectPropertyValues(E19,"Rate")</f>
         <v>HKD2x5F_Quote</v>
       </c>
-      <c r="G19" s="146" t="e">
+      <c r="G19" s="146">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="H19" s="146"/>
       <c r="I19" s="145" t="b">
@@ -6251,9 +6251,9 @@
         <f>_xll.ohObjectPropertyValues(E20,"Rate")</f>
         <v>HKD3x6F_Quote</v>
       </c>
-      <c r="G20" s="146" t="e">
+      <c r="G20" s="146">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="H20" s="146"/>
       <c r="I20" s="145" t="b">
@@ -6296,9 +6296,9 @@
         <f>_xll.ohObjectPropertyValues(E21,"Rate")</f>
         <v>HKD4x7F_Quote</v>
       </c>
-      <c r="G21" s="146" t="e">
+      <c r="G21" s="146">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="H21" s="146"/>
       <c r="I21" s="145" t="b">
@@ -6341,9 +6341,9 @@
         <f>_xll.ohObjectPropertyValues(E22,"Rate")</f>
         <v>HKD5x8F_Quote</v>
       </c>
-      <c r="G22" s="146" t="e">
+      <c r="G22" s="146">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="H22" s="146"/>
       <c r="I22" s="145" t="b">
@@ -6386,9 +6386,9 @@
         <f>_xll.ohObjectPropertyValues(E23,"Rate")</f>
         <v>HKD6x9F_Quote</v>
       </c>
-      <c r="G23" s="146" t="e">
+      <c r="G23" s="146">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.5000000000000005E-3</v>
       </c>
       <c r="H23" s="146"/>
       <c r="I23" s="145" t="b">
@@ -6431,9 +6431,9 @@
         <f>_xll.ohObjectPropertyValues(E24,"Rate")</f>
         <v>HKD7x10F_Quote</v>
       </c>
-      <c r="G24" s="146" t="e">
+      <c r="G24" s="146">
         <f>_xll.qlRateHelperQuoteValue($E24,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="H24" s="146"/>
       <c r="I24" s="145" t="b">
@@ -6476,9 +6476,9 @@
         <f>_xll.ohObjectPropertyValues(E25,"Rate")</f>
         <v>HKD8x11F_Quote</v>
       </c>
-      <c r="G25" s="146" t="e">
+      <c r="G25" s="146">
         <f>_xll.qlRateHelperQuoteValue($E25,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.6999999999999993E-3</v>
       </c>
       <c r="H25" s="146"/>
       <c r="I25" s="145" t="b">
@@ -6521,9 +6521,9 @@
         <f>_xll.ohObjectPropertyValues(E26,"Rate")</f>
         <v>HKD9x12F_Quote</v>
       </c>
-      <c r="G26" s="146" t="e">
+      <c r="G26" s="146">
         <f>_xll.qlRateHelperQuoteValue($E26,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="H26" s="146"/>
       <c r="I26" s="145" t="b">
@@ -9343,17 +9343,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_1S12</v>
       </c>
-      <c r="F89" s="155" t="str">
+      <c r="F89" s="155" t="e">
         <f>_xll.ohObjectPropertyValues(E89,"Rate")</f>
-        <v>HKD1S12_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G89" s="154" t="e">
         <f>_xll.qlRateHelperQuoteValue($E89,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H89" s="154">
+      <c r="H89" s="154" t="e">
         <f>_xll.qlSwapRateHelperSpread($E89,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I89" s="153" t="b">
         <v>0</v>
@@ -9364,13 +9364,13 @@
       <c r="K89" s="153">
         <v>1</v>
       </c>
-      <c r="L89" s="152">
+      <c r="L89" s="152" t="e">
         <f>_xll.qlRateHelperEarliestDate($E89,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M89" s="151">
+        <v>#NUM!</v>
+      </c>
+      <c r="M89" s="151" t="e">
         <f>_xll.qlRateHelperLatestDate($E89,Trigger)</f>
-        <v>41962</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.2">
@@ -9385,17 +9385,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_2S12</v>
       </c>
-      <c r="F90" s="147" t="str">
+      <c r="F90" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E90,"Rate")</f>
-        <v>HKD2S12_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G90" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E90,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H90" s="146">
+      <c r="H90" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E90,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I90" s="145" t="b">
         <v>0</v>
@@ -9406,13 +9406,13 @@
       <c r="K90" s="145">
         <v>1</v>
       </c>
-      <c r="L90" s="144">
+      <c r="L90" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E90,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M90" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M90" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E90,Trigger)</f>
-        <v>41962</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.2">
@@ -9427,17 +9427,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_3S12</v>
       </c>
-      <c r="F91" s="147" t="str">
+      <c r="F91" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E91,"Rate")</f>
-        <v>HKD3S12_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G91" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E91,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H91" s="146">
+      <c r="H91" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E91,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I91" s="145" t="b">
         <v>0</v>
@@ -9448,13 +9448,13 @@
       <c r="K91" s="145">
         <v>1</v>
       </c>
-      <c r="L91" s="144">
+      <c r="L91" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E91,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M91" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M91" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E91,Trigger)</f>
-        <v>41962</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.2">
@@ -9469,17 +9469,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_4S12</v>
       </c>
-      <c r="F92" s="147" t="str">
+      <c r="F92" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E92,"Rate")</f>
-        <v>HKD4S12_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G92" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E92,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H92" s="146">
+      <c r="H92" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E92,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I92" s="145" t="b">
         <v>0</v>
@@ -9490,13 +9490,13 @@
       <c r="K92" s="145">
         <v>1</v>
       </c>
-      <c r="L92" s="144">
+      <c r="L92" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E92,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M92" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M92" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E92,Trigger)</f>
-        <v>41962</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.2">
@@ -9511,17 +9511,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_1S24</v>
       </c>
-      <c r="F93" s="147" t="str">
+      <c r="F93" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E93,"Rate")</f>
-        <v>HKD1S24_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G93" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E93,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H93" s="146">
+      <c r="H93" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E93,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I93" s="145" t="b">
         <v>0</v>
@@ -9532,13 +9532,13 @@
       <c r="K93" s="145">
         <v>1</v>
       </c>
-      <c r="L93" s="144">
+      <c r="L93" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E93,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M93" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M93" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E93,Trigger)</f>
-        <v>42327</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.2">
@@ -9553,17 +9553,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_2S24</v>
       </c>
-      <c r="F94" s="147" t="str">
+      <c r="F94" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E94,"Rate")</f>
-        <v>HKD2S24_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G94" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E94,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H94" s="146">
+      <c r="H94" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E94,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I94" s="145" t="b">
         <v>0</v>
@@ -9574,13 +9574,13 @@
       <c r="K94" s="145">
         <v>1</v>
       </c>
-      <c r="L94" s="144">
+      <c r="L94" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E94,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M94" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M94" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E94,Trigger)</f>
-        <v>42327</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.2">
@@ -9595,17 +9595,17 @@
         <f t="shared" si="5"/>
         <v>HKD_YC3MRH_1S36</v>
       </c>
-      <c r="F95" s="140" t="str">
+      <c r="F95" s="140" t="e">
         <f>_xll.ohObjectPropertyValues(E95,"Rate")</f>
-        <v>HKD1S36_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G95" s="139" t="e">
         <f>_xll.qlRateHelperQuoteValue($E95,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H95" s="139">
+      <c r="H95" s="139" t="e">
         <f>_xll.qlSwapRateHelperSpread($E95,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I95" s="138" t="b">
         <v>0</v>
@@ -9616,13 +9616,13 @@
       <c r="K95" s="138">
         <v>1</v>
       </c>
-      <c r="L95" s="137">
+      <c r="L95" s="137" t="e">
         <f>_xll.qlRateHelperEarliestDate($E95,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M95" s="136">
+        <v>#NUM!</v>
+      </c>
+      <c r="M95" s="136" t="e">
         <f>_xll.qlRateHelperLatestDate($E95,Trigger)</f>
-        <v>42695</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.2">
@@ -9645,9 +9645,9 @@
         <f>_xll.ohObjectPropertyValues(E96,"Rate")</f>
         <v>HKDQM3H1Y_Quote</v>
       </c>
-      <c r="G96" s="146" t="e">
+      <c r="G96" s="146">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.3E-3</v>
       </c>
       <c r="H96" s="146">
         <f>_xll.qlSwapRateHelperSpread($E96,Trigger)</f>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="I96" s="145" t="b">
         <f t="shared" ref="I96:I132" si="8">IF(ISERROR(G96),FALSE,TRUE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" s="145">
         <v>50</v>
@@ -9747,9 +9747,9 @@
         <f>_xll.ohObjectPropertyValues(E98,"Rate")</f>
         <v>HKDQM3H18M_Quote</v>
       </c>
-      <c r="G98" s="146" t="e">
+      <c r="G98" s="146">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.6999999999999993E-3</v>
       </c>
       <c r="H98" s="146">
         <f>_xll.qlSwapRateHelperSpread($E98,Trigger)</f>
@@ -9757,7 +9757,7 @@
       </c>
       <c r="I98" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J98" s="145">
         <v>50</v>
@@ -9849,9 +9849,9 @@
         <f>_xll.ohObjectPropertyValues(E100,"Rate")</f>
         <v>HKDQM3H2Y_Quote</v>
       </c>
-      <c r="G100" s="146" t="e">
+      <c r="G100" s="146">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
-        <v>#NUM!</v>
+        <v>5.3E-3</v>
       </c>
       <c r="H100" s="146">
         <f>_xll.qlSwapRateHelperSpread($E100,Trigger)</f>
@@ -9859,7 +9859,7 @@
       </c>
       <c r="I100" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J100" s="145">
         <v>50</v>
@@ -9900,9 +9900,9 @@
         <f>_xll.ohObjectPropertyValues(E101,"Rate")</f>
         <v>HKDQM3H3Y_Quote</v>
       </c>
-      <c r="G101" s="146" t="e">
+      <c r="G101" s="146">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
-        <v>#NUM!</v>
+        <v>7.6E-3</v>
       </c>
       <c r="H101" s="146">
         <f>_xll.qlSwapRateHelperSpread($E101,Trigger)</f>
@@ -9910,7 +9910,7 @@
       </c>
       <c r="I101" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J101" s="145">
         <v>50</v>
@@ -9951,9 +9951,9 @@
         <f>_xll.ohObjectPropertyValues(E102,"Rate")</f>
         <v>HKDQM3H4Y_Quote</v>
       </c>
-      <c r="G102" s="146" t="e">
+      <c r="G102" s="146">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.1099999999999999E-2</v>
       </c>
       <c r="H102" s="146">
         <f>_xll.qlSwapRateHelperSpread($E102,Trigger)</f>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="I102" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J102" s="145">
         <v>50</v>
@@ -10002,9 +10002,9 @@
         <f>_xll.ohObjectPropertyValues(E103,"Rate")</f>
         <v>HKDQM3H5Y_Quote</v>
       </c>
-      <c r="G103" s="146" t="e">
+      <c r="G103" s="146">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1.47E-2</v>
       </c>
       <c r="H103" s="146">
         <f>_xll.qlSwapRateHelperSpread($E103,Trigger)</f>
@@ -10012,7 +10012,7 @@
       </c>
       <c r="I103" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J103" s="145">
         <v>50</v>
@@ -10104,9 +10104,9 @@
         <f>_xll.ohObjectPropertyValues(E105,"Rate")</f>
         <v>HKDQM3H7Y_Quote</v>
       </c>
-      <c r="G105" s="146" t="e">
+      <c r="G105" s="146">
         <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.0300000000000002E-2</v>
       </c>
       <c r="H105" s="146">
         <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
@@ -10114,7 +10114,7 @@
       </c>
       <c r="I105" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J105" s="145">
         <v>50</v>
@@ -10257,9 +10257,9 @@
         <f>_xll.ohObjectPropertyValues(E108,"Rate")</f>
         <v>HKDQM3H10Y_Quote</v>
       </c>
-      <c r="G108" s="146" t="e">
+      <c r="G108" s="146">
         <f>_xll.qlRateHelperQuoteValue($E108,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.5599999999999998E-2</v>
       </c>
       <c r="H108" s="146">
         <f>_xll.qlSwapRateHelperSpread($E108,Trigger)</f>
@@ -10267,7 +10267,7 @@
       </c>
       <c r="I108" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J108" s="145">
         <v>50</v>
@@ -10359,9 +10359,9 @@
         <f>_xll.ohObjectPropertyValues(E110,"Rate")</f>
         <v>HKDQM3H12Y_Quote</v>
       </c>
-      <c r="G110" s="146" t="e">
+      <c r="G110" s="146">
         <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.76E-2</v>
       </c>
       <c r="H110" s="146">
         <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
@@ -10369,7 +10369,7 @@
       </c>
       <c r="I110" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" s="145">
         <v>50</v>
@@ -10512,9 +10512,9 @@
         <f>_xll.ohObjectPropertyValues(E113,"Rate")</f>
         <v>HKDQM3H15Y_Quote</v>
       </c>
-      <c r="G113" s="146" t="e">
+      <c r="G113" s="146">
         <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="H113" s="146">
         <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
@@ -10522,7 +10522,7 @@
       </c>
       <c r="I113" s="145" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" s="145">
         <v>50</v>
@@ -11018,17 +11018,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H25Y</v>
       </c>
-      <c r="F123" s="147" t="str">
+      <c r="F123" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E123,"Rate")</f>
-        <v>HKDQM3H25Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G123" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E123,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H123" s="146">
+      <c r="H123" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E123,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I123" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11040,13 +11040,13 @@
       <c r="K123" s="145">
         <v>1</v>
       </c>
-      <c r="L123" s="144">
+      <c r="L123" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E123,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M123" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M123" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E123,Trigger)</f>
-        <v>50728</v>
+        <v>#NUM!</v>
       </c>
       <c r="O123" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11069,17 +11069,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H26Y</v>
       </c>
-      <c r="F124" s="147" t="str">
+      <c r="F124" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E124,"Rate")</f>
-        <v>HKDQM3H26Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G124" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E124,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H124" s="146">
+      <c r="H124" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E124,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I124" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11091,13 +11091,13 @@
       <c r="K124" s="145">
         <v>1</v>
       </c>
-      <c r="L124" s="144">
+      <c r="L124" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E124,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M124" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M124" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E124,Trigger)</f>
-        <v>51095</v>
+        <v>#NUM!</v>
       </c>
       <c r="O124" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11120,17 +11120,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H27Y</v>
       </c>
-      <c r="F125" s="147" t="str">
+      <c r="F125" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E125,"Rate")</f>
-        <v>HKDQM3H27Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G125" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E125,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H125" s="146">
+      <c r="H125" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E125,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I125" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11142,13 +11142,13 @@
       <c r="K125" s="145">
         <v>1</v>
       </c>
-      <c r="L125" s="144">
+      <c r="L125" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E125,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M125" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M125" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E125,Trigger)</f>
-        <v>51459</v>
+        <v>#NUM!</v>
       </c>
       <c r="O125" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11171,17 +11171,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H28Y</v>
       </c>
-      <c r="F126" s="147" t="str">
+      <c r="F126" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E126,"Rate")</f>
-        <v>HKDQM3H28Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G126" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E126,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H126" s="146">
+      <c r="H126" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E126,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I126" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11193,13 +11193,13 @@
       <c r="K126" s="145">
         <v>1</v>
       </c>
-      <c r="L126" s="144">
+      <c r="L126" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E126,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M126" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M126" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E126,Trigger)</f>
-        <v>51824</v>
+        <v>#NUM!</v>
       </c>
       <c r="O126" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11222,17 +11222,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H29Y</v>
       </c>
-      <c r="F127" s="147" t="str">
+      <c r="F127" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E127,"Rate")</f>
-        <v>HKDQM3H29Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G127" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E127,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H127" s="146">
+      <c r="H127" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E127,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I127" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11244,13 +11244,13 @@
       <c r="K127" s="145">
         <v>1</v>
       </c>
-      <c r="L127" s="144">
+      <c r="L127" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E127,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M127" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M127" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E127,Trigger)</f>
-        <v>52189</v>
+        <v>#NUM!</v>
       </c>
       <c r="O127" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11273,17 +11273,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H30Y</v>
       </c>
-      <c r="F128" s="147" t="str">
+      <c r="F128" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E128,"Rate")</f>
-        <v>HKDQM3H30Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G128" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E128,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H128" s="146">
+      <c r="H128" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E128,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I128" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11295,13 +11295,13 @@
       <c r="K128" s="145">
         <v>1</v>
       </c>
-      <c r="L128" s="144">
+      <c r="L128" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E128,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M128" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M128" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E128,Trigger)</f>
-        <v>52554</v>
+        <v>#NUM!</v>
       </c>
       <c r="O128" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11324,17 +11324,17 @@
         <f t="shared" si="10"/>
         <v>HKD_YC3MRH_QM3H35Y</v>
       </c>
-      <c r="F129" s="147" t="str">
+      <c r="F129" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E129,"Rate")</f>
-        <v>HKDQM3H35Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G129" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E129,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H129" s="146">
+      <c r="H129" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E129,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I129" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11346,13 +11346,13 @@
       <c r="K129" s="145">
         <v>1</v>
       </c>
-      <c r="L129" s="144">
+      <c r="L129" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E129,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M129" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M129" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E129,Trigger)</f>
-        <v>54381</v>
+        <v>#NUM!</v>
       </c>
       <c r="O129" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11375,17 +11375,17 @@
         <f t="shared" ref="E130:E161" si="12">RateHelperPrefix&amp;"_"&amp;$B130&amp;$C130&amp;$D130</f>
         <v>HKD_YC3MRH_QM3H40Y</v>
       </c>
-      <c r="F130" s="147" t="str">
+      <c r="F130" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E130,"Rate")</f>
-        <v>HKDQM3H40Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G130" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E130,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H130" s="146">
+      <c r="H130" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E130,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I130" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11397,13 +11397,13 @@
       <c r="K130" s="145">
         <v>1</v>
       </c>
-      <c r="L130" s="144">
+      <c r="L130" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E130,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M130" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M130" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E130,Trigger)</f>
-        <v>56207</v>
+        <v>#NUM!</v>
       </c>
       <c r="O130" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11426,17 +11426,17 @@
         <f t="shared" si="12"/>
         <v>HKD_YC3MRH_QM3H50Y</v>
       </c>
-      <c r="F131" s="147" t="str">
+      <c r="F131" s="147" t="e">
         <f>_xll.ohObjectPropertyValues(E131,"Rate")</f>
-        <v>HKDQM3H50Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G131" s="146" t="e">
         <f>_xll.qlRateHelperQuoteValue($E131,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H131" s="146">
+      <c r="H131" s="146" t="e">
         <f>_xll.qlSwapRateHelperSpread($E131,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I131" s="145" t="b">
         <f t="shared" si="8"/>
@@ -11448,13 +11448,13 @@
       <c r="K131" s="145">
         <v>1</v>
       </c>
-      <c r="L131" s="144">
+      <c r="L131" s="144" t="e">
         <f>_xll.qlRateHelperEarliestDate($E131,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M131" s="143">
+        <v>#NUM!</v>
+      </c>
+      <c r="M131" s="143" t="e">
         <f>_xll.qlRateHelperLatestDate($E131,Trigger)</f>
-        <v>59859</v>
+        <v>#NUM!</v>
       </c>
       <c r="O131" s="150" t="e">
         <f t="shared" si="9"/>
@@ -11477,17 +11477,17 @@
         <f t="shared" si="12"/>
         <v>HKD_YC3MRH_QM3H60Y</v>
       </c>
-      <c r="F132" s="140" t="str">
+      <c r="F132" s="140" t="e">
         <f>_xll.ohObjectPropertyValues(E132,"Rate")</f>
-        <v>HKDQM3H60Y_Quote</v>
+        <v>#NUM!</v>
       </c>
       <c r="G132" s="139" t="e">
         <f>_xll.qlRateHelperQuoteValue($E132,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H132" s="139">
+      <c r="H132" s="139" t="e">
         <f>_xll.qlSwapRateHelperSpread($E132,Trigger)</f>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
       <c r="I132" s="138" t="b">
         <f t="shared" si="8"/>
@@ -11499,13 +11499,13 @@
       <c r="K132" s="138">
         <v>1</v>
       </c>
-      <c r="L132" s="137">
+      <c r="L132" s="137" t="e">
         <f>_xll.qlRateHelperEarliestDate($E132,Trigger)</f>
-        <v>41597</v>
-      </c>
-      <c r="M132" s="136">
+        <v>#NUM!</v>
+      </c>
+      <c r="M132" s="136" t="e">
         <f>_xll.qlRateHelperLatestDate($E132,Trigger)</f>
-        <v>63513</v>
+        <v>#NUM!</v>
       </c>
       <c r="O132" s="150" t="e">
         <f t="shared" si="9"/>
@@ -13229,8 +13229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -13246,10 +13246,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="193" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="193"/>
+      <c r="B1" s="194"/>
       <c r="D1" s="185" t="s">
         <v>156</v>
       </c>
@@ -13263,9 +13263,9 @@
       <c r="H1" s="183" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="165" t="e">
+      <c r="I1" s="165">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -13275,16 +13275,16 @@
       <c r="B2" s="181">
         <v>0</v>
       </c>
-      <c r="C2" s="197" t="s">
+      <c r="C2" s="186" t="s">
         <v>158</v>
       </c>
       <c r="D2" s="173" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>HKD_YC3MRH_1x4F</v>
       </c>
-      <c r="E2" s="172" t="e">
+      <c r="E2" s="172">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="F2" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -13298,8 +13298,8 @@
         <f>_xll.qlRateHelperLatestDate($D2)</f>
         <v>41717</v>
       </c>
-      <c r="I2" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I2" s="165">
+        <v>0.99865364000379186</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -13309,15 +13309,15 @@
       <c r="B3" s="180">
         <v>0</v>
       </c>
-      <c r="C3" s="197" t="s">
+      <c r="C3" s="186" t="s">
         <v>159</v>
       </c>
       <c r="D3" s="173" t="str">
         <v>HKD_YC3MRH_2x5F</v>
       </c>
-      <c r="E3" s="172" t="e">
+      <c r="E3" s="172">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="F3" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -13331,8 +13331,8 @@
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41751</v>
       </c>
-      <c r="I3" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I3" s="165">
+        <v>0.99827251130700834</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -13342,15 +13342,15 @@
       <c r="B4" s="180">
         <v>0</v>
       </c>
-      <c r="C4" s="197" t="s">
+      <c r="C4" s="186" t="s">
         <v>160</v>
       </c>
       <c r="D4" s="173" t="str">
         <v>HKD_YC3MRH_3x6F</v>
       </c>
-      <c r="E4" s="172" t="e">
+      <c r="E4" s="172">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="F4" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -13364,8 +13364,8 @@
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41778</v>
       </c>
-      <c r="I4" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I4" s="165">
+        <v>0.9979699290571088</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -13375,15 +13375,15 @@
       <c r="B5" s="179" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="197" t="s">
+      <c r="C5" s="186" t="s">
         <v>161</v>
       </c>
       <c r="D5" s="173" t="str">
         <v>HKD_YC3MRH_4x7F</v>
       </c>
-      <c r="E5" s="172" t="e">
+      <c r="E5" s="172">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>#NUM!</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="F5" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -13397,8 +13397,8 @@
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41809</v>
       </c>
-      <c r="I5" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I5" s="165">
+        <v>0.99759755316932308</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -13409,15 +13409,15 @@
         <f>_xll.ohRangeRetrieveError(Selected!D2)</f>
         <v/>
       </c>
-      <c r="C6" s="197" t="s">
+      <c r="C6" s="186" t="s">
         <v>162</v>
       </c>
       <c r="D6" s="173" t="str">
         <v>HKD_YC3MRH_5x8F</v>
       </c>
-      <c r="E6" s="172" t="e">
+      <c r="E6" s="172">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>#NUM!</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="F6" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -13431,8 +13431,8 @@
         <f>_xll.qlRateHelperLatestDate($D6)</f>
         <v>41842</v>
       </c>
-      <c r="I6" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I6" s="165">
+        <v>0.99717862002060076</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -13444,15 +13444,15 @@
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
-      <c r="C7" s="197" t="s">
+      <c r="C7" s="186" t="s">
         <v>163</v>
       </c>
       <c r="D7" s="173" t="str">
         <v>HKD_YC3MRH_6x9F</v>
       </c>
-      <c r="E7" s="172" t="e">
+      <c r="E7" s="172">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>#NUM!</v>
+        <v>4.5000000000000005E-3</v>
       </c>
       <c r="F7" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -13466,20 +13466,20 @@
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41870</v>
       </c>
-      <c r="I7" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I7" s="165">
+        <v>0.99683926753185581</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C8" s="197" t="s">
+      <c r="C8" s="186" t="s">
         <v>164</v>
       </c>
       <c r="D8" s="173" t="str">
         <v>HKD_YC3MRH_7x10F</v>
       </c>
-      <c r="E8" s="172" t="e">
+      <c r="E8" s="172">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>#NUM!</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="F8" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -13493,20 +13493,20 @@
         <f>_xll.qlRateHelperLatestDate($D8)</f>
         <v>41901</v>
       </c>
-      <c r="I8" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I8" s="165">
+        <v>0.99644222618257106</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C9" s="197" t="s">
+      <c r="C9" s="186" t="s">
         <v>165</v>
       </c>
       <c r="D9" s="173" t="str">
         <v>HKD_YC3MRH_8x11F</v>
       </c>
-      <c r="E9" s="172" t="e">
+      <c r="E9" s="172">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>#NUM!</v>
+        <v>4.6999999999999993E-3</v>
       </c>
       <c r="F9" s="172" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -13520,280 +13520,280 @@
         <f>_xll.qlRateHelperLatestDate($D9)</f>
         <v>41933</v>
       </c>
-      <c r="I9" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I9" s="165">
+        <v>0.9960111163011619</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="197" t="s">
+      <c r="C10" s="186" t="s">
         <v>166</v>
       </c>
       <c r="D10" s="173" t="str">
-        <v>HKD_YC3MRH_9x12F</v>
-      </c>
-      <c r="E10" s="172" t="e">
+        <v>HKD_YC3MRH_QM3H1Y</v>
+      </c>
+      <c r="E10" s="172">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" s="172" t="str">
+        <v>4.3E-3</v>
+      </c>
+      <c r="F10" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G10" s="171">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41870</v>
+        <v>41597</v>
       </c>
       <c r="H10" s="170">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
         <v>41962</v>
       </c>
-      <c r="I10" s="165" t="e">
-        <v>#NUM!</v>
+      <c r="I10" s="165">
+        <v>0.99571132137697649</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="197" t="s">
+      <c r="C11" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E11" s="172" t="e">
+      <c r="D11" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H18M</v>
+      </c>
+      <c r="E11" s="172">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F11" s="172" t="str">
+        <v>4.6999999999999993E-3</v>
+      </c>
+      <c r="F11" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
-        <v>--</v>
-      </c>
-      <c r="G11" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G11" s="171">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H11" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H11" s="170">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I11" s="165" t="e">
-        <v>#NUM!</v>
+        <v>42143</v>
+      </c>
+      <c r="I11" s="165">
+        <v>0.99299630830453089</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="174"/>
-      <c r="C12" s="197" t="s">
+      <c r="C12" s="186" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E12" s="172" t="e">
+      <c r="D12" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H2Y</v>
+      </c>
+      <c r="E12" s="172">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F12" s="172" t="str">
+        <v>5.3E-3</v>
+      </c>
+      <c r="F12" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
-        <v>--</v>
-      </c>
-      <c r="G12" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G12" s="171">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H12" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H12" s="170">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I12" s="165" t="e">
-        <v>#NUM!</v>
+        <v>42327</v>
+      </c>
+      <c r="I12" s="165">
+        <v>0.98945601666677208</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="174"/>
-      <c r="C13" s="197" t="s">
+      <c r="C13" s="186" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E13" s="172" t="e">
+      <c r="D13" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H3Y</v>
+      </c>
+      <c r="E13" s="172">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F13" s="172" t="str">
+        <v>7.6E-3</v>
+      </c>
+      <c r="F13" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
-        <v>--</v>
-      </c>
-      <c r="G13" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G13" s="171">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H13" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H13" s="170">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I13" s="165" t="e">
-        <v>#NUM!</v>
+        <v>42695</v>
+      </c>
+      <c r="I13" s="165">
+        <v>0.97735274243881276</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="197" t="s">
+      <c r="C14" s="186" t="s">
         <v>170</v>
       </c>
-      <c r="D14" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E14" s="172" t="e">
+      <c r="D14" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H4Y</v>
+      </c>
+      <c r="E14" s="172">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F14" s="172" t="str">
+        <v>1.1099999999999999E-2</v>
+      </c>
+      <c r="F14" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
-        <v>--</v>
-      </c>
-      <c r="G14" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G14" s="171">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H14" s="170">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I14" s="165" t="e">
-        <v>#NUM!</v>
+        <v>43059</v>
+      </c>
+      <c r="I14" s="165">
+        <v>0.95624270446839932</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="197" t="s">
+      <c r="C15" s="186" t="s">
         <v>171</v>
       </c>
-      <c r="D15" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E15" s="172" t="e">
+      <c r="D15" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H5Y</v>
+      </c>
+      <c r="E15" s="172">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F15" s="172" t="str">
+        <v>1.47E-2</v>
+      </c>
+      <c r="F15" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
-        <v>--</v>
-      </c>
-      <c r="G15" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G15" s="171">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H15" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H15" s="170">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I15" s="165" t="e">
-        <v>#NUM!</v>
+        <v>43423</v>
+      </c>
+      <c r="I15" s="165">
+        <v>0.92828234810586951</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="197" t="s">
+      <c r="C16" s="186" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E16" s="172" t="e">
+      <c r="D16" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H7Y</v>
+      </c>
+      <c r="E16" s="172">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F16" s="172" t="str">
+        <v>2.0300000000000002E-2</v>
+      </c>
+      <c r="F16" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
-        <v>--</v>
-      </c>
-      <c r="G16" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G16" s="171">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H16" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H16" s="170">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I16" s="165" t="e">
-        <v>#NUM!</v>
+        <v>44154</v>
+      </c>
+      <c r="I16" s="165">
+        <v>0.8646603036537861</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C17" s="197" t="s">
+      <c r="C17" s="186" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E17" s="172" t="e">
+      <c r="D17" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H10Y</v>
+      </c>
+      <c r="E17" s="172">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F17" s="172" t="str">
+        <v>2.5599999999999998E-2</v>
+      </c>
+      <c r="F17" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
-        <v>--</v>
-      </c>
-      <c r="G17" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G17" s="171">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H17" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H17" s="170">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I17" s="165" t="e">
-        <v>#NUM!</v>
+        <v>45250</v>
+      </c>
+      <c r="I17" s="165">
+        <v>0.76696491798650923</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C18" s="197" t="s">
+      <c r="C18" s="186" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E18" s="172" t="e">
+      <c r="D18" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H12Y</v>
+      </c>
+      <c r="E18" s="172">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="172" t="str">
+        <v>2.76E-2</v>
+      </c>
+      <c r="F18" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
-        <v>--</v>
-      </c>
-      <c r="G18" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G18" s="171">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H18" s="170">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="165" t="e">
-        <v>#NUM!</v>
+        <v>45980</v>
+      </c>
+      <c r="I18" s="165">
+        <v>0.7082834265744945</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C19" s="197" t="s">
+      <c r="C19" s="186" t="s">
         <v>175</v>
       </c>
-      <c r="D19" s="173" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E19" s="172" t="e">
+      <c r="D19" s="173" t="str">
+        <v>HKD_YC3MRH_QM3H15Y</v>
+      </c>
+      <c r="E19" s="172">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="172" t="str">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="F19" s="172">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
-        <v>--</v>
-      </c>
-      <c r="G19" s="171" t="e">
+        <v>0</v>
+      </c>
+      <c r="G19" s="171">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="170" t="e">
+        <v>41597</v>
+      </c>
+      <c r="H19" s="170">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="165" t="e">
-        <v>#NUM!</v>
+        <v>47077</v>
+      </c>
+      <c r="I19" s="165">
+        <v>0.63770446228634647</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.2">
@@ -13817,7 +13817,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I20" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.2">
@@ -13841,7 +13841,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I21" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.2">
@@ -13865,7 +13865,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I22" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.2">
@@ -13889,7 +13889,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I23" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.2">
@@ -13913,7 +13913,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I24" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.2">
@@ -13937,7 +13937,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I25" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.2">
@@ -13961,7 +13961,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I26" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.2">
@@ -13985,7 +13985,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I27" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.2">
@@ -14009,7 +14009,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I28" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.2">
@@ -14033,7 +14033,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I29" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.2">
@@ -14057,7 +14057,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I30" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.2">
@@ -14081,7 +14081,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I31" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.2">
@@ -14105,7 +14105,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I32" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.2">
@@ -14129,7 +14129,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I33" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.2">
@@ -14153,7 +14153,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I34" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.2">
@@ -14177,7 +14177,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I35" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.2">
@@ -14201,7 +14201,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I36" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.2">
@@ -14225,7 +14225,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I37" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.2">
@@ -14249,7 +14249,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.2">
@@ -14273,7 +14273,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.2">
@@ -14297,7 +14297,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.2">
@@ -14321,7 +14321,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.2">
@@ -14345,7 +14345,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.2">
@@ -14369,7 +14369,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.2">
@@ -14393,7 +14393,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.2">
@@ -14417,7 +14417,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.2">
@@ -14441,7 +14441,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.2">
@@ -14465,7 +14465,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.2">
@@ -14489,7 +14489,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.2">
@@ -14513,7 +14513,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.2">
@@ -14537,7 +14537,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
@@ -14561,7 +14561,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
@@ -14585,7 +14585,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
@@ -14609,7 +14609,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -14633,7 +14633,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
@@ -14657,7 +14657,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
@@ -14681,7 +14681,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
@@ -14705,7 +14705,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
@@ -14729,7 +14729,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
@@ -14753,7 +14753,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
@@ -14777,7 +14777,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
@@ -14801,7 +14801,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
@@ -14825,7 +14825,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
@@ -14849,7 +14849,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
@@ -14873,7 +14873,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.2">
@@ -14897,7 +14897,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.2">
@@ -14921,7 +14921,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.2">
@@ -14945,7 +14945,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.2">
@@ -14969,7 +14969,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.2">
@@ -14993,7 +14993,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.2">
@@ -15017,7 +15017,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.2">
@@ -15041,7 +15041,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.2">
@@ -15065,7 +15065,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.2">
@@ -15089,7 +15089,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.2">
@@ -15113,7 +15113,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.2">
@@ -15137,7 +15137,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.2">
@@ -15161,7 +15161,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.2">
@@ -15185,7 +15185,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.2">
@@ -15209,7 +15209,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.2">
@@ -15233,7 +15233,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.2">
@@ -15257,7 +15257,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="81" spans="4:9" x14ac:dyDescent="0.2">
@@ -15281,7 +15281,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="82" spans="4:9" x14ac:dyDescent="0.2">
@@ -15305,7 +15305,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="83" spans="4:9" x14ac:dyDescent="0.2">
@@ -15329,7 +15329,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="84" spans="4:9" x14ac:dyDescent="0.2">
@@ -15353,7 +15353,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="85" spans="4:9" x14ac:dyDescent="0.2">
@@ -15377,7 +15377,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.2">
@@ -15401,7 +15401,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.2">
@@ -15425,7 +15425,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.2">
@@ -15449,7 +15449,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.2">
@@ -15473,7 +15473,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="90" spans="4:9" x14ac:dyDescent="0.2">
@@ -15497,7 +15497,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="91" spans="4:9" x14ac:dyDescent="0.2">
@@ -15521,7 +15521,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="92" spans="4:9" x14ac:dyDescent="0.2">
@@ -15545,7 +15545,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.2">
@@ -15569,7 +15569,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.2">
@@ -15593,7 +15593,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.2">
@@ -15617,7 +15617,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.2">
@@ -15641,7 +15641,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
@@ -15665,7 +15665,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
@@ -15689,7 +15689,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
@@ -15713,7 +15713,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
@@ -15737,7 +15737,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
@@ -15761,7 +15761,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
@@ -15785,7 +15785,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
@@ -15809,7 +15809,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
@@ -15833,7 +15833,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
@@ -15857,7 +15857,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
@@ -15881,7 +15881,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
@@ -15905,7 +15905,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
@@ -15929,7 +15929,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
@@ -15953,7 +15953,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
@@ -15977,7 +15977,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
@@ -16001,7 +16001,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
@@ -16025,7 +16025,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="113" spans="4:9" x14ac:dyDescent="0.2">
@@ -16049,7 +16049,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
@@ -16073,7 +16073,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
@@ -16097,7 +16097,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
@@ -16121,7 +16121,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
@@ -16145,7 +16145,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
@@ -16169,7 +16169,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
@@ -16193,7 +16193,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
@@ -16217,7 +16217,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
@@ -16241,7 +16241,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
@@ -16265,7 +16265,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
@@ -16289,7 +16289,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
@@ -16313,7 +16313,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
@@ -16337,7 +16337,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -16361,7 +16361,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="165" t="e">
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -16384,7 +16384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16404,13 +16404,13 @@
       </c>
     </row>
     <row r="2" spans="1:33" s="90" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="195" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="197"/>
     </row>
     <row r="3" spans="1:33" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="90"/>
@@ -17370,9 +17370,9 @@
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
         <v>41597</v>
       </c>
-      <c r="D27" s="101" t="e">
+      <c r="D27" s="101">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="E27" s="95"/>
       <c r="F27" s="94"/>
@@ -17409,11 +17409,11 @@
       <c r="B28" s="98"/>
       <c r="C28" s="100">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>41962</v>
-      </c>
-      <c r="D28" s="99" t="e">
+        <v>47077</v>
+      </c>
+      <c r="D28" s="99">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>#NUM!</v>
+        <v>0.63770446228634647</v>
       </c>
       <c r="E28" s="95"/>
       <c r="F28" s="94"/>
@@ -17452,8 +17452,8 @@
         <v>96</v>
       </c>
       <c r="D29" s="96" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 1st instrument (maturity: March 19th, 2014) has an invalid quote</v>
+        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v/>
       </c>
       <c r="E29" s="95"/>
       <c r="F29" s="94"/>

</xml_diff>

<commit_message>
add references to trigger range
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="4"/>
+    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HKD_YCRH_FRAs_3M" sheetId="5" r:id="rId1"/>
@@ -2104,7 +2104,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2193,7 +2195,7 @@
       </c>
       <c r="H3" s="37" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_T3F1#0004</v>
+        <v>HKD_YC3MRH_T3F1#0001</v>
       </c>
       <c r="I3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -2227,7 +2229,7 @@
       </c>
       <c r="H4" s="27" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_TOM3F1#0004</v>
+        <v>HKD_YC3MRH_TOM3F1#0001</v>
       </c>
       <c r="I4" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -2262,7 +2264,7 @@
       </c>
       <c r="H5" s="32" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0004</v>
+        <v>HKD_YC3MRH_1x4F#0001</v>
       </c>
       <c r="I5" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -2297,7 +2299,7 @@
       </c>
       <c r="H6" s="32" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0004</v>
+        <v>HKD_YC3MRH_2x5F#0001</v>
       </c>
       <c r="I6" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -2332,7 +2334,7 @@
       </c>
       <c r="H7" s="32" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0004</v>
+        <v>HKD_YC3MRH_3x6F#0001</v>
       </c>
       <c r="I7" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -2367,7 +2369,7 @@
       </c>
       <c r="H8" s="32" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0004</v>
+        <v>HKD_YC3MRH_4x7F#0001</v>
       </c>
       <c r="I8" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -2402,7 +2404,7 @@
       </c>
       <c r="H9" s="32" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0004</v>
+        <v>HKD_YC3MRH_5x8F#0001</v>
       </c>
       <c r="I9" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -2437,7 +2439,7 @@
       </c>
       <c r="H10" s="32" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0004</v>
+        <v>HKD_YC3MRH_6x9F#0001</v>
       </c>
       <c r="I10" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -2472,7 +2474,7 @@
       </c>
       <c r="H11" s="32" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0004</v>
+        <v>HKD_YC3MRH_7x10F#0001</v>
       </c>
       <c r="I11" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -2507,7 +2509,7 @@
       </c>
       <c r="H12" s="32" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0004</v>
+        <v>HKD_YC3MRH_8x11F#0001</v>
       </c>
       <c r="I12" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -2542,7 +2544,7 @@
       </c>
       <c r="H13" s="27" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0004</v>
+        <v>HKD_YC3MRH_9x12F#0001</v>
       </c>
       <c r="I13" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -2577,7 +2579,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2714,7 +2716,7 @@
       </c>
       <c r="L4" s="70" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H_Hibor3M#0010</v>
+        <v>HKD_YC3MRH_QM3H_Hibor3M#0001</v>
       </c>
       <c r="M4" s="69" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -2793,8 +2795,8 @@
         <v>HKD_YC3MRH_QM3H1Y</v>
       </c>
       <c r="L6" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H1Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H1Y#0002</v>
       </c>
       <c r="M6" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -2840,8 +2842,8 @@
         <v>HKD_YC3MRH_QM3H15M</v>
       </c>
       <c r="L7" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15M#0007</v>
+        <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H15M#0002</v>
       </c>
       <c r="M7" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -2887,8 +2889,8 @@
         <v>HKD_YC3MRH_QM3H18M</v>
       </c>
       <c r="L8" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18M#0007</v>
+        <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H18M#0002</v>
       </c>
       <c r="M8" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -2934,8 +2936,8 @@
         <v>HKD_YC3MRH_QM3H21M</v>
       </c>
       <c r="L9" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21M#0007</v>
+        <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H21M#0002</v>
       </c>
       <c r="M9" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -2981,8 +2983,8 @@
         <v>HKD_YC3MRH_QM3H2Y</v>
       </c>
       <c r="L10" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H2Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H2Y#0002</v>
       </c>
       <c r="M10" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -3028,8 +3030,8 @@
         <v>HKD_YC3MRH_QM3H3Y</v>
       </c>
       <c r="L11" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H3Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H3Y#0002</v>
       </c>
       <c r="M11" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -3075,8 +3077,8 @@
         <v>HKD_YC3MRH_QM3H4Y</v>
       </c>
       <c r="L12" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H4Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H4Y#0002</v>
       </c>
       <c r="M12" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -3122,8 +3124,8 @@
         <v>HKD_YC3MRH_QM3H5Y</v>
       </c>
       <c r="L13" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H5Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H5Y#0002</v>
       </c>
       <c r="M13" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -3169,8 +3171,8 @@
         <v>HKD_YC3MRH_QM3H6Y</v>
       </c>
       <c r="L14" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H6Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H6Y#0002</v>
       </c>
       <c r="M14" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -3216,8 +3218,8 @@
         <v>HKD_YC3MRH_QM3H7Y</v>
       </c>
       <c r="L15" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H7Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H7Y#0002</v>
       </c>
       <c r="M15" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -3263,8 +3265,8 @@
         <v>HKD_YC3MRH_QM3H8Y</v>
       </c>
       <c r="L16" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H8Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H8Y#0002</v>
       </c>
       <c r="M16" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -3310,8 +3312,8 @@
         <v>HKD_YC3MRH_QM3H9Y</v>
       </c>
       <c r="L17" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H9Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H9Y#0002</v>
       </c>
       <c r="M17" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -3357,8 +3359,8 @@
         <v>HKD_YC3MRH_QM3H10Y</v>
       </c>
       <c r="L18" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H10Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H10Y#0002</v>
       </c>
       <c r="M18" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -3404,8 +3406,8 @@
         <v>HKD_YC3MRH_QM3H11Y</v>
       </c>
       <c r="L19" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H11Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H11Y#0002</v>
       </c>
       <c r="M19" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -3451,8 +3453,8 @@
         <v>HKD_YC3MRH_QM3H12Y</v>
       </c>
       <c r="L20" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H12Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H12Y#0002</v>
       </c>
       <c r="M20" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -3498,8 +3500,8 @@
         <v>HKD_YC3MRH_QM3H13Y</v>
       </c>
       <c r="L21" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H13Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H13Y#0002</v>
       </c>
       <c r="M21" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -3545,8 +3547,8 @@
         <v>HKD_YC3MRH_QM3H14Y</v>
       </c>
       <c r="L22" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H14Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H14Y#0002</v>
       </c>
       <c r="M22" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -3592,8 +3594,8 @@
         <v>HKD_YC3MRH_QM3H15Y</v>
       </c>
       <c r="L23" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H15Y#0002</v>
       </c>
       <c r="M23" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -3639,8 +3641,8 @@
         <v>HKD_YC3MRH_QM3H16Y</v>
       </c>
       <c r="L24" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H16Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H16Y#0002</v>
       </c>
       <c r="M24" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -3686,8 +3688,8 @@
         <v>HKD_YC3MRH_QM3H17Y</v>
       </c>
       <c r="L25" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H17Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H17Y#0002</v>
       </c>
       <c r="M25" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -3733,8 +3735,8 @@
         <v>HKD_YC3MRH_QM3H18Y</v>
       </c>
       <c r="L26" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H18Y#0002</v>
       </c>
       <c r="M26" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -3780,8 +3782,8 @@
         <v>HKD_YC3MRH_QM3H19Y</v>
       </c>
       <c r="L27" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H19Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H19Y#0002</v>
       </c>
       <c r="M27" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -3827,8 +3829,8 @@
         <v>HKD_YC3MRH_QM3H20Y</v>
       </c>
       <c r="L28" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H20Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H20Y#0002</v>
       </c>
       <c r="M28" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -3874,8 +3876,8 @@
         <v>HKD_YC3MRH_QM3H21Y</v>
       </c>
       <c r="L29" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H21Y#0002</v>
       </c>
       <c r="M29" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -3921,8 +3923,8 @@
         <v>HKD_YC3MRH_QM3H22Y</v>
       </c>
       <c r="L30" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H22Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H22Y#0002</v>
       </c>
       <c r="M30" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -3968,8 +3970,8 @@
         <v>HKD_YC3MRH_QM3H23Y</v>
       </c>
       <c r="L31" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H23Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H23Y#0002</v>
       </c>
       <c r="M31" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -4015,8 +4017,8 @@
         <v>HKD_YC3MRH_QM3H24Y</v>
       </c>
       <c r="L32" s="58" t="str">
-        <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H24Y#0007</v>
+        <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_QM3H24Y#0002</v>
       </c>
       <c r="M32" s="57" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -4062,7 +4064,7 @@
         <v>HKD_YC3MRH_QM3H25Y</v>
       </c>
       <c r="L33" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M33" s="57" t="str">
@@ -4109,7 +4111,7 @@
         <v>HKD_YC3MRH_QM3H26Y</v>
       </c>
       <c r="L34" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M34" s="57" t="str">
@@ -4156,7 +4158,7 @@
         <v>HKD_YC3MRH_QM3H27Y</v>
       </c>
       <c r="L35" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M35" s="57" t="str">
@@ -4203,7 +4205,7 @@
         <v>HKD_YC3MRH_QM3H28Y</v>
       </c>
       <c r="L36" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M36" s="57" t="str">
@@ -4250,7 +4252,7 @@
         <v>HKD_YC3MRH_QM3H29Y</v>
       </c>
       <c r="L37" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M37" s="57" t="str">
@@ -4297,7 +4299,7 @@
         <v>HKD_YC3MRH_QM3H30Y</v>
       </c>
       <c r="L38" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M38" s="57" t="str">
@@ -4344,7 +4346,7 @@
         <v>HKD_YC3MRH_QM3H35Y</v>
       </c>
       <c r="L39" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M39" s="57" t="str">
@@ -4391,7 +4393,7 @@
         <v>HKD_YC3MRH_QM3H40Y</v>
       </c>
       <c r="L40" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M40" s="57" t="str">
@@ -4438,7 +4440,7 @@
         <v>HKD_YC3MRH_QM3H50Y</v>
       </c>
       <c r="L41" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M41" s="57" t="str">
@@ -4485,7 +4487,7 @@
         <v>HKD_YC3MRH_QM3H60Y</v>
       </c>
       <c r="L42" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M42" s="57" t="str">
@@ -4547,7 +4549,7 @@
         <v>HKD_YC3MRH_1S12</v>
       </c>
       <c r="L44" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M44" s="57" t="str">
@@ -4592,7 +4594,7 @@
         <v>HKD_YC3MRH_2S12</v>
       </c>
       <c r="L45" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M45" s="57" t="str">
@@ -4637,7 +4639,7 @@
         <v>HKD_YC3MRH_3S12</v>
       </c>
       <c r="L46" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M46" s="57" t="str">
@@ -4682,7 +4684,7 @@
         <v>HKD_YC3MRH_4S12</v>
       </c>
       <c r="L47" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M47" s="57" t="str">
@@ -4727,7 +4729,7 @@
         <v>HKD_YC3MRH_1S24</v>
       </c>
       <c r="L48" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M48" s="57" t="str">
@@ -4772,7 +4774,7 @@
         <v>HKD_YC3MRH_2S24</v>
       </c>
       <c r="L49" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M49" s="57" t="str">
@@ -4817,7 +4819,7 @@
         <v>HKD_YC3MRH_1S36</v>
       </c>
       <c r="L50" s="58" t="e">
-        <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
+        <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
       <c r="M50" s="57" t="str">
@@ -12905,7 +12907,7 @@
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="154" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_RateHelpersSelected#0004</v>
+        <v>HKD_YC3MRH_RateHelpersSelected#0001</v>
       </c>
       <c r="B7" s="153" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -15851,7 +15853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16171,7 +16175,7 @@
       </c>
       <c r="D10" s="107" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC3M#0004</v>
+        <v>_HKDYC3M#0001</v>
       </c>
       <c r="E10" s="82"/>
       <c r="F10" s="81"/>

</xml_diff>

<commit_message>
remove redundant rows in ratehelper selection
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="143">
   <si>
     <t>_Quote</t>
   </si>
@@ -633,6 +633,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>=qlPiecewiseYieldCurveData(YieldCurve)</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1297,7 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
@@ -1639,6 +1642,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1661,18 +1676,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="3"/>
@@ -1986,9 +1993,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2077,7 +2082,7 @@
       </c>
       <c r="H3" s="37" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_T3F1#0004</v>
+        <v>HKD_YC3MRH_T3F1#0001</v>
       </c>
       <c r="I3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -2111,7 +2116,7 @@
       </c>
       <c r="H4" s="27" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_TOM3F1#0004</v>
+        <v>HKD_YC3MRH_TOM3F1#0001</v>
       </c>
       <c r="I4" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -2146,7 +2151,7 @@
       </c>
       <c r="H5" s="32" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0004</v>
+        <v>HKD_YC3MRH_1x4F#0001</v>
       </c>
       <c r="I5" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -2181,7 +2186,7 @@
       </c>
       <c r="H6" s="32" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0004</v>
+        <v>HKD_YC3MRH_2x5F#0001</v>
       </c>
       <c r="I6" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -2216,7 +2221,7 @@
       </c>
       <c r="H7" s="32" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0004</v>
+        <v>HKD_YC3MRH_3x6F#0001</v>
       </c>
       <c r="I7" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -2251,7 +2256,7 @@
       </c>
       <c r="H8" s="32" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0004</v>
+        <v>HKD_YC3MRH_4x7F#0001</v>
       </c>
       <c r="I8" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -2286,7 +2291,7 @@
       </c>
       <c r="H9" s="32" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0004</v>
+        <v>HKD_YC3MRH_5x8F#0001</v>
       </c>
       <c r="I9" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -2321,7 +2326,7 @@
       </c>
       <c r="H10" s="32" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0004</v>
+        <v>HKD_YC3MRH_6x9F#0001</v>
       </c>
       <c r="I10" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -2356,7 +2361,7 @@
       </c>
       <c r="H11" s="32" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0004</v>
+        <v>HKD_YC3MRH_7x10F#0001</v>
       </c>
       <c r="I11" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -2391,7 +2396,7 @@
       </c>
       <c r="H12" s="32" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0004</v>
+        <v>HKD_YC3MRH_8x11F#0001</v>
       </c>
       <c r="I12" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -2426,7 +2431,7 @@
       </c>
       <c r="H13" s="27" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0004</v>
+        <v>HKD_YC3MRH_9x12F#0001</v>
       </c>
       <c r="I13" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -2461,9 +2466,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2600,7 +2603,7 @@
       </c>
       <c r="L4" s="69" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H_Hibor3M#0006</v>
+        <v>HKD_YC3MRH_QM3H_Hibor3M#0001</v>
       </c>
       <c r="M4" s="68" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -2680,7 +2683,7 @@
       </c>
       <c r="L6" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H1Y#0006</v>
+        <v>HKD_YC3MRH_QM3H1Y#0001</v>
       </c>
       <c r="M6" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -2727,7 +2730,7 @@
       </c>
       <c r="L7" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15M#0006</v>
+        <v>HKD_YC3MRH_QM3H15M#0001</v>
       </c>
       <c r="M7" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -2774,7 +2777,7 @@
       </c>
       <c r="L8" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18M#0006</v>
+        <v>HKD_YC3MRH_QM3H18M#0001</v>
       </c>
       <c r="M8" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -2821,7 +2824,7 @@
       </c>
       <c r="L9" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21M#0006</v>
+        <v>HKD_YC3MRH_QM3H21M#0001</v>
       </c>
       <c r="M9" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -2868,7 +2871,7 @@
       </c>
       <c r="L10" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H2Y#0006</v>
+        <v>HKD_YC3MRH_QM3H2Y#0001</v>
       </c>
       <c r="M10" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -2915,7 +2918,7 @@
       </c>
       <c r="L11" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H3Y#0006</v>
+        <v>HKD_YC3MRH_QM3H3Y#0001</v>
       </c>
       <c r="M11" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -2962,7 +2965,7 @@
       </c>
       <c r="L12" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H4Y#0006</v>
+        <v>HKD_YC3MRH_QM3H4Y#0001</v>
       </c>
       <c r="M12" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -3009,7 +3012,7 @@
       </c>
       <c r="L13" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H5Y#0006</v>
+        <v>HKD_YC3MRH_QM3H5Y#0001</v>
       </c>
       <c r="M13" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -3056,7 +3059,7 @@
       </c>
       <c r="L14" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H6Y#0006</v>
+        <v>HKD_YC3MRH_QM3H6Y#0001</v>
       </c>
       <c r="M14" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -3103,7 +3106,7 @@
       </c>
       <c r="L15" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H7Y#0006</v>
+        <v>HKD_YC3MRH_QM3H7Y#0001</v>
       </c>
       <c r="M15" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -3150,7 +3153,7 @@
       </c>
       <c r="L16" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H8Y#0006</v>
+        <v>HKD_YC3MRH_QM3H8Y#0001</v>
       </c>
       <c r="M16" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -3197,7 +3200,7 @@
       </c>
       <c r="L17" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H9Y#0006</v>
+        <v>HKD_YC3MRH_QM3H9Y#0001</v>
       </c>
       <c r="M17" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -3244,7 +3247,7 @@
       </c>
       <c r="L18" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H10Y#0006</v>
+        <v>HKD_YC3MRH_QM3H10Y#0001</v>
       </c>
       <c r="M18" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -3291,7 +3294,7 @@
       </c>
       <c r="L19" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H11Y#0006</v>
+        <v>HKD_YC3MRH_QM3H11Y#0001</v>
       </c>
       <c r="M19" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -3338,7 +3341,7 @@
       </c>
       <c r="L20" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H12Y#0006</v>
+        <v>HKD_YC3MRH_QM3H12Y#0001</v>
       </c>
       <c r="M20" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -3385,7 +3388,7 @@
       </c>
       <c r="L21" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H13Y#0006</v>
+        <v>HKD_YC3MRH_QM3H13Y#0001</v>
       </c>
       <c r="M21" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -3432,7 +3435,7 @@
       </c>
       <c r="L22" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H14Y#0006</v>
+        <v>HKD_YC3MRH_QM3H14Y#0001</v>
       </c>
       <c r="M22" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -3479,7 +3482,7 @@
       </c>
       <c r="L23" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15Y#0006</v>
+        <v>HKD_YC3MRH_QM3H15Y#0001</v>
       </c>
       <c r="M23" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -3526,7 +3529,7 @@
       </c>
       <c r="L24" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H16Y#0006</v>
+        <v>HKD_YC3MRH_QM3H16Y#0001</v>
       </c>
       <c r="M24" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -3573,7 +3576,7 @@
       </c>
       <c r="L25" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H17Y#0006</v>
+        <v>HKD_YC3MRH_QM3H17Y#0001</v>
       </c>
       <c r="M25" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -3620,7 +3623,7 @@
       </c>
       <c r="L26" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18Y#0006</v>
+        <v>HKD_YC3MRH_QM3H18Y#0001</v>
       </c>
       <c r="M26" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -3667,7 +3670,7 @@
       </c>
       <c r="L27" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H19Y#0006</v>
+        <v>HKD_YC3MRH_QM3H19Y#0001</v>
       </c>
       <c r="M27" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -3714,7 +3717,7 @@
       </c>
       <c r="L28" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H20Y#0006</v>
+        <v>HKD_YC3MRH_QM3H20Y#0001</v>
       </c>
       <c r="M28" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -3761,7 +3764,7 @@
       </c>
       <c r="L29" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21Y#0006</v>
+        <v>HKD_YC3MRH_QM3H21Y#0001</v>
       </c>
       <c r="M29" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -3808,7 +3811,7 @@
       </c>
       <c r="L30" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H22Y#0006</v>
+        <v>HKD_YC3MRH_QM3H22Y#0001</v>
       </c>
       <c r="M30" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -3855,7 +3858,7 @@
       </c>
       <c r="L31" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H23Y#0006</v>
+        <v>HKD_YC3MRH_QM3H23Y#0001</v>
       </c>
       <c r="M31" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -3902,7 +3905,7 @@
       </c>
       <c r="L32" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H24Y#0006</v>
+        <v>HKD_YC3MRH_QM3H24Y#0001</v>
       </c>
       <c r="M32" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -4425,9 +4428,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K123"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4445,38 +4446,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="158" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="166" t="s">
+      <c r="B1" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="166" t="s">
+      <c r="C1" s="158" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="166" t="s">
+      <c r="D1" s="158" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="166" t="s">
+      <c r="E1" s="158" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="166" t="s">
+      <c r="F1" s="158" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="166" t="s">
+      <c r="G1" s="158" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="166" t="s">
+      <c r="H1" s="158" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="166" t="s">
+      <c r="I1" s="158" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="167" t="str">
+      <c r="A2" s="159" t="str">
         <f>HKD_YCRH_FRAs_3M!H3</f>
-        <v>HKD_YC3MRH_T3F1#0004</v>
+        <v>HKD_YC3MRH_T3F1#0001</v>
       </c>
       <c r="B2" s="128" t="str">
         <f>_xll.ohObjectPropertyValues(A2,"Rate")</f>
@@ -4512,9 +4513,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="168" t="str">
+      <c r="A3" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H4</f>
-        <v>HKD_YC3MRH_TOM3F1#0004</v>
+        <v>HKD_YC3MRH_TOM3F1#0001</v>
       </c>
       <c r="B3" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A3,"Rate")</f>
@@ -4550,9 +4551,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="168" t="str">
+      <c r="A4" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H5</f>
-        <v>HKD_YC3MRH_1x4F#0004</v>
+        <v>HKD_YC3MRH_1x4F#0001</v>
       </c>
       <c r="B4" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A4,"Rate")</f>
@@ -4588,9 +4589,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="168" t="str">
+      <c r="A5" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H6</f>
-        <v>HKD_YC3MRH_2x5F#0004</v>
+        <v>HKD_YC3MRH_2x5F#0001</v>
       </c>
       <c r="B5" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A5,"Rate")</f>
@@ -4626,9 +4627,9 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="168" t="str">
+      <c r="A6" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H7</f>
-        <v>HKD_YC3MRH_3x6F#0004</v>
+        <v>HKD_YC3MRH_3x6F#0001</v>
       </c>
       <c r="B6" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A6,"Rate")</f>
@@ -4664,9 +4665,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="168" t="str">
+      <c r="A7" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H8</f>
-        <v>HKD_YC3MRH_4x7F#0004</v>
+        <v>HKD_YC3MRH_4x7F#0001</v>
       </c>
       <c r="B7" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A7,"Rate")</f>
@@ -4702,9 +4703,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="168" t="str">
+      <c r="A8" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H9</f>
-        <v>HKD_YC3MRH_5x8F#0004</v>
+        <v>HKD_YC3MRH_5x8F#0001</v>
       </c>
       <c r="B8" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A8,"Rate")</f>
@@ -4740,9 +4741,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="168" t="str">
+      <c r="A9" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H10</f>
-        <v>HKD_YC3MRH_6x9F#0004</v>
+        <v>HKD_YC3MRH_6x9F#0001</v>
       </c>
       <c r="B9" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A9,"Rate")</f>
@@ -4772,9 +4773,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="168" t="str">
+      <c r="A10" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H11</f>
-        <v>HKD_YC3MRH_7x10F#0004</v>
+        <v>HKD_YC3MRH_7x10F#0001</v>
       </c>
       <c r="B10" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A10,"Rate")</f>
@@ -4804,9 +4805,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="168" t="str">
+      <c r="A11" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H12</f>
-        <v>HKD_YC3MRH_8x11F#0004</v>
+        <v>HKD_YC3MRH_8x11F#0001</v>
       </c>
       <c r="B11" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A11,"Rate")</f>
@@ -4836,9 +4837,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="169" t="str">
+      <c r="A12" s="161" t="str">
         <f>HKD_YCRH_FRAs_3M!H13</f>
-        <v>HKD_YC3MRH_9x12F#0004</v>
+        <v>HKD_YC3MRH_9x12F#0001</v>
       </c>
       <c r="B12" s="117" t="str">
         <f>_xll.ohObjectPropertyValues(A12,"Rate")</f>
@@ -4868,9 +4869,9 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="168" t="str">
+      <c r="A13" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L6</f>
-        <v>HKD_YC3MRH_QM3H1Y#0006</v>
+        <v>HKD_YC3MRH_QM3H1Y#0001</v>
       </c>
       <c r="B13" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A13,"Rate")</f>
@@ -4904,9 +4905,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="168" t="str">
+      <c r="A14" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L7</f>
-        <v>HKD_YC3MRH_QM3H15M#0006</v>
+        <v>HKD_YC3MRH_QM3H15M#0001</v>
       </c>
       <c r="B14" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A14,"Rate")</f>
@@ -4940,9 +4941,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="168" t="str">
+      <c r="A15" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L8</f>
-        <v>HKD_YC3MRH_QM3H18M#0006</v>
+        <v>HKD_YC3MRH_QM3H18M#0001</v>
       </c>
       <c r="B15" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A15,"Rate")</f>
@@ -4976,9 +4977,9 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="168" t="str">
+      <c r="A16" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L9</f>
-        <v>HKD_YC3MRH_QM3H21M#0006</v>
+        <v>HKD_YC3MRH_QM3H21M#0001</v>
       </c>
       <c r="B16" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A16,"Rate")</f>
@@ -5012,9 +5013,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="168" t="str">
+      <c r="A17" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L10</f>
-        <v>HKD_YC3MRH_QM3H2Y#0006</v>
+        <v>HKD_YC3MRH_QM3H2Y#0001</v>
       </c>
       <c r="B17" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A17,"Rate")</f>
@@ -5048,9 +5049,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="168" t="str">
+      <c r="A18" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L11</f>
-        <v>HKD_YC3MRH_QM3H3Y#0006</v>
+        <v>HKD_YC3MRH_QM3H3Y#0001</v>
       </c>
       <c r="B18" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A18,"Rate")</f>
@@ -5084,9 +5085,9 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="168" t="str">
+      <c r="A19" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L12</f>
-        <v>HKD_YC3MRH_QM3H4Y#0006</v>
+        <v>HKD_YC3MRH_QM3H4Y#0001</v>
       </c>
       <c r="B19" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A19,"Rate")</f>
@@ -5120,9 +5121,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="168" t="str">
+      <c r="A20" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L13</f>
-        <v>HKD_YC3MRH_QM3H5Y#0006</v>
+        <v>HKD_YC3MRH_QM3H5Y#0001</v>
       </c>
       <c r="B20" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A20,"Rate")</f>
@@ -5156,9 +5157,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="168" t="str">
+      <c r="A21" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L14</f>
-        <v>HKD_YC3MRH_QM3H6Y#0006</v>
+        <v>HKD_YC3MRH_QM3H6Y#0001</v>
       </c>
       <c r="B21" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A21,"Rate")</f>
@@ -5192,9 +5193,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="168" t="str">
+      <c r="A22" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L15</f>
-        <v>HKD_YC3MRH_QM3H7Y#0006</v>
+        <v>HKD_YC3MRH_QM3H7Y#0001</v>
       </c>
       <c r="B22" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A22,"Rate")</f>
@@ -5228,9 +5229,9 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="168" t="str">
+      <c r="A23" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L16</f>
-        <v>HKD_YC3MRH_QM3H8Y#0006</v>
+        <v>HKD_YC3MRH_QM3H8Y#0001</v>
       </c>
       <c r="B23" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A23,"Rate")</f>
@@ -5264,9 +5265,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="168" t="str">
+      <c r="A24" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L17</f>
-        <v>HKD_YC3MRH_QM3H9Y#0006</v>
+        <v>HKD_YC3MRH_QM3H9Y#0001</v>
       </c>
       <c r="B24" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A24,"Rate")</f>
@@ -5300,9 +5301,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="168" t="str">
+      <c r="A25" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L18</f>
-        <v>HKD_YC3MRH_QM3H10Y#0006</v>
+        <v>HKD_YC3MRH_QM3H10Y#0001</v>
       </c>
       <c r="B25" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A25,"Rate")</f>
@@ -5336,9 +5337,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="168" t="str">
+      <c r="A26" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L19</f>
-        <v>HKD_YC3MRH_QM3H11Y#0006</v>
+        <v>HKD_YC3MRH_QM3H11Y#0001</v>
       </c>
       <c r="B26" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A26,"Rate")</f>
@@ -5372,9 +5373,9 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="168" t="str">
+      <c r="A27" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L20</f>
-        <v>HKD_YC3MRH_QM3H12Y#0006</v>
+        <v>HKD_YC3MRH_QM3H12Y#0001</v>
       </c>
       <c r="B27" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A27,"Rate")</f>
@@ -5408,9 +5409,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="168" t="str">
+      <c r="A28" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L21</f>
-        <v>HKD_YC3MRH_QM3H13Y#0006</v>
+        <v>HKD_YC3MRH_QM3H13Y#0001</v>
       </c>
       <c r="B28" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A28,"Rate")</f>
@@ -5444,9 +5445,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="168" t="str">
+      <c r="A29" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L22</f>
-        <v>HKD_YC3MRH_QM3H14Y#0006</v>
+        <v>HKD_YC3MRH_QM3H14Y#0001</v>
       </c>
       <c r="B29" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A29,"Rate")</f>
@@ -5480,9 +5481,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="168" t="str">
+      <c r="A30" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L23</f>
-        <v>HKD_YC3MRH_QM3H15Y#0006</v>
+        <v>HKD_YC3MRH_QM3H15Y#0001</v>
       </c>
       <c r="B30" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A30,"Rate")</f>
@@ -5516,9 +5517,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="168" t="str">
+      <c r="A31" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L24</f>
-        <v>HKD_YC3MRH_QM3H16Y#0006</v>
+        <v>HKD_YC3MRH_QM3H16Y#0001</v>
       </c>
       <c r="B31" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A31,"Rate")</f>
@@ -5552,9 +5553,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="168" t="str">
+      <c r="A32" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L25</f>
-        <v>HKD_YC3MRH_QM3H17Y#0006</v>
+        <v>HKD_YC3MRH_QM3H17Y#0001</v>
       </c>
       <c r="B32" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A32,"Rate")</f>
@@ -5588,9 +5589,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="168" t="str">
+      <c r="A33" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L26</f>
-        <v>HKD_YC3MRH_QM3H18Y#0006</v>
+        <v>HKD_YC3MRH_QM3H18Y#0001</v>
       </c>
       <c r="B33" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A33,"Rate")</f>
@@ -5624,9 +5625,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="168" t="str">
+      <c r="A34" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L27</f>
-        <v>HKD_YC3MRH_QM3H19Y#0006</v>
+        <v>HKD_YC3MRH_QM3H19Y#0001</v>
       </c>
       <c r="B34" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A34,"Rate")</f>
@@ -5660,9 +5661,9 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="168" t="str">
+      <c r="A35" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L28</f>
-        <v>HKD_YC3MRH_QM3H20Y#0006</v>
+        <v>HKD_YC3MRH_QM3H20Y#0001</v>
       </c>
       <c r="B35" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A35,"Rate")</f>
@@ -5696,9 +5697,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="168" t="str">
+      <c r="A36" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L29</f>
-        <v>HKD_YC3MRH_QM3H21Y#0006</v>
+        <v>HKD_YC3MRH_QM3H21Y#0001</v>
       </c>
       <c r="B36" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A36,"Rate")</f>
@@ -5732,9 +5733,9 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="168" t="str">
+      <c r="A37" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L30</f>
-        <v>HKD_YC3MRH_QM3H22Y#0006</v>
+        <v>HKD_YC3MRH_QM3H22Y#0001</v>
       </c>
       <c r="B37" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A37,"Rate")</f>
@@ -5768,9 +5769,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="168" t="str">
+      <c r="A38" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L31</f>
-        <v>HKD_YC3MRH_QM3H23Y#0006</v>
+        <v>HKD_YC3MRH_QM3H23Y#0001</v>
       </c>
       <c r="B38" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A38,"Rate")</f>
@@ -5804,9 +5805,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="168" t="str">
+      <c r="A39" s="160" t="str">
         <f>HKD_YCRH_Swaps_3M!L32</f>
-        <v>HKD_YC3MRH_QM3H24Y#0006</v>
+        <v>HKD_YC3MRH_QM3H24Y#0001</v>
       </c>
       <c r="B39" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A39,"Rate")</f>
@@ -5840,7 +5841,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="168" t="e">
+      <c r="A40" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L33</f>
         <v>#NUM!</v>
       </c>
@@ -5876,7 +5877,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="168" t="e">
+      <c r="A41" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L34</f>
         <v>#NUM!</v>
       </c>
@@ -5912,7 +5913,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="168" t="e">
+      <c r="A42" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L35</f>
         <v>#NUM!</v>
       </c>
@@ -5948,7 +5949,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="168" t="e">
+      <c r="A43" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L36</f>
         <v>#NUM!</v>
       </c>
@@ -5984,7 +5985,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="168" t="e">
+      <c r="A44" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L37</f>
         <v>#NUM!</v>
       </c>
@@ -6020,7 +6021,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="168" t="e">
+      <c r="A45" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L38</f>
         <v>#NUM!</v>
       </c>
@@ -6056,7 +6057,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="168" t="e">
+      <c r="A46" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L39</f>
         <v>#NUM!</v>
       </c>
@@ -6092,7 +6093,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="168" t="e">
+      <c r="A47" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L40</f>
         <v>#NUM!</v>
       </c>
@@ -6128,7 +6129,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="168" t="e">
+      <c r="A48" s="160" t="e">
         <f>HKD_YCRH_Swaps_3M!L41</f>
         <v>#NUM!</v>
       </c>
@@ -6164,7 +6165,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="169" t="e">
+      <c r="A49" s="161" t="e">
         <f>HKD_YCRH_Swaps_3M!L42</f>
         <v>#NUM!</v>
       </c>
@@ -6443,7 +6444,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -6462,10 +6463,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="162" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="159"/>
+      <c r="B1" s="163"/>
       <c r="D1" s="151" t="s">
         <v>120</v>
       </c>
@@ -6480,7 +6481,7 @@
         <v>105</v>
       </c>
       <c r="I1" s="131">
-        <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
+        <f t="array" ref="I1:I50">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
         <v>1</v>
       </c>
     </row>
@@ -6495,7 +6496,7 @@
         <v>122</v>
       </c>
       <c r="D2" s="139" t="str">
-        <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
+        <f t="array" ref="D2:D50">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>HKD_YC3MRH_1x4F</v>
       </c>
       <c r="E2" s="138">
@@ -6653,8 +6654,8 @@
     </row>
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="142" t="str">
-        <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_RateHelpersSelected#0022</v>
+        <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D50),TRUE,,ObjectOverwrite)</f>
+        <v>HKD_YC3MRH_RateHelpersSelected#0008</v>
       </c>
       <c r="B7" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -7732,23 +7733,23 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D50" s="139" t="e">
+    <row r="50" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="135" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E50" s="138" t="e">
+      <c r="E50" s="134" t="e">
         <f>_xll.qlRateHelperRate($D50)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F50" s="138" t="str">
+      <c r="F50" s="134" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D50)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D50)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D50)),_xll.qlSwapRateHelperSpread($D50))</f>
         <v>--</v>
       </c>
-      <c r="G50" s="137" t="e">
+      <c r="G50" s="133" t="e">
         <f>_xll.qlRateHelperEarliestDate($D50)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H50" s="136" t="e">
+      <c r="H50" s="132" t="e">
         <f>_xll.qlRateHelperLatestDate($D50)</f>
         <v>#VALUE!</v>
       </c>
@@ -7757,1827 +7758,237 @@
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D51" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E51" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D51)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F51" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D51)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D51)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D51)),_xll.qlSwapRateHelperSpread($D51))</f>
-        <v>--</v>
-      </c>
-      <c r="G51" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D51)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H51" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D51)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I51" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I51" s="131"/>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D52" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E52" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D52)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F52" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D52)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D52)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D52)),_xll.qlSwapRateHelperSpread($D52))</f>
-        <v>--</v>
-      </c>
-      <c r="G52" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D52)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H52" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D52)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I52" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I52" s="131"/>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D53" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E53" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D53)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F53" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D53)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D53)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D53)),_xll.qlSwapRateHelperSpread($D53))</f>
-        <v>--</v>
-      </c>
-      <c r="G53" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D53)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H53" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D53)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I53" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="D53" s="170"/>
+      <c r="I53" s="131"/>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D54" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E54" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F54" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D54)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D54)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D54)),_xll.qlSwapRateHelperSpread($D54))</f>
-        <v>--</v>
-      </c>
-      <c r="G54" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H54" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I54" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I54" s="131"/>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D55" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E55" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D55)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F55" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D55)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D55)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D55)),_xll.qlSwapRateHelperSpread($D55))</f>
-        <v>--</v>
-      </c>
-      <c r="G55" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D55)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H55" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D55)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I55" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I55" s="131"/>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D56" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E56" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D56)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F56" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D56)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D56)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D56)),_xll.qlSwapRateHelperSpread($D56))</f>
-        <v>--</v>
-      </c>
-      <c r="G56" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D56)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H56" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D56)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I56" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I56" s="131"/>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D57" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E57" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D57)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F57" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D57)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D57)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D57)),_xll.qlSwapRateHelperSpread($D57))</f>
-        <v>--</v>
-      </c>
-      <c r="G57" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D57)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H57" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D57)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I57" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I57" s="131"/>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D58" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E58" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D58)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F58" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D58)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D58)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D58)),_xll.qlSwapRateHelperSpread($D58))</f>
-        <v>--</v>
-      </c>
-      <c r="G58" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D58)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H58" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D58)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I58" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I58" s="131"/>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D59" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E59" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D59)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F59" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D59)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D59)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D59)),_xll.qlSwapRateHelperSpread($D59))</f>
-        <v>--</v>
-      </c>
-      <c r="G59" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D59)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H59" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D59)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I59" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I59" s="131"/>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D60" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E60" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D60)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F60" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D60)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D60)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D60)),_xll.qlSwapRateHelperSpread($D60))</f>
-        <v>--</v>
-      </c>
-      <c r="G60" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D60)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H60" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D60)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I60" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I60" s="131"/>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D61" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E61" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D61)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F61" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D61)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D61)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D61)),_xll.qlSwapRateHelperSpread($D61))</f>
-        <v>--</v>
-      </c>
-      <c r="G61" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D61)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H61" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D61)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I61" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I61" s="131"/>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D62" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E62" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D62)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F62" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D62)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D62)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D62)),_xll.qlSwapRateHelperSpread($D62))</f>
-        <v>--</v>
-      </c>
-      <c r="G62" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D62)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H62" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D62)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I62" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I62" s="131"/>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D63" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E63" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D63)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F63" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D63)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D63)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D63)),_xll.qlSwapRateHelperSpread($D63))</f>
-        <v>--</v>
-      </c>
-      <c r="G63" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D63)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H63" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D63)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I63" s="131" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="I63" s="131"/>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D64" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E64" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D64)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F64" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D64)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D64)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D64)),_xll.qlSwapRateHelperSpread($D64))</f>
-        <v>--</v>
-      </c>
-      <c r="G64" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D64)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H64" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D64)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I64" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D65" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E65" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D65)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F65" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D65)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D65)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D65)),_xll.qlSwapRateHelperSpread($D65))</f>
-        <v>--</v>
-      </c>
-      <c r="G65" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D65)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H65" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D65)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I65" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D66" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E66" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D66)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F66" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D66)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D66)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D66)),_xll.qlSwapRateHelperSpread($D66))</f>
-        <v>--</v>
-      </c>
-      <c r="G66" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D66)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H66" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D66)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I66" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D67" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E67" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D67)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F67" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D67)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D67)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D67)),_xll.qlSwapRateHelperSpread($D67))</f>
-        <v>--</v>
-      </c>
-      <c r="G67" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D67)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H67" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D67)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I67" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D68" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E68" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D68)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F68" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D68)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D68)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D68)),_xll.qlSwapRateHelperSpread($D68))</f>
-        <v>--</v>
-      </c>
-      <c r="G68" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D68)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H68" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D68)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I68" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D69" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E69" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D69)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F69" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D69)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D69)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D69)),_xll.qlSwapRateHelperSpread($D69))</f>
-        <v>--</v>
-      </c>
-      <c r="G69" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D69)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H69" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D69)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I69" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D70" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E70" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D70)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F70" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D70)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D70)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D70)),_xll.qlSwapRateHelperSpread($D70))</f>
-        <v>--</v>
-      </c>
-      <c r="G70" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D70)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H70" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D70)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I70" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D71" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E71" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D71)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F71" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D71)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D71)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D71)),_xll.qlSwapRateHelperSpread($D71))</f>
-        <v>--</v>
-      </c>
-      <c r="G71" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D71)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H71" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D71)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I71" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D72" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E72" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F72" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D72)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D72)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D72)),_xll.qlSwapRateHelperSpread($D72))</f>
-        <v>--</v>
-      </c>
-      <c r="G72" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H72" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D72)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I72" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D73" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E73" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F73" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D73)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D73)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D73)),_xll.qlSwapRateHelperSpread($D73))</f>
-        <v>--</v>
-      </c>
-      <c r="G73" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H73" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D73)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I73" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D74" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E74" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F74" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D74)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D74)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D74)),_xll.qlSwapRateHelperSpread($D74))</f>
-        <v>--</v>
-      </c>
-      <c r="G74" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H74" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D74)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I74" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D75" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E75" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F75" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D75)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D75)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D75)),_xll.qlSwapRateHelperSpread($D75))</f>
-        <v>--</v>
-      </c>
-      <c r="G75" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H75" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D75)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I75" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D76" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E76" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D76)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F76" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D76)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D76)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D76)),_xll.qlSwapRateHelperSpread($D76))</f>
-        <v>--</v>
-      </c>
-      <c r="G76" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D76)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H76" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D76)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I76" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D77" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E77" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D77)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F77" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D77)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D77)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D77)),_xll.qlSwapRateHelperSpread($D77))</f>
-        <v>--</v>
-      </c>
-      <c r="G77" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D77)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H77" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D77)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I77" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D78" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E78" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D78)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F78" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D78)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D78)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D78)),_xll.qlSwapRateHelperSpread($D78))</f>
-        <v>--</v>
-      </c>
-      <c r="G78" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D78)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H78" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D78)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I78" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D79" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E79" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D79)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F79" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D79)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D79)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D79)),_xll.qlSwapRateHelperSpread($D79))</f>
-        <v>--</v>
-      </c>
-      <c r="G79" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D79)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H79" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D79)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I79" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D80" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E80" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D80)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F80" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D80)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D80)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D80)),_xll.qlSwapRateHelperSpread($D80))</f>
-        <v>--</v>
-      </c>
-      <c r="G80" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D80)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H80" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D80)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I80" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D81" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E81" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D81)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F81" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D81)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D81)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D81)),_xll.qlSwapRateHelperSpread($D81))</f>
-        <v>--</v>
-      </c>
-      <c r="G81" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D81)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H81" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D81)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I81" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D82" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E82" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D82)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F82" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D82)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D82)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D82)),_xll.qlSwapRateHelperSpread($D82))</f>
-        <v>--</v>
-      </c>
-      <c r="G82" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D82)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H82" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D82)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I82" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D83" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E83" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D83)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F83" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D83)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D83)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D83)),_xll.qlSwapRateHelperSpread($D83))</f>
-        <v>--</v>
-      </c>
-      <c r="G83" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D83)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H83" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D83)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I83" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D84" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E84" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D84)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F84" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D84)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D84)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D84)),_xll.qlSwapRateHelperSpread($D84))</f>
-        <v>--</v>
-      </c>
-      <c r="G84" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D84)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H84" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D84)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I84" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D85" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E85" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D85)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F85" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D85)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D85)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D85)),_xll.qlSwapRateHelperSpread($D85))</f>
-        <v>--</v>
-      </c>
-      <c r="G85" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D85)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H85" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D85)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I85" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D86" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E86" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D86)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F86" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D86)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D86)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D86)),_xll.qlSwapRateHelperSpread($D86))</f>
-        <v>--</v>
-      </c>
-      <c r="G86" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D86)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H86" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D86)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I86" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D87" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E87" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D87)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F87" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D87)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D87)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D87)),_xll.qlSwapRateHelperSpread($D87))</f>
-        <v>--</v>
-      </c>
-      <c r="G87" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D87)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H87" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D87)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I87" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D88" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E88" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D88)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F88" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D88)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D88)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D88)),_xll.qlSwapRateHelperSpread($D88))</f>
-        <v>--</v>
-      </c>
-      <c r="G88" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D88)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H88" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D88)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I88" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D89" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E89" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D89)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F89" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D89)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D89)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D89)),_xll.qlSwapRateHelperSpread($D89))</f>
-        <v>--</v>
-      </c>
-      <c r="G89" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D89)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H89" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D89)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I89" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D90" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E90" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D90)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F90" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D90)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D90)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D90)),_xll.qlSwapRateHelperSpread($D90))</f>
-        <v>--</v>
-      </c>
-      <c r="G90" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D90)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H90" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D90)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I90" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D91" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E91" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D91)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F91" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D91)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D91)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D91)),_xll.qlSwapRateHelperSpread($D91))</f>
-        <v>--</v>
-      </c>
-      <c r="G91" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D91)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H91" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D91)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I91" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D92" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E92" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D92)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F92" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D92)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D92)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D92)),_xll.qlSwapRateHelperSpread($D92))</f>
-        <v>--</v>
-      </c>
-      <c r="G92" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D92)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H92" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D92)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I92" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D93" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E93" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D93)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F93" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D93)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D93)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D93)),_xll.qlSwapRateHelperSpread($D93))</f>
-        <v>--</v>
-      </c>
-      <c r="G93" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D93)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H93" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D93)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I93" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D94" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E94" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D94)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F94" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D94)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D94)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D94)),_xll.qlSwapRateHelperSpread($D94))</f>
-        <v>--</v>
-      </c>
-      <c r="G94" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D94)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H94" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D94)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I94" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D95" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E95" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D95)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F95" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D95)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D95)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D95)),_xll.qlSwapRateHelperSpread($D95))</f>
-        <v>--</v>
-      </c>
-      <c r="G95" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D95)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H95" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D95)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I95" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D96" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E96" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F96" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D96)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D96)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D96)),_xll.qlSwapRateHelperSpread($D96))</f>
-        <v>--</v>
-      </c>
-      <c r="G96" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H96" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I96" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="97" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D97" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E97" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D97)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F97" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D97)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D97)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D97)),_xll.qlSwapRateHelperSpread($D97))</f>
-        <v>--</v>
-      </c>
-      <c r="G97" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D97)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H97" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D97)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I97" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="98" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D98" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E98" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D98)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F98" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D98)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D98)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D98)),_xll.qlSwapRateHelperSpread($D98))</f>
-        <v>--</v>
-      </c>
-      <c r="G98" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D98)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H98" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D98)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I98" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="99" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D99" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E99" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D99)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F99" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D99)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D99)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D99)),_xll.qlSwapRateHelperSpread($D99))</f>
-        <v>--</v>
-      </c>
-      <c r="G99" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D99)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H99" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D99)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I99" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="100" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D100" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E100" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D100)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F100" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D100)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D100)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D100)),_xll.qlSwapRateHelperSpread($D100))</f>
-        <v>--</v>
-      </c>
-      <c r="G100" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D100)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H100" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D100)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I100" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="101" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D101" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E101" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D101)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F101" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D101)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D101)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D101)),_xll.qlSwapRateHelperSpread($D101))</f>
-        <v>--</v>
-      </c>
-      <c r="G101" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D101)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H101" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D101)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I101" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="102" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D102" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E102" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D102)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F102" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D102)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D102)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D102)),_xll.qlSwapRateHelperSpread($D102))</f>
-        <v>--</v>
-      </c>
-      <c r="G102" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D102)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H102" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D102)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I102" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="103" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D103" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E103" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D103)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F103" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D103)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D103)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D103)),_xll.qlSwapRateHelperSpread($D103))</f>
-        <v>--</v>
-      </c>
-      <c r="G103" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D103)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H103" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D103)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I103" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="104" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D104" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E104" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F104" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D104)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D104)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D104)),_xll.qlSwapRateHelperSpread($D104))</f>
-        <v>--</v>
-      </c>
-      <c r="G104" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H104" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D104)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I104" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="105" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D105" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E105" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D105)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F105" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D105)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D105)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D105)),_xll.qlSwapRateHelperSpread($D105))</f>
-        <v>--</v>
-      </c>
-      <c r="G105" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D105)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H105" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D105)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I105" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="106" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D106" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E106" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D106)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F106" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D106)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D106)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D106)),_xll.qlSwapRateHelperSpread($D106))</f>
-        <v>--</v>
-      </c>
-      <c r="G106" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D106)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H106" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D106)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I106" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="107" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D107" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E107" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F107" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D107)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D107)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D107)),_xll.qlSwapRateHelperSpread($D107))</f>
-        <v>--</v>
-      </c>
-      <c r="G107" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H107" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D107)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I107" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="108" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D108" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E108" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D108)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F108" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D108)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D108)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D108)),_xll.qlSwapRateHelperSpread($D108))</f>
-        <v>--</v>
-      </c>
-      <c r="G108" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D108)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H108" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D108)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I108" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="109" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D109" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E109" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D109)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F109" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D109)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D109)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D109)),_xll.qlSwapRateHelperSpread($D109))</f>
-        <v>--</v>
-      </c>
-      <c r="G109" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D109)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H109" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D109)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I109" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="110" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D110" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E110" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D110)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F110" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D110)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D110)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D110)),_xll.qlSwapRateHelperSpread($D110))</f>
-        <v>--</v>
-      </c>
-      <c r="G110" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D110)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H110" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D110)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I110" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="111" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D111" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E111" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F111" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D111)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D111)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D111)),_xll.qlSwapRateHelperSpread($D111))</f>
-        <v>--</v>
-      </c>
-      <c r="G111" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H111" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D111)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I111" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="112" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D112" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E112" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D112)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F112" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D112)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D112)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D112)),_xll.qlSwapRateHelperSpread($D112))</f>
-        <v>--</v>
-      </c>
-      <c r="G112" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D112)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H112" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D112)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I112" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D113" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E113" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D113)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F113" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D113)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D113)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D113)),_xll.qlSwapRateHelperSpread($D113))</f>
-        <v>--</v>
-      </c>
-      <c r="G113" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D113)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H113" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D113)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I113" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="114" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D114" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E114" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D114)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F114" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D114)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D114)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D114)),_xll.qlSwapRateHelperSpread($D114))</f>
-        <v>--</v>
-      </c>
-      <c r="G114" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D114)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H114" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D114)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I114" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D115" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E115" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D115)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F115" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D115)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D115)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D115)),_xll.qlSwapRateHelperSpread($D115))</f>
-        <v>--</v>
-      </c>
-      <c r="G115" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D115)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H115" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D115)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I115" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="116" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D116" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E116" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D116)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F116" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D116)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D116)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D116)),_xll.qlSwapRateHelperSpread($D116))</f>
-        <v>--</v>
-      </c>
-      <c r="G116" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D116)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H116" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D116)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I116" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D117" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E117" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D117)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F117" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D117)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D117)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D117)),_xll.qlSwapRateHelperSpread($D117))</f>
-        <v>--</v>
-      </c>
-      <c r="G117" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D117)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H117" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D117)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I117" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D118" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E118" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D118)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F118" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D118)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D118)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D118)),_xll.qlSwapRateHelperSpread($D118))</f>
-        <v>--</v>
-      </c>
-      <c r="G118" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D118)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H118" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D118)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I118" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D119" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E119" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D119)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F119" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D119)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D119)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D119)),_xll.qlSwapRateHelperSpread($D119))</f>
-        <v>--</v>
-      </c>
-      <c r="G119" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D119)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H119" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D119)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I119" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D120" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E120" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D120)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F120" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D120)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D120)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D120)),_xll.qlSwapRateHelperSpread($D120))</f>
-        <v>--</v>
-      </c>
-      <c r="G120" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D120)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H120" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D120)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I120" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D121" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E121" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D121)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F121" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D121)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D121)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D121)),_xll.qlSwapRateHelperSpread($D121))</f>
-        <v>--</v>
-      </c>
-      <c r="G121" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D121)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H121" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D121)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I121" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D122" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E122" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D122)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F122" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D122)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D122)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D122)),_xll.qlSwapRateHelperSpread($D122))</f>
-        <v>--</v>
-      </c>
-      <c r="G122" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D122)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H122" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D122)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I122" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D123" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E123" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D123)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F123" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D123)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D123)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D123)),_xll.qlSwapRateHelperSpread($D123))</f>
-        <v>--</v>
-      </c>
-      <c r="G123" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D123)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H123" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D123)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I123" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D124" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E124" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D124)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F124" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D124)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D124)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D124)),_xll.qlSwapRateHelperSpread($D124))</f>
-        <v>--</v>
-      </c>
-      <c r="G124" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D124)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H124" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D124)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I124" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D125" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E125" s="138" t="e">
-        <f>_xll.qlRateHelperRate($D125)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F125" s="138" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D125)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D125)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D125)),_xll.qlSwapRateHelperSpread($D125))</f>
-        <v>--</v>
-      </c>
-      <c r="G125" s="137" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D125)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H125" s="136" t="e">
-        <f>_xll.qlRateHelperLatestDate($D125)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I125" s="131" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D126" s="135" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E126" s="134" t="e">
-        <f>_xll.qlRateHelperRate($D126)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F126" s="134" t="str">
-        <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D126)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D126)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D126)),_xll.qlSwapRateHelperSpread($D126))</f>
-        <v>--</v>
-      </c>
-      <c r="G126" s="133" t="e">
-        <f>_xll.qlRateHelperEarliestDate($D126)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H126" s="132" t="e">
-        <f>_xll.qlRateHelperLatestDate($D126)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I126" s="131" t="e">
-        <v>#N/A</v>
+      <c r="I64" s="131"/>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I65" s="131"/>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I66" s="131"/>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I67" s="131"/>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I68" s="131"/>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I69" s="131"/>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I70" s="131"/>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I71" s="131"/>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I72" s="131"/>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I73" s="131"/>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I74" s="131"/>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I75" s="131"/>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I76" s="131"/>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I77" s="131"/>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I78" s="131"/>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I79" s="131"/>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I80" s="131"/>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I81" s="131"/>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I82" s="131"/>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I83" s="131"/>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I84" s="131"/>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I85" s="131"/>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I86" s="131"/>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I87" s="131"/>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I88" s="131"/>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I89" s="131"/>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I90" s="131"/>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I91" s="131"/>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I92" s="131"/>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I93" s="131"/>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I94" s="131"/>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I95" s="131"/>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I96" s="131"/>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I97" s="131"/>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I98" s="131"/>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I99" s="131"/>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I100" s="131"/>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I101" s="131"/>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I102" s="131"/>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I103" s="131"/>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I104" s="131"/>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I105" s="131"/>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I106" s="131"/>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I107" s="131"/>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I108" s="131"/>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I109" s="131"/>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I110" s="131"/>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I111" s="131"/>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I112" s="131"/>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I113" s="131"/>
+    </row>
+    <row r="114" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I114" s="131"/>
+    </row>
+    <row r="115" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I115" s="131"/>
+    </row>
+    <row r="116" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I116" s="131"/>
+    </row>
+    <row r="117" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I117" s="131"/>
+    </row>
+    <row r="118" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I118" s="131"/>
+    </row>
+    <row r="119" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I119" s="131"/>
+    </row>
+    <row r="120" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I120" s="131"/>
+    </row>
+    <row r="121" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I121" s="131"/>
+    </row>
+    <row r="122" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I122" s="131"/>
+    </row>
+    <row r="123" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I123" s="131"/>
+    </row>
+    <row r="124" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I124" s="131"/>
+    </row>
+    <row r="125" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I125" s="131"/>
+    </row>
+    <row r="126" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I126" s="131"/>
+    </row>
+    <row r="129" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I129" s="171" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -9601,9 +8012,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AE73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9625,19 +8034,19 @@
       </c>
     </row>
     <row r="2" spans="1:31" s="76" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="162"/>
-      <c r="H2" s="163" t="s">
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="166"/>
+      <c r="H2" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="165"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
+      <c r="K2" s="169"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="76"/>
@@ -9688,7 +8097,9 @@
       <c r="I4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="8">
+        <v>41598.597199074073</v>
+      </c>
       <c r="K4" s="13"/>
       <c r="L4" s="76"/>
       <c r="M4" s="76"/>
@@ -9923,7 +8334,7 @@
       </c>
       <c r="D10" s="106" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC3M#0022</v>
+        <v>_HKDYC3M#0003</v>
       </c>
       <c r="E10" s="81"/>
       <c r="F10" s="80"/>
@@ -10006,12 +8417,12 @@
       <c r="E12" s="81"/>
       <c r="F12" s="80"/>
       <c r="G12" s="76"/>
-      <c r="H12" s="163" t="s">
+      <c r="H12" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="164"/>
-      <c r="J12" s="164"/>
-      <c r="K12" s="165"/>
+      <c r="I12" s="168"/>
+      <c r="J12" s="168"/>
+      <c r="K12" s="169"/>
       <c r="L12" s="76"/>
       <c r="M12" s="76"/>
       <c r="N12" s="76"/>
@@ -10485,7 +8896,7 @@
       <c r="A24" s="76"/>
       <c r="B24" s="84"/>
       <c r="C24" s="86">
-        <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
+        <f>MAX(_xll.ohPack(Selected!H2:H50))</f>
         <v>47077</v>
       </c>
       <c r="D24" s="85">

</xml_diff>

<commit_message>
delete 3M swaps past 24 months
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
@@ -31,7 +31,7 @@
     <definedName name="IborType">'General Settings'!$D$6</definedName>
     <definedName name="IndexTenor">'General Settings'!$D$5</definedName>
     <definedName name="InterpolatorID">'General Settings'!$D$21</definedName>
-    <definedName name="MinDistance">RateHelpers!$G$2:$G$49</definedName>
+    <definedName name="MinDistance">RateHelpers!$G$2:$G$39</definedName>
     <definedName name="MoneyMarketDayCounter">'General Settings'!$J$18</definedName>
     <definedName name="Months">'General Settings'!$D$4</definedName>
     <definedName name="NDays">'General Settings'!$D$13</definedName>
@@ -43,9 +43,9 @@
     <definedName name="RateHelperPrefix" localSheetId="4">'General Settings'!$D$8</definedName>
     <definedName name="RateHelperPrefix" localSheetId="2">'General Settings'!$D$8</definedName>
     <definedName name="RateHelperPrefix" localSheetId="3">'General Settings'!$D$8</definedName>
-    <definedName name="RateHelpers">RateHelpers!$A$2:$A$49</definedName>
-    <definedName name="RateHelpersIncluded">RateHelpers!$E$2:$E$49</definedName>
-    <definedName name="RateHelpersPriority">RateHelpers!$F$2:$F$49</definedName>
+    <definedName name="RateHelpers">RateHelpers!$A$2:$A$39</definedName>
+    <definedName name="RateHelpersIncluded">RateHelpers!$E$2:$E$39</definedName>
+    <definedName name="RateHelpersPriority">RateHelpers!$F$2:$F$39</definedName>
     <definedName name="RateHelpersSelected">Selected!$A$7</definedName>
     <definedName name="SerializationPath">'General Settings'!$J$8</definedName>
     <definedName name="Serialize">'General Settings'!$J$7</definedName>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="133">
   <si>
     <t>_Quote</t>
   </si>
@@ -291,36 +291,6 @@
   </si>
   <si>
     <t>Quarterly</t>
-  </si>
-  <si>
-    <t>60Y</t>
-  </si>
-  <si>
-    <t>50Y</t>
-  </si>
-  <si>
-    <t>40Y</t>
-  </si>
-  <si>
-    <t>35Y</t>
-  </si>
-  <si>
-    <t>30Y</t>
-  </si>
-  <si>
-    <t>29Y</t>
-  </si>
-  <si>
-    <t>28Y</t>
-  </si>
-  <si>
-    <t>27Y</t>
-  </si>
-  <si>
-    <t>26Y</t>
-  </si>
-  <si>
-    <t>25Y</t>
   </si>
   <si>
     <t>24Y</t>
@@ -1297,7 +1267,7 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
@@ -1654,6 +1624,10 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1676,10 +1650,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="3"/>
@@ -1997,7 +1973,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="3" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="19" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="19" bestFit="1" customWidth="1"/>
@@ -2006,13 +1982,13 @@
     <col min="7" max="7" width="19.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.28515625" style="19" customWidth="1"/>
-    <col min="10" max="10" width="3" style="19" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="19" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="153" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -2082,7 +2058,7 @@
       </c>
       <c r="H3" s="37" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_T3F1#0001</v>
+        <v>HKD_YC3MRH_T3F1#0000</v>
       </c>
       <c r="I3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -2116,7 +2092,7 @@
       </c>
       <c r="H4" s="27" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_TOM3F1#0001</v>
+        <v>HKD_YC3MRH_TOM3F1#0000</v>
       </c>
       <c r="I4" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -2151,7 +2127,7 @@
       </c>
       <c r="H5" s="32" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0001</v>
+        <v>HKD_YC3MRH_1x4F#0000</v>
       </c>
       <c r="I5" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -2186,7 +2162,7 @@
       </c>
       <c r="H6" s="32" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0001</v>
+        <v>HKD_YC3MRH_2x5F#0000</v>
       </c>
       <c r="I6" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -2221,7 +2197,7 @@
       </c>
       <c r="H7" s="32" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0001</v>
+        <v>HKD_YC3MRH_3x6F#0000</v>
       </c>
       <c r="I7" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -2256,7 +2232,7 @@
       </c>
       <c r="H8" s="32" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0001</v>
+        <v>HKD_YC3MRH_4x7F#0000</v>
       </c>
       <c r="I8" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -2291,7 +2267,7 @@
       </c>
       <c r="H9" s="32" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0001</v>
+        <v>HKD_YC3MRH_5x8F#0000</v>
       </c>
       <c r="I9" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -2326,7 +2302,7 @@
       </c>
       <c r="H10" s="32" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0001</v>
+        <v>HKD_YC3MRH_6x9F#0000</v>
       </c>
       <c r="I10" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -2361,7 +2337,7 @@
       </c>
       <c r="H11" s="32" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0001</v>
+        <v>HKD_YC3MRH_7x10F#0000</v>
       </c>
       <c r="I11" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -2396,7 +2372,7 @@
       </c>
       <c r="H12" s="32" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0001</v>
+        <v>HKD_YC3MRH_8x11F#0000</v>
       </c>
       <c r="I12" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -2431,7 +2407,7 @@
       </c>
       <c r="H13" s="27" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0001</v>
+        <v>HKD_YC3MRH_9x12F#0000</v>
       </c>
       <c r="I13" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -2464,13 +2440,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="19" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="19" bestFit="1" customWidth="1"/>
@@ -2480,14 +2456,14 @@
     <col min="8" max="8" width="15.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="19" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" style="19" customWidth="1"/>
-    <col min="15" max="15" width="2.5703125" style="19" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="19"/>
-    <col min="17" max="17" width="19.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="19"/>
+    <col min="14" max="15" width="2.7109375" style="19" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="9.140625" style="19"/>
   </cols>
@@ -2519,7 +2495,7 @@
       <c r="H2" s="53"/>
       <c r="I2" s="53"/>
       <c r="J2" s="73" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="K2" s="73" t="str">
         <f>Currency&amp;"_YC"&amp;$J$2&amp;"RH"</f>
@@ -2535,22 +2511,22 @@
     <row r="3" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30"/>
       <c r="B3" s="43" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
       <c r="E3" s="43"/>
       <c r="F3" s="43" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G3" s="43" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I3" s="43" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="J3" s="43" t="s">
         <v>17</v>
@@ -2559,31 +2535,31 @@
         <f>K2&amp;"_Swaps.xml"</f>
         <v>HKD_YC3MRH_Swaps.xml</v>
       </c>
-      <c r="L3" s="41" t="e">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(L4:L42,SerializationPath&amp;K3,FileOverwrite,,Serialize),"---")</f>
-        <v>#NUM!</v>
+      <c r="L3" s="41">
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(L4:L32,SerializationPath&amp;K3,FileOverwrite,,Serialize),"---")</f>
+        <v>28</v>
       </c>
       <c r="M3" s="56" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L3)</f>
-        <v>ohObjectSave - operToVectorImpl: error converting parameter 'ObjectList' to type 'class std::basic_string&lt;char,struct std::char_traits&lt;char&gt;,class std::allocator&lt;char&gt; &gt;' : Unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'class s</v>
+        <v/>
       </c>
       <c r="N3" s="157" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="P3" s="71" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="Q3" s="71" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="R3" s="71" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S3" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" s="71" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="T3" s="172" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -2610,7 +2586,7 @@
         <v/>
       </c>
       <c r="N4" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="P4" s="67">
         <v>0</v>
@@ -2619,12 +2595,12 @@
         <v>21</v>
       </c>
       <c r="R4" s="67" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="S4" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="T4" s="67" t="s">
+      <c r="T4" s="173" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2643,7 +2619,7 @@
       <c r="L5" s="53"/>
       <c r="M5" s="53"/>
       <c r="N5" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -2652,13 +2628,13 @@
         <v>16</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F6" s="61" t="s">
         <v>27</v>
@@ -2667,18 +2643,18 @@
         <v>26</v>
       </c>
       <c r="H6" s="64" t="str">
-        <f t="shared" ref="H6:H42" si="0">IF(UPPER(RIGHT($D6))="B",BondBasisDayCounter,IF(UPPER(RIGHT($D6))="M",MoneyMarketDayCounter,"--"))</f>
+        <f t="shared" ref="H6:H32" si="0">IF(UPPER(RIGHT($D6))="B",BondBasisDayCounter,IF(UPPER(RIGHT($D6))="M",MoneyMarketDayCounter,"--"))</f>
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="I6" s="59">
         <v>0</v>
       </c>
       <c r="J6" s="63" t="str">
-        <f t="shared" ref="J6:J42" si="1">Currency&amp;$D6&amp;$E6&amp;$C6&amp;"_Quote"</f>
+        <f t="shared" ref="J6:J32" si="1">Currency&amp;$D6&amp;$E6&amp;$C6&amp;"_Quote"</f>
         <v>HKDQM3H1Y_Quote</v>
       </c>
       <c r="K6" s="58" t="str">
-        <f t="shared" ref="K6:K42" si="2">$K$2&amp;"_"&amp;$D6&amp;$E6&amp;$C6</f>
+        <f t="shared" ref="K6:K32" si="2">$K$2&amp;"_"&amp;$D6&amp;$E6&amp;$C6</f>
         <v>HKD_YC3MRH_QM3H1Y</v>
       </c>
       <c r="L6" s="57" t="str">
@@ -2690,7 +2666,7 @@
         <v/>
       </c>
       <c r="N6" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -2699,13 +2675,13 @@
         <v>16</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F7" s="61" t="s">
         <v>27</v>
@@ -2737,7 +2713,7 @@
         <v/>
       </c>
       <c r="N7" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -2746,13 +2722,13 @@
         <v>16</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F8" s="61" t="s">
         <v>27</v>
@@ -2784,7 +2760,7 @@
         <v/>
       </c>
       <c r="N8" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -2793,13 +2769,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F9" s="61" t="s">
         <v>27</v>
@@ -2831,7 +2807,7 @@
         <v/>
       </c>
       <c r="N9" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -2840,13 +2816,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F10" s="61" t="s">
         <v>27</v>
@@ -2878,7 +2854,7 @@
         <v/>
       </c>
       <c r="N10" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -2887,13 +2863,13 @@
         <v>16</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>27</v>
@@ -2925,7 +2901,7 @@
         <v/>
       </c>
       <c r="N11" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -2934,13 +2910,13 @@
         <v>16</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D12" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F12" s="61" t="s">
         <v>27</v>
@@ -2972,7 +2948,7 @@
         <v/>
       </c>
       <c r="N12" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -2981,13 +2957,13 @@
         <v>16</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F13" s="61" t="s">
         <v>27</v>
@@ -3019,7 +2995,7 @@
         <v/>
       </c>
       <c r="N13" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -3028,13 +3004,13 @@
         <v>16</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F14" s="61" t="s">
         <v>27</v>
@@ -3066,7 +3042,7 @@
         <v/>
       </c>
       <c r="N14" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -3075,13 +3051,13 @@
         <v>16</v>
       </c>
       <c r="C15" s="62" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F15" s="61" t="s">
         <v>27</v>
@@ -3113,7 +3089,7 @@
         <v/>
       </c>
       <c r="N15" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -3122,13 +3098,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="62" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F16" s="61" t="s">
         <v>27</v>
@@ -3160,7 +3136,7 @@
         <v/>
       </c>
       <c r="N16" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -3169,13 +3145,13 @@
         <v>16</v>
       </c>
       <c r="C17" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="61" t="s">
-        <v>63</v>
-      </c>
       <c r="E17" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F17" s="61" t="s">
         <v>27</v>
@@ -3207,7 +3183,7 @@
         <v/>
       </c>
       <c r="N17" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -3216,13 +3192,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="61" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="61" t="s">
-        <v>62</v>
       </c>
       <c r="F18" s="61" t="s">
         <v>27</v>
@@ -3254,7 +3230,7 @@
         <v/>
       </c>
       <c r="N18" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -3263,13 +3239,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F19" s="61" t="s">
         <v>27</v>
@@ -3301,7 +3277,7 @@
         <v/>
       </c>
       <c r="N19" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -3310,13 +3286,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="62" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E20" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F20" s="61" t="s">
         <v>27</v>
@@ -3348,7 +3324,7 @@
         <v/>
       </c>
       <c r="N20" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -3357,13 +3333,13 @@
         <v>16</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F21" s="61" t="s">
         <v>27</v>
@@ -3395,7 +3371,7 @@
         <v/>
       </c>
       <c r="N21" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -3404,13 +3380,13 @@
         <v>16</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E22" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F22" s="61" t="s">
         <v>27</v>
@@ -3442,7 +3418,7 @@
         <v/>
       </c>
       <c r="N22" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -3451,13 +3427,13 @@
         <v>16</v>
       </c>
       <c r="C23" s="62" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E23" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F23" s="61" t="s">
         <v>27</v>
@@ -3489,7 +3465,7 @@
         <v/>
       </c>
       <c r="N23" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -3498,13 +3474,13 @@
         <v>16</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E24" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F24" s="61" t="s">
         <v>27</v>
@@ -3536,7 +3512,7 @@
         <v/>
       </c>
       <c r="N24" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -3545,13 +3521,13 @@
         <v>16</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D25" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E25" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F25" s="61" t="s">
         <v>27</v>
@@ -3583,7 +3559,7 @@
         <v/>
       </c>
       <c r="N25" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -3592,13 +3568,13 @@
         <v>16</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E26" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F26" s="61" t="s">
         <v>27</v>
@@ -3630,7 +3606,7 @@
         <v/>
       </c>
       <c r="N26" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -3639,13 +3615,13 @@
         <v>16</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E27" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F27" s="61" t="s">
         <v>27</v>
@@ -3677,7 +3653,7 @@
         <v/>
       </c>
       <c r="N27" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -3686,13 +3662,13 @@
         <v>16</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D28" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E28" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F28" s="61" t="s">
         <v>27</v>
@@ -3724,7 +3700,7 @@
         <v/>
       </c>
       <c r="N28" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -3733,13 +3709,13 @@
         <v>16</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D29" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E29" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F29" s="61" t="s">
         <v>27</v>
@@ -3771,7 +3747,7 @@
         <v/>
       </c>
       <c r="N29" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -3780,13 +3756,13 @@
         <v>16</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E30" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F30" s="61" t="s">
         <v>27</v>
@@ -3818,7 +3794,7 @@
         <v/>
       </c>
       <c r="N30" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -3827,13 +3803,13 @@
         <v>16</v>
       </c>
       <c r="C31" s="62" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D31" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E31" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F31" s="61" t="s">
         <v>27</v>
@@ -3865,7 +3841,7 @@
         <v/>
       </c>
       <c r="N31" s="55" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -3874,13 +3850,13 @@
         <v>16</v>
       </c>
       <c r="C32" s="62" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D32" s="61" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E32" s="61" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F32" s="61" t="s">
         <v>27</v>
@@ -3912,495 +3888,25 @@
         <v/>
       </c>
       <c r="N32" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H33" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I33" s="59">
-        <v>0</v>
-      </c>
-      <c r="J33" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H25Y_Quote</v>
-      </c>
-      <c r="K33" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H25Y</v>
-      </c>
-      <c r="L33" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M33" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L33)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H25Y_Quote'</v>
-      </c>
-      <c r="N33" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="B34" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G34" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I34" s="59">
-        <v>0</v>
-      </c>
-      <c r="J34" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H26Y_Quote</v>
-      </c>
-      <c r="K34" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H26Y</v>
-      </c>
-      <c r="L34" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M34" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L34)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H26Y_Quote'</v>
-      </c>
-      <c r="N34" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I35" s="59">
-        <v>0</v>
-      </c>
-      <c r="J35" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H27Y_Quote</v>
-      </c>
-      <c r="K35" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H27Y</v>
-      </c>
-      <c r="L35" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M35" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L35)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H27Y_Quote'</v>
-      </c>
-      <c r="N35" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I36" s="59">
-        <v>0</v>
-      </c>
-      <c r="J36" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H28Y_Quote</v>
-      </c>
-      <c r="K36" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H28Y</v>
-      </c>
-      <c r="L36" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M36" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L36)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H28Y_Quote'</v>
-      </c>
-      <c r="N36" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I37" s="59">
-        <v>0</v>
-      </c>
-      <c r="J37" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H29Y_Quote</v>
-      </c>
-      <c r="K37" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H29Y</v>
-      </c>
-      <c r="L37" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M37" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L37)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H29Y_Quote'</v>
-      </c>
-      <c r="N37" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="B38" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I38" s="59">
-        <v>0</v>
-      </c>
-      <c r="J38" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H30Y_Quote</v>
-      </c>
-      <c r="K38" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H30Y</v>
-      </c>
-      <c r="L38" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M38" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L38)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H30Y_Quote'</v>
-      </c>
-      <c r="N38" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
-      <c r="B39" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G39" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H39" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I39" s="59">
-        <v>0</v>
-      </c>
-      <c r="J39" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H35Y_Quote</v>
-      </c>
-      <c r="K39" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H35Y</v>
-      </c>
-      <c r="L39" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M39" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L39)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H35Y_Quote'</v>
-      </c>
-      <c r="N39" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="30"/>
-      <c r="B40" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H40" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I40" s="59">
-        <v>0</v>
-      </c>
-      <c r="J40" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H40Y_Quote</v>
-      </c>
-      <c r="K40" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H40Y</v>
-      </c>
-      <c r="L40" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M40" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L40)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H40Y_Quote'</v>
-      </c>
-      <c r="N40" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H41" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I41" s="59">
-        <v>0</v>
-      </c>
-      <c r="J41" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H50Y_Quote</v>
-      </c>
-      <c r="K41" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H50Y</v>
-      </c>
-      <c r="L41" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M41" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L41)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H50Y_Quote'</v>
-      </c>
-      <c r="N41" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="H42" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v>Actual/365 (Fixed)</v>
-      </c>
-      <c r="I42" s="59">
-        <v>0</v>
-      </c>
-      <c r="J42" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>HKDQM3H60Y_Quote</v>
-      </c>
-      <c r="K42" s="58" t="str">
-        <f t="shared" si="2"/>
-        <v>HKD_YC3MRH_QM3H60Y</v>
-      </c>
-      <c r="L42" s="57" t="e">
-        <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M42" s="56" t="str">
-        <f ca="1">_xll.ohRangeRetrieveError(L42)</f>
-        <v>qlSwapRateHelper2 - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'HKDQM3H60Y_Quote'</v>
-      </c>
-      <c r="N42" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="54"/>
-      <c r="O43" s="53"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="53"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -4410,10 +3916,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F32">
       <formula1>"Annual,Semiannual,EveryFourthMonth,Quarterly,Bimonthly,Monthly,Biweekly,Weekly,Daily,Once,NoFrequency"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G32">
       <formula1>"Following,Modified Following,Preceding,Modified Preceding,Month End Reference,Unadjusted Month End,Unadjusted"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4426,7 +3932,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4447,37 +3953,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="158" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B1" s="158" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C1" s="158" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D1" s="158" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E1" s="158" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F1" s="158" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G1" s="158" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="H1" s="158" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I1" s="158" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="159" t="str">
         <f>HKD_YCRH_FRAs_3M!H3</f>
-        <v>HKD_YC3MRH_T3F1#0001</v>
+        <v>HKD_YC3MRH_T3F1#0000</v>
       </c>
       <c r="B2" s="128" t="str">
         <f>_xll.ohObjectPropertyValues(A2,"Rate")</f>
@@ -4509,13 +4015,13 @@
         <v>10</v>
       </c>
       <c r="K2" s="111" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H4</f>
-        <v>HKD_YC3MRH_TOM3F1#0001</v>
+        <v>HKD_YC3MRH_TOM3F1#0000</v>
       </c>
       <c r="B3" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A3,"Rate")</f>
@@ -4547,13 +4053,13 @@
         <v>20</v>
       </c>
       <c r="K3" s="111" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H5</f>
-        <v>HKD_YC3MRH_1x4F#0001</v>
+        <v>HKD_YC3MRH_1x4F#0000</v>
       </c>
       <c r="B4" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A4,"Rate")</f>
@@ -4585,13 +4091,13 @@
         <v>30</v>
       </c>
       <c r="K4" s="111" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H6</f>
-        <v>HKD_YC3MRH_2x5F#0001</v>
+        <v>HKD_YC3MRH_2x5F#0000</v>
       </c>
       <c r="B5" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A5,"Rate")</f>
@@ -4623,13 +4129,13 @@
         <v>40</v>
       </c>
       <c r="K5" s="111" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H7</f>
-        <v>HKD_YC3MRH_3x6F#0001</v>
+        <v>HKD_YC3MRH_3x6F#0000</v>
       </c>
       <c r="B6" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A6,"Rate")</f>
@@ -4661,13 +4167,13 @@
         <v>50</v>
       </c>
       <c r="K6" s="111" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H8</f>
-        <v>HKD_YC3MRH_4x7F#0001</v>
+        <v>HKD_YC3MRH_4x7F#0000</v>
       </c>
       <c r="B7" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A7,"Rate")</f>
@@ -4699,13 +4205,13 @@
         <v>60</v>
       </c>
       <c r="K7" s="111" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H9</f>
-        <v>HKD_YC3MRH_5x8F#0001</v>
+        <v>HKD_YC3MRH_5x8F#0000</v>
       </c>
       <c r="B8" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A8,"Rate")</f>
@@ -4737,13 +4243,13 @@
         <v>70</v>
       </c>
       <c r="K8" s="111" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H10</f>
-        <v>HKD_YC3MRH_6x9F#0001</v>
+        <v>HKD_YC3MRH_6x9F#0000</v>
       </c>
       <c r="B9" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A9,"Rate")</f>
@@ -4775,7 +4281,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H11</f>
-        <v>HKD_YC3MRH_7x10F#0001</v>
+        <v>HKD_YC3MRH_7x10F#0000</v>
       </c>
       <c r="B10" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A10,"Rate")</f>
@@ -4807,7 +4313,7 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="160" t="str">
         <f>HKD_YCRH_FRAs_3M!H12</f>
-        <v>HKD_YC3MRH_8x11F#0001</v>
+        <v>HKD_YC3MRH_8x11F#0000</v>
       </c>
       <c r="B11" s="122" t="str">
         <f>_xll.ohObjectPropertyValues(A11,"Rate")</f>
@@ -4839,7 +4345,7 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="161" t="str">
         <f>HKD_YCRH_FRAs_3M!H13</f>
-        <v>HKD_YC3MRH_9x12F#0001</v>
+        <v>HKD_YC3MRH_9x12F#0000</v>
       </c>
       <c r="B12" s="117" t="str">
         <f>_xll.ohObjectPropertyValues(A12,"Rate")</f>
@@ -4869,37 +4375,37 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="160" t="str">
+      <c r="A13" s="159" t="str">
         <f>HKD_YCRH_Swaps_3M!L6</f>
         <v>HKD_YC3MRH_QM3H1Y#0001</v>
       </c>
-      <c r="B13" s="122" t="str">
+      <c r="B13" s="128" t="str">
         <f>_xll.ohObjectPropertyValues(A13,"Rate")</f>
         <v>HKDQM3H1Y_Quote</v>
       </c>
-      <c r="C13" s="121">
+      <c r="C13" s="127">
         <f>_xll.qlRateHelperQuoteValue($A13,Trigger)</f>
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="D13" s="121">
+      <c r="D13" s="127">
         <f>_xll.qlSwapRateHelperSpread($A13,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="120" t="b">
-        <f t="shared" ref="E13:E49" si="0">IF(ISERROR(C13),FALSE,TRUE)</f>
+      <c r="E13" s="126" t="b">
+        <f t="shared" ref="E13:E39" si="0">IF(ISERROR(C13),FALSE,TRUE)</f>
         <v>1</v>
       </c>
-      <c r="F13" s="120">
+      <c r="F13" s="126">
         <v>50</v>
       </c>
-      <c r="G13" s="120">
+      <c r="G13" s="126">
         <v>1</v>
       </c>
-      <c r="H13" s="119">
+      <c r="H13" s="125">
         <f>_xll.qlRateHelperEarliestDate($A13,Trigger)</f>
         <v>41598</v>
       </c>
-      <c r="I13" s="118">
+      <c r="I13" s="124">
         <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
         <v>41963</v>
       </c>
@@ -5805,632 +5311,272 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="160" t="str">
+      <c r="A39" s="161" t="str">
         <f>HKD_YCRH_Swaps_3M!L32</f>
         <v>HKD_YC3MRH_QM3H24Y#0001</v>
       </c>
-      <c r="B39" s="122" t="str">
+      <c r="B39" s="117" t="str">
         <f>_xll.ohObjectPropertyValues(A39,"Rate")</f>
         <v>HKDQM3H24Y_Quote</v>
       </c>
-      <c r="C39" s="121" t="e">
+      <c r="C39" s="116" t="e">
         <f>_xll.qlRateHelperQuoteValue($A39,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="D39" s="121">
+      <c r="D39" s="116">
         <f>_xll.qlSwapRateHelperSpread($A39,Trigger)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="120" t="b">
+      <c r="E39" s="115" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F39" s="120">
+      <c r="F39" s="115">
         <v>50</v>
       </c>
-      <c r="G39" s="120">
+      <c r="G39" s="115">
         <v>1</v>
       </c>
-      <c r="H39" s="119">
+      <c r="H39" s="114">
         <f>_xll.qlRateHelperEarliestDate($A39,Trigger)</f>
         <v>41598</v>
       </c>
-      <c r="I39" s="118">
+      <c r="I39" s="113">
         <f>_xll.qlRateHelperLatestDate($A39,Trigger)</f>
         <v>50364</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L33</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B40" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A40,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C40" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A40,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D40" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A40,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E40" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="120">
-        <v>50</v>
-      </c>
-      <c r="G40" s="120">
-        <v>1</v>
-      </c>
-      <c r="H40" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A40,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I40" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A40,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L34</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B41" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A41,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C41" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A41,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D41" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A41,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E41" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="120">
-        <v>50</v>
-      </c>
-      <c r="G41" s="120">
-        <v>1</v>
-      </c>
-      <c r="H41" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A41,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I41" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A41,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L35</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B42" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A42,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C42" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A42,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D42" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A42,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E42" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="120">
-        <v>50</v>
-      </c>
-      <c r="G42" s="120">
-        <v>1</v>
-      </c>
-      <c r="H42" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A42,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I42" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A42,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L36</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B43" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A43,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C43" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A43,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D43" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A43,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E43" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="120">
-        <v>50</v>
-      </c>
-      <c r="G43" s="120">
-        <v>1</v>
-      </c>
-      <c r="H43" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A43,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I43" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A43,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L37</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B44" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A44,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C44" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A44,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D44" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A44,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E44" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F44" s="120">
-        <v>50</v>
-      </c>
-      <c r="G44" s="120">
-        <v>1</v>
-      </c>
-      <c r="H44" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A44,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I44" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A44,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L38</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B45" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A45,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C45" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A45,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D45" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A45,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E45" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F45" s="120">
-        <v>50</v>
-      </c>
-      <c r="G45" s="120">
-        <v>1</v>
-      </c>
-      <c r="H45" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A45,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I45" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A45,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L39</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B46" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A46,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C46" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A46,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D46" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A46,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E46" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="120">
-        <v>50</v>
-      </c>
-      <c r="G46" s="120">
-        <v>1</v>
-      </c>
-      <c r="H46" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A46,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I46" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A46,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L40</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B47" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A47,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C47" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A47,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D47" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A47,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E47" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="120">
-        <v>50</v>
-      </c>
-      <c r="G47" s="120">
-        <v>1</v>
-      </c>
-      <c r="H47" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A47,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I47" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A47,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="160" t="e">
-        <f>HKD_YCRH_Swaps_3M!L41</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B48" s="122" t="e">
-        <f>_xll.ohObjectPropertyValues(A48,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C48" s="121" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A48,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D48" s="121" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A48,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E48" s="120" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="120">
-        <v>50</v>
-      </c>
-      <c r="G48" s="120">
-        <v>1</v>
-      </c>
-      <c r="H48" s="119" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A48,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I48" s="118" t="e">
-        <f>_xll.qlRateHelperLatestDate($A48,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="161" t="e">
-        <f>HKD_YCRH_Swaps_3M!L42</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B49" s="117" t="e">
-        <f>_xll.ohObjectPropertyValues(A49,"Rate")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C49" s="116" t="e">
-        <f>_xll.qlRateHelperQuoteValue($A49,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D49" s="116" t="e">
-        <f>_xll.qlSwapRateHelperSpread($A49,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E49" s="115" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="115">
-        <v>50</v>
-      </c>
-      <c r="G49" s="115">
-        <v>1</v>
-      </c>
-      <c r="H49" s="114" t="e">
-        <f>_xll.qlRateHelperEarliestDate($A49,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I49" s="113" t="e">
-        <f>_xll.qlRateHelperLatestDate($A49,Trigger)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="68" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J68" s="130"/>
-    </row>
-    <row r="69" spans="10:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J69" s="123"/>
-    </row>
-    <row r="70" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J70" s="129"/>
-    </row>
-    <row r="73" spans="10:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="10:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J58" s="130"/>
+    </row>
+    <row r="59" spans="10:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J59" s="123"/>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J60" s="129"/>
+    </row>
+    <row r="63" spans="10:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="11:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K77" s="123" t="e">
+        <f>IF(D13=#REF!,C13-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="78" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K78" s="123" t="e">
+        <f>IF(D14=#REF!,C14-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="79" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K79" s="123" t="e">
+        <f>IF(D15=#REF!,C15-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="80" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K80" s="123" t="e">
+        <f>IF(D16=#REF!,C16-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="81" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K81" s="123" t="e">
+        <f>IF(D17=#REF!,C17-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="82" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K82" s="123" t="e">
+        <f>IF(D18=#REF!,C18-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="83" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K83" s="123" t="e">
+        <f>IF(D19=#REF!,C19-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="84" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K84" s="123" t="e">
+        <f>IF(D20=#REF!,C20-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="85" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K85" s="123" t="e">
+        <f>IF(D21=#REF!,C21-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="86" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K86" s="123" t="e">
+        <f>IF(D22=#REF!,C22-#REF!,"--")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
     <row r="87" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K87" s="123" t="e">
-        <f>IF(D13=#REF!,C13-#REF!,"--")</f>
+        <f>IF(D23=#REF!,C23-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="88" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K88" s="123" t="e">
-        <f>IF(D14=#REF!,C14-#REF!,"--")</f>
+        <f>IF(D24=#REF!,C24-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="89" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K89" s="123" t="e">
-        <f>IF(D15=#REF!,C15-#REF!,"--")</f>
+        <f>IF(D25=#REF!,C25-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="90" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K90" s="123" t="e">
-        <f>IF(D16=#REF!,C16-#REF!,"--")</f>
+        <f>IF(D26=#REF!,C26-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="91" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K91" s="123" t="e">
-        <f>IF(D17=#REF!,C17-#REF!,"--")</f>
+        <f>IF(D27=#REF!,C27-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="92" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K92" s="123" t="e">
-        <f>IF(D18=#REF!,C18-#REF!,"--")</f>
+        <f>IF(D28=#REF!,C28-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="93" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K93" s="123" t="e">
-        <f>IF(D19=#REF!,C19-#REF!,"--")</f>
+        <f>IF(D29=#REF!,C29-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="94" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K94" s="123" t="e">
-        <f>IF(D20=#REF!,C20-#REF!,"--")</f>
+        <f>IF(D30=#REF!,C30-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="95" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K95" s="123" t="e">
-        <f>IF(D21=#REF!,C21-#REF!,"--")</f>
+        <f>IF(D31=#REF!,C31-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="96" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K96" s="123" t="e">
-        <f>IF(D22=#REF!,C22-#REF!,"--")</f>
+        <f>IF(D32=#REF!,C32-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="97" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K97" s="123" t="e">
-        <f>IF(D23=#REF!,C23-#REF!,"--")</f>
+        <f>IF(D33=#REF!,C33-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="98" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K98" s="123" t="e">
-        <f>IF(D24=#REF!,C24-#REF!,"--")</f>
+        <f>IF(D34=#REF!,C34-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="99" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K99" s="123" t="e">
-        <f>IF(D25=#REF!,C25-#REF!,"--")</f>
+        <f>IF(D35=#REF!,C35-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="100" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K100" s="123" t="e">
-        <f>IF(D26=#REF!,C26-#REF!,"--")</f>
+        <f>IF(D36=#REF!,C36-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="101" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K101" s="123" t="e">
-        <f>IF(D27=#REF!,C27-#REF!,"--")</f>
+        <f>IF(D37=#REF!,C37-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="102" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K102" s="123" t="e">
-        <f>IF(D28=#REF!,C28-#REF!,"--")</f>
+        <f>IF(D38=#REF!,C38-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="103" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K103" s="123" t="e">
-        <f>IF(D29=#REF!,C29-#REF!,"--")</f>
+        <f>IF(D39=#REF!,C39-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="104" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K104" s="123" t="e">
-        <f>IF(D30=#REF!,C30-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="105" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K105" s="123" t="e">
-        <f>IF(D31=#REF!,C31-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="106" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K106" s="123" t="e">
-        <f>IF(D32=#REF!,C32-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="107" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K107" s="123" t="e">
-        <f>IF(D33=#REF!,C33-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="108" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K108" s="123" t="e">
-        <f>IF(D34=#REF!,C34-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="109" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K109" s="123" t="e">
-        <f>IF(D35=#REF!,C35-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="110" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K110" s="123" t="e">
-        <f>IF(D36=#REF!,C36-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="111" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K111" s="123" t="e">
-        <f>IF(D37=#REF!,C37-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="112" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K112" s="123" t="e">
-        <f>IF(D38=#REF!,C38-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="113" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K113" s="123" t="e">
-        <f>IF(D39=#REF!,C39-#REF!,"--")</f>
+        <f>IF(#REF!=#REF!,#REF!-#REF!,"--")</f>
         <v>#REF!</v>
-      </c>
-    </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K114" s="123" t="e">
-        <f>IF(D40=#REF!,C40-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="115" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K115" s="123" t="e">
-        <f>IF(D41=#REF!,C41-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="116" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K116" s="123" t="e">
-        <f>IF(D42=#REF!,C42-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="117" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K117" s="123" t="e">
-        <f>IF(D43=#REF!,C43-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="118" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K118" s="123" t="e">
-        <f>IF(D44=#REF!,C44-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="119" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K119" s="123" t="e">
-        <f>IF(D45=#REF!,C45-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="120" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K120" s="123" t="e">
-        <f>IF(D46=#REF!,C46-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="121" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K121" s="123" t="e">
-        <f>IF(D47=#REF!,C47-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="122" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K122" s="123" t="e">
-        <f>IF(D48=#REF!,C48-#REF!,"--")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="123" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K123" s="123" t="e">
-        <f>IF(D49=#REF!,C49-#REF!,"--")</f>
-        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -6463,22 +5609,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="162" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="163"/>
+      <c r="A1" s="164" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="165"/>
       <c r="D1" s="151" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E1" s="150" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F1" s="150"/>
       <c r="G1" s="150" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H1" s="149" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="I1" s="131">
         <f t="array" ref="I1:I50">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
@@ -6487,13 +5633,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="148" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B2" s="147">
         <v>0</v>
       </c>
       <c r="C2" s="152" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D2" s="139" t="str">
         <f t="array" ref="D2:D50">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
@@ -6521,13 +5667,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="144" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B3" s="146">
         <v>0</v>
       </c>
       <c r="C3" s="152" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D3" s="139" t="str">
         <v>HKD_YC3MRH_2x5F</v>
@@ -6554,13 +5700,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="144" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B4" s="146">
         <v>0</v>
       </c>
       <c r="C4" s="152" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D4" s="139" t="str">
         <v>HKD_YC3MRH_3x6F</v>
@@ -6587,13 +5733,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="144" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="145" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="152" t="s">
         <v>115</v>
-      </c>
-      <c r="B5" s="145" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="152" t="s">
-        <v>125</v>
       </c>
       <c r="D5" s="139" t="str">
         <v>HKD_YC3MRH_4x7F</v>
@@ -6620,14 +5766,14 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="144" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B6" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(Selected!D2)</f>
         <v/>
       </c>
       <c r="C6" s="152" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D6" s="139" t="str">
         <v>HKD_YC3MRH_5x8F</v>
@@ -6655,14 +5801,14 @@
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="142" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D50),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_RateHelpersSelected#0008</v>
+        <v>HKD_YC3MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
       <c r="C7" s="152" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D7" s="139" t="str">
         <v>HKD_YC3MRH_6x9F</v>
@@ -6689,7 +5835,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="152" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D8" s="139" t="str">
         <v>HKD_YC3MRH_7x10F</v>
@@ -6716,7 +5862,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" s="152" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D9" s="139" t="str">
         <v>HKD_YC3MRH_8x11F</v>
@@ -6743,7 +5889,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" s="152" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D10" s="139" t="str">
         <v>HKD_YC3MRH_QM3H1Y</v>
@@ -6770,7 +5916,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" s="152" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D11" s="139" t="str">
         <v>HKD_YC3MRH_QM3H18M</v>
@@ -6798,7 +5944,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="140"/>
       <c r="C12" s="152" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D12" s="139" t="str">
         <v>HKD_YC3MRH_QM3H2Y</v>
@@ -6826,7 +5972,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="140"/>
       <c r="C13" s="152" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D13" s="139" t="str">
         <v>HKD_YC3MRH_QM3H3Y</v>
@@ -6853,7 +5999,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="152" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D14" s="139" t="str">
         <v>HKD_YC3MRH_QM3H4Y</v>
@@ -6880,7 +6026,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" s="152" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D15" s="139" t="str">
         <v>HKD_YC3MRH_QM3H5Y</v>
@@ -6907,7 +6053,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="152" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D16" s="139" t="str">
         <v>HKD_YC3MRH_QM3H7Y</v>
@@ -6934,7 +6080,7 @@
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C17" s="152" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D17" s="139" t="str">
         <v>HKD_YC3MRH_QM3H10Y</v>
@@ -6961,7 +6107,7 @@
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C18" s="152" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D18" s="139" t="str">
         <v>HKD_YC3MRH_QM3H12Y</v>
@@ -6988,7 +6134,7 @@
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C19" s="152" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D19" s="139" t="str">
         <v>HKD_YC3MRH_QM3H15Y</v>
@@ -7764,7 +6910,7 @@
       <c r="I52" s="131"/>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D53" s="170"/>
+      <c r="D53" s="162"/>
       <c r="I53" s="131"/>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -7987,8 +7133,8 @@
       <c r="I126" s="131"/>
     </row>
     <row r="129" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I129" s="171" t="s">
-        <v>142</v>
+      <c r="I129" s="163" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -8034,19 +7180,19 @@
       </c>
     </row>
     <row r="2" spans="1:31" s="76" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="164" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="166"/>
-      <c r="H2" s="167" t="s">
+      <c r="B2" s="166" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="168"/>
+      <c r="H2" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="169"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="171"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="76"/>
@@ -8085,7 +7231,7 @@
       <c r="A4" s="76"/>
       <c r="B4" s="84"/>
       <c r="C4" s="109" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D4" s="155">
         <v>3</v>
@@ -8098,7 +7244,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="8">
-        <v>41598.597199074073</v>
+        <v>41598.603819444441</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="76"/>
@@ -8126,7 +7272,7 @@
       <c r="A5" s="76"/>
       <c r="B5" s="84"/>
       <c r="C5" s="108" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D5" s="85" t="str">
         <f>_xll.qlPeriodEquivalent(D4&amp;"M")</f>
@@ -8168,10 +7314,10 @@
       <c r="A6" s="76"/>
       <c r="B6" s="84"/>
       <c r="C6" s="108" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D6" s="85" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="80"/>
@@ -8209,10 +7355,10 @@
       <c r="A7" s="76"/>
       <c r="B7" s="84"/>
       <c r="C7" s="108" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D7" s="85" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E7" s="81"/>
       <c r="F7" s="80"/>
@@ -8250,7 +7396,7 @@
       <c r="A8" s="76"/>
       <c r="B8" s="84"/>
       <c r="C8" s="156" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D8" s="107" t="str">
         <f>Currency&amp;"_YC"&amp;IndexTenor&amp;"RH"</f>
@@ -8330,11 +7476,11 @@
       <c r="A10" s="76"/>
       <c r="B10" s="84"/>
       <c r="C10" s="104" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D10" s="106" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC3M#0003</v>
+        <v>_HKDYC3M#0002</v>
       </c>
       <c r="E10" s="81"/>
       <c r="F10" s="80"/>
@@ -8368,14 +7514,14 @@
       <c r="A11" s="76"/>
       <c r="B11" s="84"/>
       <c r="C11" s="91" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D11" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
       <c r="E11" s="154" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="76"/>
@@ -8408,7 +7554,7 @@
       <c r="A12" s="76"/>
       <c r="B12" s="84"/>
       <c r="C12" s="104" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D12" s="103" t="str">
         <f>"_"&amp;Currency&amp;"YC"&amp;IndexTenor</f>
@@ -8417,12 +7563,12 @@
       <c r="E12" s="81"/>
       <c r="F12" s="80"/>
       <c r="G12" s="76"/>
-      <c r="H12" s="167" t="s">
+      <c r="H12" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="168"/>
-      <c r="J12" s="168"/>
-      <c r="K12" s="169"/>
+      <c r="I12" s="170"/>
+      <c r="J12" s="170"/>
+      <c r="K12" s="171"/>
       <c r="L12" s="76"/>
       <c r="M12" s="76"/>
       <c r="N12" s="76"/>
@@ -8448,7 +7594,7 @@
       <c r="A13" s="76"/>
       <c r="B13" s="84"/>
       <c r="C13" s="93" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D13" s="102">
         <v>0</v>
@@ -8527,7 +7673,7 @@
       <c r="A15" s="76"/>
       <c r="B15" s="84"/>
       <c r="C15" s="93" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D15" s="101"/>
       <c r="E15" s="81"/>
@@ -8566,7 +7712,7 @@
       <c r="A16" s="76"/>
       <c r="B16" s="84"/>
       <c r="C16" s="93" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D16" s="100" t="str">
         <f>Currency&amp;"TOY_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
@@ -8611,7 +7757,7 @@
       <c r="A17" s="76"/>
       <c r="B17" s="84"/>
       <c r="C17" s="93" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D17" s="98">
         <f>DATE(YEAR(_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),NDays&amp;"D")),12,31)</f>
@@ -8656,7 +7802,7 @@
       <c r="A18" s="76"/>
       <c r="B18" s="84"/>
       <c r="C18" s="93" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D18" s="96" t="e">
         <f>NA()</f>
@@ -8701,7 +7847,7 @@
       <c r="A19" s="76"/>
       <c r="B19" s="84"/>
       <c r="C19" s="93" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D19" s="94"/>
       <c r="E19" s="81"/>
@@ -8740,10 +7886,10 @@
       <c r="A20" s="76"/>
       <c r="B20" s="84"/>
       <c r="C20" s="93" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D20" s="92" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E20" s="81"/>
       <c r="F20" s="80"/>
@@ -8782,10 +7928,10 @@
       <c r="A21" s="76"/>
       <c r="B21" s="84"/>
       <c r="C21" s="91" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D21" s="90" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E21" s="81"/>
       <c r="F21" s="80"/>
@@ -8935,7 +8081,7 @@
       <c r="A25" s="76"/>
       <c r="B25" s="84"/>
       <c r="C25" s="83" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D25" s="82" t="str">
         <f>_xll.ohRangeRetrieveError(Selected!I1)</f>

</xml_diff>

<commit_message>
consolidate named ranges for calendars
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD_YC3MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15330" yWindow="105" windowWidth="14325" windowHeight="8250"/>
+    <workbookView xWindow="22710" yWindow="-15" windowWidth="7635" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="8" r:id="rId1"/>
@@ -14,11 +14,11 @@
     <sheet name="Selected" sheetId="12" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Accuracy">'General Settings'!$D$19</definedName>
+    <definedName name="Accuracy">'General Settings'!$D$18</definedName>
     <definedName name="BondBasisDayCounter">'General Settings'!$J$17</definedName>
     <definedName name="Calendar">'General Settings'!$J$19</definedName>
     <definedName name="Currency">'General Settings'!$J$14</definedName>
-    <definedName name="DayCounter">'General Settings'!$D$15</definedName>
+    <definedName name="DayCounter">'General Settings'!$D$14</definedName>
     <definedName name="DepoInclusionCriteria" localSheetId="4">Selected!$B$5</definedName>
     <definedName name="Discounting">'General Settings'!$J$20</definedName>
     <definedName name="Discounting2">'General Settings'!$J$21</definedName>
@@ -28,7 +28,7 @@
     <definedName name="FrontFuturesRollingDays" localSheetId="4">Selected!$B$4</definedName>
     <definedName name="IborType">'General Settings'!$D$6</definedName>
     <definedName name="IndexTenor">'General Settings'!$D$5</definedName>
-    <definedName name="InterpolatorID">'General Settings'!$D$21</definedName>
+    <definedName name="InterpolatorID">'General Settings'!$D$20</definedName>
     <definedName name="MinDistance">RateHelpers!$K$2:$K$169</definedName>
     <definedName name="MoneyMarketDayCounter">'General Settings'!$J$18</definedName>
     <definedName name="Months">'General Settings'!$D$4</definedName>
@@ -48,7 +48,7 @@
     <definedName name="SerializationPath">'General Settings'!$J$8</definedName>
     <definedName name="Serialize">'General Settings'!$J$7</definedName>
     <definedName name="SwapFixedFreq">'General Settings'!$D$7</definedName>
-    <definedName name="TraitsID">'General Settings'!$D$20</definedName>
+    <definedName name="TraitsID">'General Settings'!$D$19</definedName>
     <definedName name="Trigger">'General Settings'!$J$4</definedName>
     <definedName name="YieldCurve">'General Settings'!$D$10</definedName>
   </definedNames>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0">
+    <comment ref="D19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="147">
   <si>
     <t>_Quote</t>
   </si>
@@ -2130,7 +2130,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="8">
-        <v>41599.519687499997</v>
+        <v>41599.618692129632</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="76"/>
@@ -2365,8 +2365,8 @@
         <v>81</v>
       </c>
       <c r="D10" s="106" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D18),NA(),D16:E16),IF(ISERROR(D18),NA(),D17:E17),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_HKDYC3M#0000</v>
+        <f>_xll.qlPiecewiseYieldCurve(D12,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D17),NA(),D15:E15),IF(ISERROR(D17),NA(),D16:E16),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
+        <v>_HKDYC3M#0002</v>
       </c>
       <c r="E10" s="81"/>
       <c r="F10" s="80"/>
@@ -2517,12 +2517,9 @@
       <c r="A14" s="76"/>
       <c r="B14" s="84"/>
       <c r="C14" s="93" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="101" t="str">
-        <f>Calendar</f>
-        <v>HongKong::HKEx</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D14" s="101"/>
       <c r="E14" s="81"/>
       <c r="F14" s="80"/>
       <c r="G14" s="76"/>
@@ -2559,10 +2556,16 @@
       <c r="A15" s="76"/>
       <c r="B15" s="84"/>
       <c r="C15" s="93" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="101"/>
-      <c r="E15" s="81"/>
+        <v>77</v>
+      </c>
+      <c r="D15" s="100" t="str">
+        <f>Currency&amp;"TOY_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
+        <v>HKDTOY_SYNTH3M_Quote</v>
+      </c>
+      <c r="E15" s="99" t="str">
+        <f>Currency&amp;"TOY2_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
+        <v>HKDTOY2_SYNTH3M_Quote</v>
+      </c>
       <c r="F15" s="80"/>
       <c r="G15" s="76"/>
       <c r="H15" s="7"/>
@@ -2598,15 +2601,15 @@
       <c r="A16" s="76"/>
       <c r="B16" s="84"/>
       <c r="C16" s="93" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="100" t="str">
-        <f>Currency&amp;"TOY_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
-        <v>HKDTOY_SYNTH3M_Quote</v>
-      </c>
-      <c r="E16" s="99" t="str">
-        <f>Currency&amp;"TOY2_SYNTH"&amp;IndexTenor&amp;"_Quote"</f>
-        <v>HKDTOY2_SYNTH3M_Quote</v>
+        <v>76</v>
+      </c>
+      <c r="D16" s="98">
+        <f>DATE(YEAR(_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),NDays&amp;"D")),12,31)</f>
+        <v>41639</v>
+      </c>
+      <c r="E16" s="97">
+        <f>DATE(YEAR(D16+1),12,31)</f>
+        <v>42004</v>
       </c>
       <c r="F16" s="80"/>
       <c r="G16" s="76"/>
@@ -2643,15 +2646,15 @@
       <c r="A17" s="76"/>
       <c r="B17" s="84"/>
       <c r="C17" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="98">
-        <f>DATE(YEAR(_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),NDays&amp;"D")),12,31)</f>
-        <v>41639</v>
-      </c>
-      <c r="E17" s="97">
-        <f>DATE(YEAR(D17+1),12,31)</f>
-        <v>42004</v>
+        <v>75</v>
+      </c>
+      <c r="D17" s="96" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="95" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="F17" s="80"/>
       <c r="G17" s="76"/>
@@ -2688,16 +2691,10 @@
       <c r="A18" s="76"/>
       <c r="B18" s="84"/>
       <c r="C18" s="93" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="96" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E18" s="95" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D18" s="94"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="80"/>
       <c r="G18" s="76"/>
       <c r="H18" s="7"/>
@@ -2733,9 +2730,11 @@
       <c r="A19" s="76"/>
       <c r="B19" s="84"/>
       <c r="C19" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="94"/>
+        <v>73</v>
+      </c>
+      <c r="D19" s="92" t="s">
+        <v>72</v>
+      </c>
       <c r="E19" s="81"/>
       <c r="F19" s="80"/>
       <c r="G19" s="76"/>
@@ -2771,11 +2770,11 @@
     <row r="20" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="76"/>
       <c r="B20" s="84"/>
-      <c r="C20" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="92" t="s">
-        <v>72</v>
+      <c r="C20" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="90" t="s">
+        <v>70</v>
       </c>
       <c r="E20" s="81"/>
       <c r="F20" s="80"/>
@@ -2813,12 +2812,8 @@
     <row r="21" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="76"/>
       <c r="B21" s="84"/>
-      <c r="C21" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="90" t="s">
-        <v>70</v>
-      </c>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
       <c r="E21" s="81"/>
       <c r="F21" s="80"/>
       <c r="G21" s="76"/>
@@ -2855,8 +2850,14 @@
     <row r="22" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="76"/>
       <c r="B22" s="84"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
+      <c r="C22" s="88">
+        <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
+        <v>41599</v>
+      </c>
+      <c r="D22" s="87">
+        <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
+        <v>1</v>
+      </c>
       <c r="E22" s="81"/>
       <c r="F22" s="80"/>
       <c r="G22" s="76"/>
@@ -2888,13 +2889,13 @@
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="76"/>
       <c r="B23" s="84"/>
-      <c r="C23" s="88">
-        <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41599</v>
-      </c>
-      <c r="D23" s="87">
-        <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>1</v>
+      <c r="C23" s="86">
+        <f>MAX(_xll.ohPack(Selected!H2:H50))</f>
+        <v>47078</v>
+      </c>
+      <c r="D23" s="85">
+        <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
+        <v>0.65497495396013317</v>
       </c>
       <c r="E23" s="81"/>
       <c r="F23" s="80"/>
@@ -2927,13 +2928,12 @@
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="76"/>
       <c r="B24" s="84"/>
-      <c r="C24" s="86">
-        <f>MAX(_xll.ohPack(Selected!H2:H50))</f>
-        <v>41964</v>
-      </c>
-      <c r="D24" s="85">
-        <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.99558456903541614</v>
+      <c r="C24" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="82" t="str">
+        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v/>
       </c>
       <c r="E24" s="81"/>
       <c r="F24" s="80"/>
@@ -2963,18 +2963,13 @@
       <c r="AD24" s="76"/>
       <c r="AE24" s="76"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="76"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="83" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="82" t="str">
-        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v/>
-      </c>
-      <c r="E25" s="81"/>
-      <c r="F25" s="80"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="159"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="77"/>
       <c r="G25" s="76"/>
       <c r="H25" s="76"/>
       <c r="I25" s="76"/>
@@ -3001,13 +2996,13 @@
       <c r="AD25" s="76"/>
       <c r="AE25" s="76"/>
     </row>
-    <row r="26" spans="1:31" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="76"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="159"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="77"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
       <c r="G26" s="76"/>
       <c r="H26" s="76"/>
       <c r="I26" s="76"/>
@@ -4257,11 +4252,6 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A64" s="76"/>
-      <c r="B64" s="76"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
       <c r="G64" s="76"/>
       <c r="H64" s="76"/>
       <c r="I64" s="76"/>
@@ -4437,16 +4427,16 @@
     <mergeCell ref="H12:K12"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20">
       <formula1>"Linear,BackwardFlat,ForwardFlat,Linear,LogLinear,CubicNaturalSpline,LogCubicNaturalSpline,MonotonicCubicNaturalSpline,MonotonicLogCubicNaturalSpline,FritschButlandCubic,FritschButlandLogCubic,KrugerCubic,KrugerLogCubic"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
       <formula1>"1D,1W,1M,2M,3M,6M,1Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19">
       <formula1>"Discount,ZeroYield,ForwardRate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),'1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14">
@@ -4560,7 +4550,7 @@
       </c>
       <c r="H3" s="37" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_T3F1#0000</v>
+        <v>HKD_YC3MRH_T3F1#0002</v>
       </c>
       <c r="I3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -4594,7 +4584,7 @@
       </c>
       <c r="H4" s="27" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_TOM3F1#0000</v>
+        <v>HKD_YC3MRH_TOM3F1#0002</v>
       </c>
       <c r="I4" s="35" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -4629,7 +4619,7 @@
       </c>
       <c r="H5" s="32" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_1x4F#0000</v>
+        <v>HKD_YC3MRH_1x4F#0002</v>
       </c>
       <c r="I5" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -4664,7 +4654,7 @@
       </c>
       <c r="H6" s="32" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_2x5F#0000</v>
+        <v>HKD_YC3MRH_2x5F#0002</v>
       </c>
       <c r="I6" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -4699,7 +4689,7 @@
       </c>
       <c r="H7" s="32" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_3x6F#0000</v>
+        <v>HKD_YC3MRH_3x6F#0002</v>
       </c>
       <c r="I7" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -4734,7 +4724,7 @@
       </c>
       <c r="H8" s="32" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_4x7F#0000</v>
+        <v>HKD_YC3MRH_4x7F#0002</v>
       </c>
       <c r="I8" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -4769,7 +4759,7 @@
       </c>
       <c r="H9" s="32" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_5x8F#0000</v>
+        <v>HKD_YC3MRH_5x8F#0002</v>
       </c>
       <c r="I9" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -4804,7 +4794,7 @@
       </c>
       <c r="H10" s="32" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_6x9F#0000</v>
+        <v>HKD_YC3MRH_6x9F#0002</v>
       </c>
       <c r="I10" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -4839,7 +4829,7 @@
       </c>
       <c r="H11" s="32" t="str">
         <f>_xll.qlFraRateHelper(G11,F11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_7x10F#0000</v>
+        <v>HKD_YC3MRH_7x10F#0002</v>
       </c>
       <c r="I11" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H11)</f>
@@ -4874,7 +4864,7 @@
       </c>
       <c r="H12" s="32" t="str">
         <f>_xll.qlFraRateHelper(G12,F12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_8x11F#0000</v>
+        <v>HKD_YC3MRH_8x11F#0002</v>
       </c>
       <c r="I12" s="31" t="str">
         <f>_xll.ohRangeRetrieveError(H12)</f>
@@ -4909,7 +4899,7 @@
       </c>
       <c r="H13" s="27" t="str">
         <f>_xll.qlFraRateHelper(G13,F13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_9x12F#0000</v>
+        <v>HKD_YC3MRH_9x12F#0002</v>
       </c>
       <c r="I13" s="26" t="str">
         <f>_xll.ohRangeRetrieveError(H13)</f>
@@ -5081,7 +5071,7 @@
       </c>
       <c r="L4" s="69" t="str">
         <f>_xll.qlIborIndex(K4,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H_Hibor3M#0000</v>
+        <v>HKD_YC3MRH_QM3H_Hibor3M#0002</v>
       </c>
       <c r="M4" s="68" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -5161,7 +5151,7 @@
       </c>
       <c r="L6" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H1Y#0000</v>
+        <v>HKD_YC3MRH_QM3H1Y#0002</v>
       </c>
       <c r="M6" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -5208,7 +5198,7 @@
       </c>
       <c r="L7" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15M#0000</v>
+        <v>HKD_YC3MRH_QM3H15M#0002</v>
       </c>
       <c r="M7" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -5255,7 +5245,7 @@
       </c>
       <c r="L8" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18M#0000</v>
+        <v>HKD_YC3MRH_QM3H18M#0002</v>
       </c>
       <c r="M8" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -5302,7 +5292,7 @@
       </c>
       <c r="L9" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21M#0000</v>
+        <v>HKD_YC3MRH_QM3H21M#0002</v>
       </c>
       <c r="M9" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -5349,7 +5339,7 @@
       </c>
       <c r="L10" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H2Y#0000</v>
+        <v>HKD_YC3MRH_QM3H2Y#0002</v>
       </c>
       <c r="M10" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -5396,7 +5386,7 @@
       </c>
       <c r="L11" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H3Y#0000</v>
+        <v>HKD_YC3MRH_QM3H3Y#0002</v>
       </c>
       <c r="M11" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -5443,7 +5433,7 @@
       </c>
       <c r="L12" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H4Y#0000</v>
+        <v>HKD_YC3MRH_QM3H4Y#0002</v>
       </c>
       <c r="M12" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -5490,7 +5480,7 @@
       </c>
       <c r="L13" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H5Y#0000</v>
+        <v>HKD_YC3MRH_QM3H5Y#0002</v>
       </c>
       <c r="M13" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -5537,7 +5527,7 @@
       </c>
       <c r="L14" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H6Y#0000</v>
+        <v>HKD_YC3MRH_QM3H6Y#0002</v>
       </c>
       <c r="M14" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -5584,7 +5574,7 @@
       </c>
       <c r="L15" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H7Y#0000</v>
+        <v>HKD_YC3MRH_QM3H7Y#0002</v>
       </c>
       <c r="M15" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -5631,7 +5621,7 @@
       </c>
       <c r="L16" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H8Y#0000</v>
+        <v>HKD_YC3MRH_QM3H8Y#0002</v>
       </c>
       <c r="M16" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -5678,7 +5668,7 @@
       </c>
       <c r="L17" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H9Y#0000</v>
+        <v>HKD_YC3MRH_QM3H9Y#0002</v>
       </c>
       <c r="M17" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -5725,7 +5715,7 @@
       </c>
       <c r="L18" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H10Y#0000</v>
+        <v>HKD_YC3MRH_QM3H10Y#0002</v>
       </c>
       <c r="M18" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -5772,7 +5762,7 @@
       </c>
       <c r="L19" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H11Y#0000</v>
+        <v>HKD_YC3MRH_QM3H11Y#0002</v>
       </c>
       <c r="M19" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -5819,7 +5809,7 @@
       </c>
       <c r="L20" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H12Y#0000</v>
+        <v>HKD_YC3MRH_QM3H12Y#0002</v>
       </c>
       <c r="M20" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -5866,7 +5856,7 @@
       </c>
       <c r="L21" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H13Y#0000</v>
+        <v>HKD_YC3MRH_QM3H13Y#0002</v>
       </c>
       <c r="M21" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -5913,7 +5903,7 @@
       </c>
       <c r="L22" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H14Y#0000</v>
+        <v>HKD_YC3MRH_QM3H14Y#0002</v>
       </c>
       <c r="M22" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -5960,7 +5950,7 @@
       </c>
       <c r="L23" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H15Y#0000</v>
+        <v>HKD_YC3MRH_QM3H15Y#0002</v>
       </c>
       <c r="M23" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -6007,7 +5997,7 @@
       </c>
       <c r="L24" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H16Y#0000</v>
+        <v>HKD_YC3MRH_QM3H16Y#0002</v>
       </c>
       <c r="M24" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -6054,7 +6044,7 @@
       </c>
       <c r="L25" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H17Y#0000</v>
+        <v>HKD_YC3MRH_QM3H17Y#0002</v>
       </c>
       <c r="M25" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -6101,7 +6091,7 @@
       </c>
       <c r="L26" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H18Y#0000</v>
+        <v>HKD_YC3MRH_QM3H18Y#0002</v>
       </c>
       <c r="M26" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -6148,7 +6138,7 @@
       </c>
       <c r="L27" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H19Y#0000</v>
+        <v>HKD_YC3MRH_QM3H19Y#0002</v>
       </c>
       <c r="M27" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -6195,7 +6185,7 @@
       </c>
       <c r="L28" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H20Y#0000</v>
+        <v>HKD_YC3MRH_QM3H20Y#0002</v>
       </c>
       <c r="M28" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -6242,7 +6232,7 @@
       </c>
       <c r="L29" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H21Y#0000</v>
+        <v>HKD_YC3MRH_QM3H21Y#0002</v>
       </c>
       <c r="M29" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -6289,7 +6279,7 @@
       </c>
       <c r="L30" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H22Y#0000</v>
+        <v>HKD_YC3MRH_QM3H22Y#0002</v>
       </c>
       <c r="M30" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -6336,7 +6326,7 @@
       </c>
       <c r="L31" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H23Y#0000</v>
+        <v>HKD_YC3MRH_QM3H23Y#0002</v>
       </c>
       <c r="M31" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -6383,7 +6373,7 @@
       </c>
       <c r="L32" s="57" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_QM3H24Y#0000</v>
+        <v>HKD_YC3MRH_QM3H24Y#0002</v>
       </c>
       <c r="M32" s="56" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -7107,13 +7097,13 @@
       <c r="K16" s="126">
         <v>1</v>
       </c>
-      <c r="L16" s="125" t="e">
+      <c r="L16" s="125">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M16" s="124" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M16" s="124">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41691</v>
       </c>
       <c r="P16" s="111" t="e">
         <v>#NUM!</v>
@@ -7152,13 +7142,13 @@
       <c r="K17" s="115">
         <v>1</v>
       </c>
-      <c r="L17" s="114" t="e">
+      <c r="L17" s="114">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M17" s="113" t="e">
+        <v>41600</v>
+      </c>
+      <c r="M17" s="113">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41694</v>
       </c>
       <c r="P17" s="111" t="e">
         <v>#NUM!</v>
@@ -7183,9 +7173,9 @@
         <f>_xll.ohObjectPropertyValues(E18,"Rate")</f>
         <v>HKD1x4F_Quote</v>
       </c>
-      <c r="G18" s="121" t="e">
+      <c r="G18" s="121">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="H18" s="121"/>
       <c r="I18" s="120" t="b">
@@ -7197,13 +7187,13 @@
       <c r="K18" s="120">
         <v>1</v>
       </c>
-      <c r="L18" s="119" t="e">
+      <c r="L18" s="119">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M18" s="118" t="e">
+        <v>41631</v>
+      </c>
+      <c r="M18" s="118">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41722</v>
       </c>
       <c r="P18" s="111" t="e">
         <v>#NUM!</v>
@@ -7228,9 +7218,9 @@
         <f>_xll.ohObjectPropertyValues(E19,"Rate")</f>
         <v>HKD2x5F_Quote</v>
       </c>
-      <c r="G19" s="121" t="e">
+      <c r="G19" s="121">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="H19" s="121"/>
       <c r="I19" s="120" t="b">
@@ -7242,13 +7232,13 @@
       <c r="K19" s="120">
         <v>1</v>
       </c>
-      <c r="L19" s="119" t="e">
+      <c r="L19" s="119">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M19" s="118" t="e">
+        <v>41660</v>
+      </c>
+      <c r="M19" s="118">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41751</v>
       </c>
       <c r="P19" s="111" t="e">
         <v>#NUM!</v>
@@ -7273,9 +7263,9 @@
         <f>_xll.ohObjectPropertyValues(E20,"Rate")</f>
         <v>HKD3x6F_Quote</v>
       </c>
-      <c r="G20" s="121" t="e">
+      <c r="G20" s="121">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="H20" s="121"/>
       <c r="I20" s="120" t="b">
@@ -7287,13 +7277,13 @@
       <c r="K20" s="120">
         <v>1</v>
       </c>
-      <c r="L20" s="119" t="e">
+      <c r="L20" s="119">
         <f>_xll.qlRateHelperEarliestDate($E20,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M20" s="118" t="e">
+        <v>41691</v>
+      </c>
+      <c r="M20" s="118">
         <f>_xll.qlRateHelperLatestDate($E20,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41780</v>
       </c>
       <c r="P20" s="111" t="e">
         <v>#NUM!</v>
@@ -7318,9 +7308,9 @@
         <f>_xll.ohObjectPropertyValues(E21,"Rate")</f>
         <v>HKD4x7F_Quote</v>
       </c>
-      <c r="G21" s="121" t="e">
+      <c r="G21" s="121">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.3E-3</v>
       </c>
       <c r="H21" s="121"/>
       <c r="I21" s="120" t="b">
@@ -7332,13 +7322,13 @@
       <c r="K21" s="120">
         <v>1</v>
       </c>
-      <c r="L21" s="119" t="e">
+      <c r="L21" s="119">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M21" s="118" t="e">
+        <v>41719</v>
+      </c>
+      <c r="M21" s="118">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41813</v>
       </c>
       <c r="P21" s="111" t="e">
         <v>#NUM!</v>
@@ -7363,9 +7353,9 @@
         <f>_xll.ohObjectPropertyValues(E22,"Rate")</f>
         <v>HKD5x8F_Quote</v>
       </c>
-      <c r="G22" s="121" t="e">
+      <c r="G22" s="121">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="H22" s="121"/>
       <c r="I22" s="120" t="b">
@@ -7377,13 +7367,13 @@
       <c r="K22" s="120">
         <v>1</v>
       </c>
-      <c r="L22" s="119" t="e">
+      <c r="L22" s="119">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M22" s="118" t="e">
+        <v>41751</v>
+      </c>
+      <c r="M22" s="118">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41842</v>
       </c>
       <c r="P22" s="111" t="e">
         <v>#NUM!</v>
@@ -7408,9 +7398,9 @@
         <f>_xll.ohObjectPropertyValues(E23,"Rate")</f>
         <v>HKD6x9F_Quote</v>
       </c>
-      <c r="G23" s="121" t="e">
+      <c r="G23" s="121">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.5000000000000005E-3</v>
       </c>
       <c r="H23" s="121"/>
       <c r="I23" s="120" t="b">
@@ -7422,13 +7412,13 @@
       <c r="K23" s="120">
         <v>1</v>
       </c>
-      <c r="L23" s="119" t="e">
+      <c r="L23" s="119">
         <f>_xll.qlRateHelperEarliestDate($E23,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M23" s="118" t="e">
+        <v>41780</v>
+      </c>
+      <c r="M23" s="118">
         <f>_xll.qlRateHelperLatestDate($E23,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41872</v>
       </c>
       <c r="P23" s="111" t="e">
         <v>#NUM!</v>
@@ -7453,9 +7443,9 @@
         <f>_xll.ohObjectPropertyValues(E24,"Rate")</f>
         <v>HKD7x10F_Quote</v>
       </c>
-      <c r="G24" s="121" t="e">
+      <c r="G24" s="121">
         <f>_xll.qlRateHelperQuoteValue($E24,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.6999999999999993E-3</v>
       </c>
       <c r="H24" s="121"/>
       <c r="I24" s="120" t="b">
@@ -7467,13 +7457,13 @@
       <c r="K24" s="120">
         <v>1</v>
       </c>
-      <c r="L24" s="119" t="e">
+      <c r="L24" s="119">
         <f>_xll.qlRateHelperEarliestDate($E24,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M24" s="118" t="e">
+        <v>41813</v>
+      </c>
+      <c r="M24" s="118">
         <f>_xll.qlRateHelperLatestDate($E24,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41905</v>
       </c>
       <c r="P24" s="111" t="e">
         <v>#NUM!</v>
@@ -7498,9 +7488,9 @@
         <f>_xll.ohObjectPropertyValues(E25,"Rate")</f>
         <v>HKD8x11F_Quote</v>
       </c>
-      <c r="G25" s="121" t="e">
+      <c r="G25" s="121">
         <f>_xll.qlRateHelperQuoteValue($E25,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="H25" s="121"/>
       <c r="I25" s="120" t="b">
@@ -7512,13 +7502,13 @@
       <c r="K25" s="120">
         <v>1</v>
       </c>
-      <c r="L25" s="119" t="e">
+      <c r="L25" s="119">
         <f>_xll.qlRateHelperEarliestDate($E25,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M25" s="118" t="e">
+        <v>41841</v>
+      </c>
+      <c r="M25" s="118">
         <f>_xll.qlRateHelperLatestDate($E25,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41933</v>
       </c>
       <c r="P25" s="111" t="e">
         <v>#NUM!</v>
@@ -7543,9 +7533,9 @@
         <f>_xll.ohObjectPropertyValues(E26,"Rate")</f>
         <v>HKD9x12F_Quote</v>
       </c>
-      <c r="G26" s="121" t="e">
+      <c r="G26" s="121">
         <f>_xll.qlRateHelperQuoteValue($E26,Trigger)</f>
-        <v>#NUM!</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H26" s="121"/>
       <c r="I26" s="120" t="b">
@@ -7557,13 +7547,13 @@
       <c r="K26" s="120">
         <v>1</v>
       </c>
-      <c r="L26" s="119" t="e">
+      <c r="L26" s="119">
         <f>_xll.qlRateHelperEarliestDate($E26,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M26" s="118" t="e">
+        <v>41872</v>
+      </c>
+      <c r="M26" s="118">
         <f>_xll.qlRateHelperLatestDate($E26,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41964</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
@@ -10667,17 +10657,17 @@
         <f>_xll.ohObjectPropertyValues(E96,"Rate")</f>
         <v>HKDQM3H1Y_Quote</v>
       </c>
-      <c r="G96" s="121" t="e">
+      <c r="G96" s="121">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H96" s="121" t="e">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="H96" s="121">
         <f>_xll.qlSwapRateHelperSpread($E96,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I96" s="120" t="b">
         <f t="shared" ref="I96:I132" si="8">IF(ISERROR(G96),FALSE,TRUE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" s="120">
         <v>50</v>
@@ -10685,13 +10675,13 @@
       <c r="K96" s="120">
         <v>1</v>
       </c>
-      <c r="L96" s="119" t="e">
+      <c r="L96" s="119">
         <f>_xll.qlRateHelperEarliestDate($E96,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M96" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M96" s="118">
         <f>_xll.qlRateHelperLatestDate($E96,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41964</v>
       </c>
       <c r="O96" s="123" t="e">
         <f t="shared" ref="O96:O132" si="9">IF(H96=H133,G96-G133,"--")</f>
@@ -10722,9 +10712,9 @@
         <f>_xll.qlRateHelperQuoteValue($E97,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H97" s="121" t="e">
+      <c r="H97" s="121">
         <f>_xll.qlSwapRateHelperSpread($E97,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I97" s="120" t="b">
         <f t="shared" si="8"/>
@@ -10736,13 +10726,13 @@
       <c r="K97" s="120">
         <v>1</v>
       </c>
-      <c r="L97" s="119" t="e">
+      <c r="L97" s="119">
         <f>_xll.qlRateHelperEarliestDate($E97,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M97" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M97" s="118">
         <f>_xll.qlRateHelperLatestDate($E97,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42058</v>
       </c>
       <c r="O97" s="123" t="e">
         <f t="shared" si="9"/>
@@ -10769,17 +10759,17 @@
         <f>_xll.ohObjectPropertyValues(E98,"Rate")</f>
         <v>HKDQM3H18M_Quote</v>
       </c>
-      <c r="G98" s="121" t="e">
+      <c r="G98" s="121">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H98" s="121" t="e">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="H98" s="121">
         <f>_xll.qlSwapRateHelperSpread($E98,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I98" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J98" s="120">
         <v>50</v>
@@ -10787,13 +10777,13 @@
       <c r="K98" s="120">
         <v>1</v>
       </c>
-      <c r="L98" s="119" t="e">
+      <c r="L98" s="119">
         <f>_xll.qlRateHelperEarliestDate($E98,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M98" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M98" s="118">
         <f>_xll.qlRateHelperLatestDate($E98,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42145</v>
       </c>
       <c r="O98" s="123" t="e">
         <f t="shared" si="9"/>
@@ -10824,9 +10814,9 @@
         <f>_xll.qlRateHelperQuoteValue($E99,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H99" s="121" t="e">
+      <c r="H99" s="121">
         <f>_xll.qlSwapRateHelperSpread($E99,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I99" s="120" t="b">
         <f t="shared" si="8"/>
@@ -10838,13 +10828,13 @@
       <c r="K99" s="120">
         <v>1</v>
       </c>
-      <c r="L99" s="119" t="e">
+      <c r="L99" s="119">
         <f>_xll.qlRateHelperEarliestDate($E99,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M99" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M99" s="118">
         <f>_xll.qlRateHelperLatestDate($E99,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42237</v>
       </c>
       <c r="O99" s="123" t="e">
         <f t="shared" si="9"/>
@@ -10871,17 +10861,17 @@
         <f>_xll.ohObjectPropertyValues(E100,"Rate")</f>
         <v>HKDQM3H2Y_Quote</v>
       </c>
-      <c r="G100" s="121" t="e">
+      <c r="G100" s="121">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H100" s="121" t="e">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="H100" s="121">
         <f>_xll.qlSwapRateHelperSpread($E100,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I100" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J100" s="120">
         <v>50</v>
@@ -10889,13 +10879,13 @@
       <c r="K100" s="120">
         <v>1</v>
       </c>
-      <c r="L100" s="119" t="e">
+      <c r="L100" s="119">
         <f>_xll.qlRateHelperEarliestDate($E100,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M100" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M100" s="118">
         <f>_xll.qlRateHelperLatestDate($E100,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42331</v>
       </c>
       <c r="O100" s="123" t="e">
         <f t="shared" si="9"/>
@@ -10922,17 +10912,17 @@
         <f>_xll.ohObjectPropertyValues(E101,"Rate")</f>
         <v>HKDQM3H3Y_Quote</v>
       </c>
-      <c r="G101" s="121" t="e">
+      <c r="G101" s="121">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H101" s="121" t="e">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="H101" s="121">
         <f>_xll.qlSwapRateHelperSpread($E101,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I101" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J101" s="120">
         <v>50</v>
@@ -10940,13 +10930,13 @@
       <c r="K101" s="120">
         <v>1</v>
       </c>
-      <c r="L101" s="119" t="e">
+      <c r="L101" s="119">
         <f>_xll.qlRateHelperEarliestDate($E101,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M101" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M101" s="118">
         <f>_xll.qlRateHelperLatestDate($E101,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42695</v>
       </c>
       <c r="O101" s="123" t="e">
         <f t="shared" si="9"/>
@@ -10973,17 +10963,17 @@
         <f>_xll.ohObjectPropertyValues(E102,"Rate")</f>
         <v>HKDQM3H4Y_Quote</v>
       </c>
-      <c r="G102" s="121" t="e">
+      <c r="G102" s="121">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H102" s="121" t="e">
+        <v>1.0899999999999998E-2</v>
+      </c>
+      <c r="H102" s="121">
         <f>_xll.qlSwapRateHelperSpread($E102,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I102" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J102" s="120">
         <v>50</v>
@@ -10991,13 +10981,13 @@
       <c r="K102" s="120">
         <v>1</v>
       </c>
-      <c r="L102" s="119" t="e">
+      <c r="L102" s="119">
         <f>_xll.qlRateHelperEarliestDate($E102,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M102" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M102" s="118">
         <f>_xll.qlRateHelperLatestDate($E102,Trigger)</f>
-        <v>#NUM!</v>
+        <v>43060</v>
       </c>
       <c r="O102" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11024,17 +11014,17 @@
         <f>_xll.ohObjectPropertyValues(E103,"Rate")</f>
         <v>HKDQM3H5Y_Quote</v>
       </c>
-      <c r="G103" s="121" t="e">
+      <c r="G103" s="121">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H103" s="121" t="e">
+        <v>1.4100000000000001E-2</v>
+      </c>
+      <c r="H103" s="121">
         <f>_xll.qlSwapRateHelperSpread($E103,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I103" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J103" s="120">
         <v>50</v>
@@ -11042,13 +11032,13 @@
       <c r="K103" s="120">
         <v>1</v>
       </c>
-      <c r="L103" s="119" t="e">
+      <c r="L103" s="119">
         <f>_xll.qlRateHelperEarliestDate($E103,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M103" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M103" s="118">
         <f>_xll.qlRateHelperLatestDate($E103,Trigger)</f>
-        <v>#NUM!</v>
+        <v>43425</v>
       </c>
       <c r="O103" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11079,9 +11069,9 @@
         <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H104" s="121" t="e">
+      <c r="H104" s="121">
         <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I104" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11093,13 +11083,13 @@
       <c r="K104" s="120">
         <v>1</v>
       </c>
-      <c r="L104" s="119" t="e">
+      <c r="L104" s="119">
         <f>_xll.qlRateHelperEarliestDate($E104,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M104" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M104" s="118">
         <f>_xll.qlRateHelperLatestDate($E104,Trigger)</f>
-        <v>#NUM!</v>
+        <v>43790</v>
       </c>
       <c r="O104" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11126,17 +11116,17 @@
         <f>_xll.ohObjectPropertyValues(E105,"Rate")</f>
         <v>HKDQM3H7Y_Quote</v>
       </c>
-      <c r="G105" s="121" t="e">
+      <c r="G105" s="121">
         <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H105" s="121" t="e">
+        <v>1.95E-2</v>
+      </c>
+      <c r="H105" s="121">
         <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I105" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J105" s="120">
         <v>50</v>
@@ -11144,13 +11134,13 @@
       <c r="K105" s="120">
         <v>1</v>
       </c>
-      <c r="L105" s="119" t="e">
+      <c r="L105" s="119">
         <f>_xll.qlRateHelperEarliestDate($E105,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M105" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M105" s="118">
         <f>_xll.qlRateHelperLatestDate($E105,Trigger)</f>
-        <v>#NUM!</v>
+        <v>44158</v>
       </c>
       <c r="O105" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11181,9 +11171,9 @@
         <f>_xll.qlRateHelperQuoteValue($E106,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H106" s="121" t="e">
+      <c r="H106" s="121">
         <f>_xll.qlSwapRateHelperSpread($E106,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I106" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11195,13 +11185,13 @@
       <c r="K106" s="120">
         <v>1</v>
       </c>
-      <c r="L106" s="119" t="e">
+      <c r="L106" s="119">
         <f>_xll.qlRateHelperEarliestDate($E106,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M106" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M106" s="118">
         <f>_xll.qlRateHelperLatestDate($E106,Trigger)</f>
-        <v>#NUM!</v>
+        <v>44522</v>
       </c>
       <c r="O106" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11232,9 +11222,9 @@
         <f>_xll.qlRateHelperQuoteValue($E107,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H107" s="121" t="e">
+      <c r="H107" s="121">
         <f>_xll.qlSwapRateHelperSpread($E107,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I107" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11246,13 +11236,13 @@
       <c r="K107" s="120">
         <v>1</v>
       </c>
-      <c r="L107" s="119" t="e">
+      <c r="L107" s="119">
         <f>_xll.qlRateHelperEarliestDate($E107,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M107" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M107" s="118">
         <f>_xll.qlRateHelperLatestDate($E107,Trigger)</f>
-        <v>#NUM!</v>
+        <v>44886</v>
       </c>
       <c r="O107" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11279,17 +11269,17 @@
         <f>_xll.ohObjectPropertyValues(E108,"Rate")</f>
         <v>HKDQM3H10Y_Quote</v>
       </c>
-      <c r="G108" s="121" t="e">
+      <c r="G108" s="121">
         <f>_xll.qlRateHelperQuoteValue($E108,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H108" s="121" t="e">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="H108" s="121">
         <f>_xll.qlSwapRateHelperSpread($E108,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I108" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J108" s="120">
         <v>50</v>
@@ -11297,13 +11287,13 @@
       <c r="K108" s="120">
         <v>1</v>
       </c>
-      <c r="L108" s="119" t="e">
+      <c r="L108" s="119">
         <f>_xll.qlRateHelperEarliestDate($E108,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M108" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M108" s="118">
         <f>_xll.qlRateHelperLatestDate($E108,Trigger)</f>
-        <v>#NUM!</v>
+        <v>45251</v>
       </c>
       <c r="O108" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11334,9 +11324,9 @@
         <f>_xll.qlRateHelperQuoteValue($E109,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H109" s="121" t="e">
+      <c r="H109" s="121">
         <f>_xll.qlSwapRateHelperSpread($E109,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I109" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11348,13 +11338,13 @@
       <c r="K109" s="120">
         <v>1</v>
       </c>
-      <c r="L109" s="119" t="e">
+      <c r="L109" s="119">
         <f>_xll.qlRateHelperEarliestDate($E109,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M109" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M109" s="118">
         <f>_xll.qlRateHelperLatestDate($E109,Trigger)</f>
-        <v>#NUM!</v>
+        <v>45617</v>
       </c>
       <c r="O109" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11381,17 +11371,17 @@
         <f>_xll.ohObjectPropertyValues(E110,"Rate")</f>
         <v>HKDQM3H12Y_Quote</v>
       </c>
-      <c r="G110" s="121" t="e">
+      <c r="G110" s="121">
         <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H110" s="121" t="e">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="H110" s="121">
         <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I110" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" s="120">
         <v>50</v>
@@ -11399,13 +11389,13 @@
       <c r="K110" s="120">
         <v>1</v>
       </c>
-      <c r="L110" s="119" t="e">
+      <c r="L110" s="119">
         <f>_xll.qlRateHelperEarliestDate($E110,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M110" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M110" s="118">
         <f>_xll.qlRateHelperLatestDate($E110,Trigger)</f>
-        <v>#NUM!</v>
+        <v>45982</v>
       </c>
       <c r="O110" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11436,9 +11426,9 @@
         <f>_xll.qlRateHelperQuoteValue($E111,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H111" s="121" t="e">
+      <c r="H111" s="121">
         <f>_xll.qlSwapRateHelperSpread($E111,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I111" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11450,13 +11440,13 @@
       <c r="K111" s="120">
         <v>1</v>
       </c>
-      <c r="L111" s="119" t="e">
+      <c r="L111" s="119">
         <f>_xll.qlRateHelperEarliestDate($E111,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M111" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M111" s="118">
         <f>_xll.qlRateHelperLatestDate($E111,Trigger)</f>
-        <v>#NUM!</v>
+        <v>46349</v>
       </c>
       <c r="O111" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11487,9 +11477,9 @@
         <f>_xll.qlRateHelperQuoteValue($E112,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H112" s="121" t="e">
+      <c r="H112" s="121">
         <f>_xll.qlSwapRateHelperSpread($E112,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I112" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11501,13 +11491,13 @@
       <c r="K112" s="120">
         <v>1</v>
       </c>
-      <c r="L112" s="119" t="e">
+      <c r="L112" s="119">
         <f>_xll.qlRateHelperEarliestDate($E112,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M112" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M112" s="118">
         <f>_xll.qlRateHelperLatestDate($E112,Trigger)</f>
-        <v>#NUM!</v>
+        <v>46713</v>
       </c>
       <c r="O112" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11534,17 +11524,17 @@
         <f>_xll.ohObjectPropertyValues(E113,"Rate")</f>
         <v>HKDQM3H15Y_Quote</v>
       </c>
-      <c r="G113" s="121" t="e">
+      <c r="G113" s="121">
         <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H113" s="121" t="e">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="H113" s="121">
         <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I113" s="120" t="b">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" s="120">
         <v>50</v>
@@ -11552,13 +11542,13 @@
       <c r="K113" s="120">
         <v>1</v>
       </c>
-      <c r="L113" s="119" t="e">
+      <c r="L113" s="119">
         <f>_xll.qlRateHelperEarliestDate($E113,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M113" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M113" s="118">
         <f>_xll.qlRateHelperLatestDate($E113,Trigger)</f>
-        <v>#NUM!</v>
+        <v>47078</v>
       </c>
       <c r="O113" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11589,9 +11579,9 @@
         <f>_xll.qlRateHelperQuoteValue($E114,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H114" s="121" t="e">
+      <c r="H114" s="121">
         <f>_xll.qlSwapRateHelperSpread($E114,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I114" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11603,13 +11593,13 @@
       <c r="K114" s="120">
         <v>1</v>
       </c>
-      <c r="L114" s="119" t="e">
+      <c r="L114" s="119">
         <f>_xll.qlRateHelperEarliestDate($E114,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M114" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M114" s="118">
         <f>_xll.qlRateHelperLatestDate($E114,Trigger)</f>
-        <v>#NUM!</v>
+        <v>47443</v>
       </c>
       <c r="O114" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11640,9 +11630,9 @@
         <f>_xll.qlRateHelperQuoteValue($E115,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H115" s="121" t="e">
+      <c r="H115" s="121">
         <f>_xll.qlSwapRateHelperSpread($E115,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I115" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11654,13 +11644,13 @@
       <c r="K115" s="120">
         <v>1</v>
       </c>
-      <c r="L115" s="119" t="e">
+      <c r="L115" s="119">
         <f>_xll.qlRateHelperEarliestDate($E115,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M115" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M115" s="118">
         <f>_xll.qlRateHelperLatestDate($E115,Trigger)</f>
-        <v>#NUM!</v>
+        <v>47808</v>
       </c>
       <c r="O115" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11691,9 +11681,9 @@
         <f>_xll.qlRateHelperQuoteValue($E116,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H116" s="121" t="e">
+      <c r="H116" s="121">
         <f>_xll.qlSwapRateHelperSpread($E116,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I116" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11705,13 +11695,13 @@
       <c r="K116" s="120">
         <v>1</v>
       </c>
-      <c r="L116" s="119" t="e">
+      <c r="L116" s="119">
         <f>_xll.qlRateHelperEarliestDate($E116,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M116" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M116" s="118">
         <f>_xll.qlRateHelperLatestDate($E116,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48173</v>
       </c>
       <c r="O116" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11742,9 +11732,9 @@
         <f>_xll.qlRateHelperQuoteValue($E117,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H117" s="121" t="e">
+      <c r="H117" s="121">
         <f>_xll.qlSwapRateHelperSpread($E117,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I117" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11756,13 +11746,13 @@
       <c r="K117" s="120">
         <v>1</v>
       </c>
-      <c r="L117" s="119" t="e">
+      <c r="L117" s="119">
         <f>_xll.qlRateHelperEarliestDate($E117,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M117" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M117" s="118">
         <f>_xll.qlRateHelperLatestDate($E117,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48540</v>
       </c>
       <c r="O117" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11793,9 +11783,9 @@
         <f>_xll.qlRateHelperQuoteValue($E118,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H118" s="121" t="e">
+      <c r="H118" s="121">
         <f>_xll.qlSwapRateHelperSpread($E118,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I118" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11807,13 +11797,13 @@
       <c r="K118" s="120">
         <v>1</v>
       </c>
-      <c r="L118" s="119" t="e">
+      <c r="L118" s="119">
         <f>_xll.qlRateHelperEarliestDate($E118,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M118" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M118" s="118">
         <f>_xll.qlRateHelperLatestDate($E118,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48904</v>
       </c>
       <c r="O118" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11844,9 +11834,9 @@
         <f>_xll.qlRateHelperQuoteValue($E119,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H119" s="121" t="e">
+      <c r="H119" s="121">
         <f>_xll.qlSwapRateHelperSpread($E119,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I119" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11858,13 +11848,13 @@
       <c r="K119" s="120">
         <v>1</v>
       </c>
-      <c r="L119" s="119" t="e">
+      <c r="L119" s="119">
         <f>_xll.qlRateHelperEarliestDate($E119,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M119" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M119" s="118">
         <f>_xll.qlRateHelperLatestDate($E119,Trigger)</f>
-        <v>#NUM!</v>
+        <v>49269</v>
       </c>
       <c r="O119" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11895,9 +11885,9 @@
         <f>_xll.qlRateHelperQuoteValue($E120,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H120" s="121" t="e">
+      <c r="H120" s="121">
         <f>_xll.qlSwapRateHelperSpread($E120,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I120" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11909,13 +11899,13 @@
       <c r="K120" s="120">
         <v>1</v>
       </c>
-      <c r="L120" s="119" t="e">
+      <c r="L120" s="119">
         <f>_xll.qlRateHelperEarliestDate($E120,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M120" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M120" s="118">
         <f>_xll.qlRateHelperLatestDate($E120,Trigger)</f>
-        <v>#NUM!</v>
+        <v>49634</v>
       </c>
       <c r="O120" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11946,9 +11936,9 @@
         <f>_xll.qlRateHelperQuoteValue($E121,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H121" s="121" t="e">
+      <c r="H121" s="121">
         <f>_xll.qlSwapRateHelperSpread($E121,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I121" s="120" t="b">
         <f t="shared" si="8"/>
@@ -11960,13 +11950,13 @@
       <c r="K121" s="120">
         <v>1</v>
       </c>
-      <c r="L121" s="119" t="e">
+      <c r="L121" s="119">
         <f>_xll.qlRateHelperEarliestDate($E121,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M121" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M121" s="118">
         <f>_xll.qlRateHelperLatestDate($E121,Trigger)</f>
-        <v>#NUM!</v>
+        <v>50000</v>
       </c>
       <c r="O121" s="123" t="e">
         <f t="shared" si="9"/>
@@ -11997,9 +11987,9 @@
         <f>_xll.qlRateHelperQuoteValue($E122,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H122" s="121" t="e">
+      <c r="H122" s="121">
         <f>_xll.qlSwapRateHelperSpread($E122,Trigger)</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
       <c r="I122" s="120" t="b">
         <f t="shared" si="8"/>
@@ -12011,13 +12001,13 @@
       <c r="K122" s="120">
         <v>1</v>
       </c>
-      <c r="L122" s="119" t="e">
+      <c r="L122" s="119">
         <f>_xll.qlRateHelperEarliestDate($E122,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M122" s="118" t="e">
+        <v>41599</v>
+      </c>
+      <c r="M122" s="118">
         <f>_xll.qlRateHelperLatestDate($E122,Trigger)</f>
-        <v>#NUM!</v>
+        <v>50367</v>
       </c>
       <c r="O122" s="123" t="e">
         <f t="shared" si="9"/>
@@ -14445,7 +14435,7 @@
     <row r="7" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="142" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>HKD_YC3MRH_RateHelpersSelected#0000</v>
+        <v>HKD_YC3MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="141" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -14524,244 +14514,244 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D10" s="139" t="str">
-        <v>HKD_YC3MRH_9x12F</v>
+        <v>HKD_YC3MRH_QM3H1Y</v>
       </c>
       <c r="E10" s="138">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F10" s="138" t="str">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="F10" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
-        <v>--</v>
+        <v>0</v>
       </c>
       <c r="G10" s="137">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41872</v>
+        <v>41599</v>
       </c>
       <c r="H10" s="136">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
         <v>41964</v>
       </c>
       <c r="I10" s="131">
-        <v>0.99558456903541614</v>
+        <v>0.99553983131021029</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E11" s="138" t="e">
+      <c r="D11" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H18M</v>
+      </c>
+      <c r="E11" s="138">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F11" s="138" t="str">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="F11" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
-        <v>--</v>
-      </c>
-      <c r="G11" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G11" s="137">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H11" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H11" s="136">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I11" s="131" t="e">
-        <v>#N/A</v>
+        <v>42145</v>
+      </c>
+      <c r="I11" s="131">
+        <v>0.99277612494794121</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="140"/>
-      <c r="D12" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E12" s="138" t="e">
+      <c r="D12" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H2Y</v>
+      </c>
+      <c r="E12" s="138">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F12" s="138" t="str">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F12" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
-        <v>--</v>
-      </c>
-      <c r="G12" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G12" s="137">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H12" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H12" s="136">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I12" s="131" t="e">
-        <v>#N/A</v>
+        <v>42331</v>
+      </c>
+      <c r="I12" s="131">
+        <v>0.98915746378839775</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="140"/>
-      <c r="D13" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E13" s="138" t="e">
+      <c r="D13" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H3Y</v>
+      </c>
+      <c r="E13" s="138">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F13" s="138" t="str">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F13" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
-        <v>--</v>
-      </c>
-      <c r="G13" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G13" s="137">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H13" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H13" s="136">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I13" s="131" t="e">
-        <v>#N/A</v>
+        <v>42695</v>
+      </c>
+      <c r="I13" s="131">
+        <v>0.97702886678265211</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E14" s="138" t="e">
+      <c r="D14" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H4Y</v>
+      </c>
+      <c r="E14" s="138">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F14" s="138" t="str">
+        <v>1.0899999999999998E-2</v>
+      </c>
+      <c r="F14" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
-        <v>--</v>
-      </c>
-      <c r="G14" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G14" s="137">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H14" s="136">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I14" s="131" t="e">
-        <v>#N/A</v>
+        <v>43060</v>
+      </c>
+      <c r="I14" s="131">
+        <v>0.95699287222516238</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E15" s="138" t="e">
+      <c r="D15" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H5Y</v>
+      </c>
+      <c r="E15" s="138">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F15" s="138" t="str">
+        <v>1.4100000000000001E-2</v>
+      </c>
+      <c r="F15" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
-        <v>--</v>
-      </c>
-      <c r="G15" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G15" s="137">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H15" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H15" s="136">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I15" s="131" t="e">
-        <v>#N/A</v>
+        <v>43425</v>
+      </c>
+      <c r="I15" s="131">
+        <v>0.93111625214964855</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E16" s="138" t="e">
+      <c r="D16" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H7Y</v>
+      </c>
+      <c r="E16" s="138">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F16" s="138" t="str">
+        <v>1.95E-2</v>
+      </c>
+      <c r="F16" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
-        <v>--</v>
-      </c>
-      <c r="G16" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G16" s="137">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H16" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H16" s="136">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I16" s="131" t="e">
-        <v>#N/A</v>
+        <v>44158</v>
+      </c>
+      <c r="I16" s="131">
+        <v>0.8696356977972467</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E17" s="138" t="e">
+      <c r="D17" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H10Y</v>
+      </c>
+      <c r="E17" s="138">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F17" s="138" t="str">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="F17" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
-        <v>--</v>
-      </c>
-      <c r="G17" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G17" s="137">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H17" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H17" s="136">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I17" s="131" t="e">
-        <v>#N/A</v>
+        <v>45251</v>
+      </c>
+      <c r="I17" s="131">
+        <v>0.77618965900787218</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D18" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E18" s="138" t="e">
+      <c r="D18" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H12Y</v>
+      </c>
+      <c r="E18" s="138">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="138" t="str">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="F18" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
-        <v>--</v>
-      </c>
-      <c r="G18" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G18" s="137">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H18" s="136">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="131" t="e">
-        <v>#N/A</v>
+        <v>45982</v>
+      </c>
+      <c r="I18" s="131">
+        <v>0.72261428151700513</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D19" s="139" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E19" s="138" t="e">
+      <c r="D19" s="139" t="str">
+        <v>HKD_YC3MRH_QM3H15Y</v>
+      </c>
+      <c r="E19" s="138">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="138" t="str">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="F19" s="138">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
-        <v>--</v>
-      </c>
-      <c r="G19" s="137" t="e">
+        <v>0</v>
+      </c>
+      <c r="G19" s="137">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="136" t="e">
+        <v>41599</v>
+      </c>
+      <c r="H19" s="136">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="131" t="e">
-        <v>#N/A</v>
+        <v>47078</v>
+      </c>
+      <c r="I19" s="131">
+        <v>0.65497495396013317</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.2">

</xml_diff>